<commit_message>
Close #130 and Close #131
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF8BE8B-C3DA-4FDC-B066-0AD504AFA60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC952475-4D03-4B0A-866F-4F3409A581BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
+    <workbookView xWindow="14115" yWindow="-16455" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
   <sheets>
     <sheet name="assert" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="20">
   <si>
     <t>Components</t>
   </si>
@@ -54,28 +54,13 @@
     <t>object (recursive)</t>
   </si>
   <si>
-    <t>object (union, explicit)</t>
-  </si>
-  <si>
     <t>Failed</t>
-  </si>
-  <si>
-    <t>object (union, implicit)</t>
-  </si>
-  <si>
-    <t>array (simple)</t>
   </si>
   <si>
     <t>array (recursive)</t>
   </si>
   <si>
-    <t>array (recursive, union)</t>
-  </si>
-  <si>
     <t>JSON.stringify()</t>
-  </si>
-  <si>
-    <t>ideal</t>
   </si>
   <si>
     <t>object (simple)</t>
@@ -281,7 +266,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>assert!$B$10</c:f>
+              <c:f>assert!$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -302,9 +287,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>assert!$A$11:$A$17</c:f>
+              <c:f>assert!$A$12:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>object (hierarchical)</c:v>
                 </c:pt>
@@ -312,49 +297,43 @@
                   <c:v>object (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>object (union, explicit)</c:v>
+                  <c:v>object (union)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>object (union, implicit)</c:v>
+                  <c:v>array (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>array (simple)</c:v>
+                  <c:v>array (union)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>array (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>array (recursive, union)</c:v>
+                  <c:v>ultimate union</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>assert!$B$11:$B$17</c:f>
+              <c:f>assert!$B$12:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5351575449685471</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.9649752671990666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9199292880977576</c:v>
+                  <c:v>1.0864403056801457</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6837835632479519</c:v>
+                  <c:v>12.855453268348597</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0687629394363727</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13.150362446101424</c:v>
+                  <c:v>128.10694791126352</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -370,7 +349,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>assert!$C$10</c:f>
+              <c:f>assert!$C$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -391,9 +370,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>assert!$A$11:$A$17</c:f>
+              <c:f>assert!$A$12:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>object (hierarchical)</c:v>
                 </c:pt>
@@ -401,37 +380,34 @@
                   <c:v>object (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>object (union, explicit)</c:v>
+                  <c:v>object (union)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>object (union, implicit)</c:v>
+                  <c:v>array (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>array (simple)</c:v>
+                  <c:v>array (union)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>array (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>array (recursive, union)</c:v>
+                  <c:v>ultimate union</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>assert!$C$11:$C$17</c:f>
+              <c:f>assert!$C$12:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.1795497921832088</c:v>
+                  <c:v>1.1477596108528645</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1.1084353191331768</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -440,9 +416,6 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -762,7 +735,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>is!$B$10</c:f>
+              <c:f>is!$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -783,9 +756,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>is!$A$11:$A$17</c:f>
+              <c:f>is!$A$12:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>object (hierarchical)</c:v>
                 </c:pt>
@@ -793,49 +766,43 @@
                   <c:v>object (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>object (union, explicit)</c:v>
+                  <c:v>object (union)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>object (union, implicit)</c:v>
+                  <c:v>array (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>array (simple)</c:v>
+                  <c:v>array (union)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>array (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>array (recursive, union)</c:v>
+                  <c:v>ultimate union</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>is!$B$11:$B$17</c:f>
+              <c:f>is!$B$12:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.8358285119706612</c:v>
+                  <c:v>2.2378141839775476</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5060927489460998</c:v>
+                  <c:v>1.6809024039883016</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2.1316749297988471</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.6529969149072363</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0524480306787893</c:v>
+                  <c:v>6.8327248471150908</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4471457758316126</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.4775714679212406</c:v>
+                  <c:v>36.482172779742911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -851,7 +818,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>is!$C$10</c:f>
+              <c:f>is!$C$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -872,9 +839,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>is!$A$11:$A$17</c:f>
+              <c:f>is!$A$12:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>object (hierarchical)</c:v>
                 </c:pt>
@@ -882,29 +849,26 @@
                   <c:v>object (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>object (union, explicit)</c:v>
+                  <c:v>object (union)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>object (union, implicit)</c:v>
+                  <c:v>array (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>array (simple)</c:v>
+                  <c:v>array (union)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>array (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>array (recursive, union)</c:v>
+                  <c:v>ultimate union</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>is!$C$11:$C$17</c:f>
+              <c:f>is!$C$12:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -912,18 +876,15 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1231,7 +1192,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>stringify!$B$11</c:f>
+              <c:f>stringify!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1252,7 +1213,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>stringify!$A$12:$A$19</c:f>
+              <c:f>stringify!$A$13:$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1284,33 +1245,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stringify!$B$12:$B$19</c:f>
+              <c:f>stringify!$B$13:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>26.688965785126815</c:v>
+                  <c:v>35.981344111709362</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1735739012359447</c:v>
+                  <c:v>4.3425769515787387</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0557200074209065</c:v>
+                  <c:v>6.1360491904729768</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.3788424695545478</c:v>
+                  <c:v>4.4639366853624463</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.6887980760818579</c:v>
+                  <c:v>3.5406524564091533</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.4026799497747047</c:v>
+                  <c:v>3.5412290949363032</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.2959219069189705</c:v>
+                  <c:v>2.2878129842191046</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.8330365319782569</c:v>
+                  <c:v>8.6813645463175586</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1326,7 +1287,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>stringify!$C$11</c:f>
+              <c:f>stringify!$C$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1347,7 +1308,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>stringify!$A$12:$A$19</c:f>
+              <c:f>stringify!$A$13:$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1379,30 +1340,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stringify!$C$12:$C$19</c:f>
+              <c:f>stringify!$C$13:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>7.8275627546227806</c:v>
+                  <c:v>8.0408170213041181</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0290020494267083</c:v>
+                  <c:v>4.1150912657759262</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0001910916545054</c:v>
+                  <c:v>0.982031430994601</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9126756478890905</c:v>
+                  <c:v>3.3182717654892566</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1628979549972689</c:v>
+                  <c:v>4.7982692196000176</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.98839528816958033</c:v>
+                  <c:v>1.0112483865019366</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.92379565755227477</c:v>
+                  <c:v>0.93026050840057539</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1421,7 +1382,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>stringify!$D$11</c:f>
+              <c:f>stringify!$D$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1442,7 +1403,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>stringify!$A$12:$A$19</c:f>
+              <c:f>stringify!$A$13:$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1474,7 +1435,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stringify!$D$12:$D$19</c:f>
+              <c:f>stringify!$D$13:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1843,19 +1804,19 @@
                   <c:v>object (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>object (union, implicit)</c:v>
+                  <c:v>object (union)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>object (union, explicit)</c:v>
+                  <c:v>array (hierarchical)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>array (hierarchical)</c:v>
+                  <c:v>array (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>array (recursive)</c:v>
+                  <c:v>array (union)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>array (recursive, union)</c:v>
+                  <c:v>ultimate union</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1867,28 +1828,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>149403.824730783</c:v>
+                  <c:v>142008.388037928</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5447.7836213373403</c:v>
+                  <c:v>5000.5586592178697</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5568.2363804247398</c:v>
+                  <c:v>5470.67612999626</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2220.7815595173702</c:v>
+                  <c:v>2229.7124015387399</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2066.36931311329</c:v>
+                  <c:v>100.912506709608</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>71.772997032640902</c:v>
+                  <c:v>260.65393093313702</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>253.03827317250099</c:v>
+                  <c:v>401.92342587552099</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>339.12248628884799</c:v>
+                  <c:v>1263.3490737377399</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1938,19 +1899,19 @@
                   <c:v>object (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>object (union, implicit)</c:v>
+                  <c:v>object (union)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>object (union, explicit)</c:v>
+                  <c:v>array (hierarchical)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>array (hierarchical)</c:v>
+                  <c:v>array (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>array (recursive)</c:v>
+                  <c:v>array (union)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>array (recursive, union)</c:v>
+                  <c:v>ultimate union</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1962,25 +1923,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5.7027225901397998</c:v>
+                  <c:v>5.4635178004934701</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.44378271070203</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.534900808229203</c:v>
+                  <c:v>52.650756057569602</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.0944910616563199</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.7614138438880702</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>32.910461481890003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31.0833180062534</c:v>
+                  <c:v>2.5849335302806402</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2033,19 +1994,19 @@
                   <c:v>object (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>object (union, implicit)</c:v>
+                  <c:v>object (union)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>object (union, explicit)</c:v>
+                  <c:v>array (hierarchical)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>array (hierarchical)</c:v>
+                  <c:v>array (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>array (recursive)</c:v>
+                  <c:v>array (union)</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>array (recursive, union)</c:v>
+                  <c:v>ultimate union</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2057,28 +2018,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4535.6355620866998</c:v>
+                  <c:v>4262.1504972790399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1256.6554180727401</c:v>
+                  <c:v>1191.4353111957901</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>956.09756097560899</c:v>
+                  <c:v>980.59339428997896</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>546.46633277684998</c:v>
+                  <c:v>520.87250846182701</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>506.87252871398903</c:v>
+                  <c:v>30.766396462785501</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.6514306949089</c:v>
+                  <c:v>78.568723968193794</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>73.283004971460102</c:v>
+                  <c:v>181.146025878003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>146.599777034559</c:v>
+                  <c:v>145.03957297993699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2417,7 +2378,7 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>109697.837837837</c:v>
+                  <c:v>152719.485693589</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>39485.635359116</c:v>
@@ -2488,7 +2449,7 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>34672.289156626503</c:v>
+                  <c:v>34128.503822351602</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30323.545604698102</c:v>
@@ -2559,7 +2520,7 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4352.6499174766104</c:v>
+                  <c:v>4244.4074690330899</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10555.514157973101</c:v>
@@ -2646,6 +2607,8 @@
         <c:axId val="798084816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="160000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2697,6 +2660,8 @@
         <c:crossAx val="798081072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="30000"/>
+        <c:minorUnit val="1000"/>
       </c:valAx>
       <c:dTable>
         <c:showHorzBorder val="1"/>
@@ -5545,13 +5510,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>245744</xdr:colOff>
+      <xdr:colOff>249554</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>245744</xdr:colOff>
+      <xdr:colOff>249554</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>1905</xdr:rowOff>
     </xdr:to>
@@ -6001,20 +5966,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4DC42C-376D-41DF-9AD8-63D3F4858048}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6025,184 +5990,168 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>19734.890354786901</v>
+        <v>19578.474514117999</v>
       </c>
       <c r="C2">
-        <v>23278.285816747299</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22471.382289416801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>31335.4966648638</v>
+        <v>20536.4943065148</v>
       </c>
       <c r="C3">
-        <v>20411.909362374801</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22763.3756205184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B4">
-        <v>4644.3401335981198</v>
-      </c>
-      <c r="C4" t="s">
+        <v>4617.0450316337901</v>
+      </c>
+      <c r="C4">
+        <v>2349.6708119970699</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
       <c r="B5">
-        <v>4361.7372182517802</v>
+        <v>1703.66320393657</v>
       </c>
       <c r="C5">
-        <v>2271.8218036943099</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1568.1148748159001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B6">
-        <v>14120.0073286918</v>
+        <v>3019.8165137614601</v>
       </c>
       <c r="C6">
-        <v>8385.8802502234103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>234.905487245366</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B7">
-        <v>1592.5858290723099</v>
+        <v>4471.8106252258704</v>
       </c>
       <c r="C7">
-        <v>1490.12074643249</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>2858.5657370517902</v>
-      </c>
-      <c r="C8">
-        <v>217.37543347326101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+        <v>34.906854765780402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="1">
-        <f xml:space="preserve"> B2/MIN($B2:$C2)</f>
+      <c r="B12" s="1">
+        <f t="shared" ref="B12:C19" si="0" xml:space="preserve"> B2/MIN($B2:$C2)</f>
         <v>1</v>
-      </c>
-      <c r="C11" s="1">
-        <f xml:space="preserve"> C2/MIN($B2:$C2)</f>
-        <v>1.1795497921832088</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1">
-        <f t="shared" ref="B12:C12" si="0" xml:space="preserve"> B3/MIN($B3:$C3)</f>
-        <v>1.5351575449685471</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
+        <v>1.1477596108528645</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1">
-        <f t="shared" ref="B13:C13" si="1" xml:space="preserve"> B4/MIN($B4:$C4)</f>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1084353191331768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9649752671990666</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C13" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1">
-        <f t="shared" ref="B14:C14" si="2" xml:space="preserve"> B5/MIN($B5:$C5)</f>
-        <v>1.9199292880977576</v>
-      </c>
-      <c r="C14" s="1">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0864403056801457</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="1">
-        <f t="shared" ref="B15:C15" si="3" xml:space="preserve"> B6/MIN($B6:$C6)</f>
-        <v>1.6837835632479519</v>
-      </c>
-      <c r="C15" s="1">
-        <f t="shared" si="3"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>12.855453268348597</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="1">
-        <f t="shared" ref="B16:C16" si="4" xml:space="preserve"> B7/MIN($B7:$C7)</f>
-        <v>1.0687629394363727</v>
-      </c>
-      <c r="C16" s="1">
-        <f t="shared" si="4"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>128.10694791126352</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="1">
-        <f t="shared" ref="B17:C17" si="5" xml:space="preserve"> B8/MIN($B8:$C8)</f>
-        <v>13.150362446101424</v>
-      </c>
-      <c r="C17" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6213,20 +6162,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AA11DE-36E1-4DB2-967D-EB7E691732BC}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6237,184 +6186,168 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>84173.473210940399</v>
+        <v>116060.60047890899</v>
       </c>
       <c r="C2">
-        <v>45850.400874635503</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51863.376910329498</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>72643.873590833493</v>
+        <v>83197.710339814599</v>
       </c>
       <c r="C3">
-        <v>48233.333333333299</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49495.860165593302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B4">
-        <v>13749.4979003103</v>
-      </c>
-      <c r="C4" t="s">
+        <v>16247.1379247683</v>
+      </c>
+      <c r="C4">
+        <v>7621.7708890076601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
       <c r="B5">
-        <v>17299.871771386701</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7592.77198211624</v>
+      </c>
+      <c r="C5">
+        <v>4593.3370556486097</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B6">
-        <v>62687.952478188199</v>
+        <v>7868.2882882882795</v>
       </c>
       <c r="C6">
-        <v>30543.015726179401</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1151.5593653109599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B7">
-        <v>6422.2507802460004</v>
+        <v>11100.3271537622</v>
       </c>
       <c r="C7">
-        <v>4437.8741157264603</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>7146.1254612546099</v>
-      </c>
-      <c r="C8">
-        <v>1103.2105931434701</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+        <v>304.26716141001799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="1">
-        <f xml:space="preserve"> B2 / MIN($B2:$C2)</f>
-        <v>1.8358285119706612</v>
-      </c>
-      <c r="C11" s="1">
-        <f xml:space="preserve"> C2 / MIN($B2:$C2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
       <c r="B12" s="1">
-        <f t="shared" ref="B12:C12" si="0" xml:space="preserve"> B3 / MIN($B3:$C3)</f>
-        <v>1.5060927489460998</v>
+        <f t="shared" ref="B12:C19" si="0" xml:space="preserve"> B2 / MIN($B2:$C2)</f>
+        <v>2.2378141839775476</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" ref="B13:C13" si="1" xml:space="preserve"> B4 / MIN($B4:$C4)</f>
+        <f t="shared" si="0"/>
+        <v>1.6809024039883016</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C13" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" ref="B14:C14" si="2" xml:space="preserve"> B5 / MIN($B5:$C5)</f>
+        <f t="shared" si="0"/>
+        <v>2.1316749297988471</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" ref="B15:C15" si="3" xml:space="preserve"> B6 / MIN($B6:$C6)</f>
-        <v>2.0524480306787893</v>
+        <f t="shared" si="0"/>
+        <v>1.6529969149072363</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" ref="B16:C16" si="4" xml:space="preserve"> B7 / MIN($B7:$C7)</f>
-        <v>1.4471457758316126</v>
+        <f t="shared" si="0"/>
+        <v>6.8327248471150908</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" ref="B17:C17" si="5" xml:space="preserve"> B8 / MIN($B8:$C8)</f>
-        <v>6.4775714679212406</v>
+        <f t="shared" si="0"/>
+        <v>36.482172779742911</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6426,20 +6359,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EFA07C-E270-4B85-8B26-6FA6BD53AA2B}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6447,286 +6380,293 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>109697.837837837</v>
+        <v>152719.485693589</v>
       </c>
       <c r="C2">
-        <v>32173.0979250091</v>
+        <v>34128.503822351602</v>
       </c>
       <c r="D2">
-        <v>4110.23187338976</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4244.4074690330899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>4877.5031571351201</v>
+        <v>5353.9839181286497</v>
       </c>
       <c r="C3">
-        <v>4708.5473220836302</v>
+        <v>5073.5157267820496</v>
       </c>
       <c r="D3">
-        <v>1168.66342193934</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1232.90478852245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>5512.3297754876703</v>
+        <v>5997.6076555023901</v>
       </c>
       <c r="C4">
-        <v>910.44221479004</v>
+        <v>959.874838947174</v>
       </c>
       <c r="D4">
-        <v>910.26827012025899</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>977.43800111877601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B5">
-        <v>2007.5132856881</v>
+        <v>2267.0339761248802</v>
       </c>
       <c r="C5">
-        <v>1335.3380718060801</v>
+        <v>1685.2019561673601</v>
       </c>
       <c r="D5">
-        <v>458.45752608047599</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>507.85531603945901</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>251.63161711385001</v>
+        <v>124.886052871467</v>
       </c>
       <c r="C6">
-        <v>352.187442796997</v>
+        <v>169.24476797088201</v>
       </c>
       <c r="D6">
-        <v>68.215069495245004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35.2720450281425</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>246.90216386166</v>
+        <v>270.56436739210602</v>
       </c>
       <c r="C7">
-        <v>71.719038817005497</v>
+        <v>77.263507283791199</v>
       </c>
       <c r="D7">
-        <v>72.561089349002003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>76.404084609773804</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B8">
-        <v>401.989683124539</v>
+        <v>411.00681023375603</v>
       </c>
       <c r="C8">
-        <v>161.74606049628599</v>
+        <v>167.12179137083501</v>
       </c>
       <c r="D8">
-        <v>175.08856983031799</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>179.65052784856201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>1212.9291453615699</v>
+        <v>1289.5822126591299</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>137.31734732109399</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <v>148.54602704204399</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1">
         <f xml:space="preserve"> B2 / $D2</f>
-        <v>26.688965785126815</v>
-      </c>
-      <c r="C12" s="1">
-        <f xml:space="preserve"> C2 / $D2</f>
-        <v>7.8275627546227806</v>
-      </c>
-      <c r="D12" s="1">
-        <f xml:space="preserve"> D2 / $D2</f>
+        <v>35.981344111709362</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" ref="C13:D13" si="0" xml:space="preserve"> C2 / $D2</f>
+        <v>8.0408170213041181</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="1">
-        <f xml:space="preserve"> B3 / $D3</f>
-        <v>4.1735739012359447</v>
-      </c>
-      <c r="C13" s="1">
-        <f xml:space="preserve"> C3 / $D3</f>
-        <v>4.0290020494267083</v>
-      </c>
-      <c r="D13" s="1">
-        <f xml:space="preserve"> D3 / $D3</f>
+      <c r="B14" s="1">
+        <f t="shared" ref="B14:D14" si="1" xml:space="preserve"> B3 / $D3</f>
+        <v>4.3425769515787387</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="1"/>
+        <v>4.1150912657759262</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="1">
-        <f xml:space="preserve"> B4 / $D4</f>
-        <v>6.0557200074209065</v>
-      </c>
-      <c r="C14" s="1">
-        <f xml:space="preserve"> C4 / $D4</f>
-        <v>1.0001910916545054</v>
-      </c>
-      <c r="D14" s="1">
-        <f xml:space="preserve"> D4 / $D4</f>
+      <c r="B15" s="1">
+        <f t="shared" ref="B15:D15" si="2" xml:space="preserve"> B4 / $D4</f>
+        <v>6.1360491904729768</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="2"/>
+        <v>0.982031430994601</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="1">
-        <f xml:space="preserve"> B5 / $D5</f>
-        <v>4.3788424695545478</v>
-      </c>
-      <c r="C15" s="1">
-        <f xml:space="preserve"> C5 / $D5</f>
-        <v>2.9126756478890905</v>
-      </c>
-      <c r="D15" s="1">
-        <f xml:space="preserve"> D5 / $D5</f>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" ref="B16:D16" si="3" xml:space="preserve"> B5 / $D5</f>
+        <v>4.4639366853624463</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="3"/>
+        <v>3.3182717654892566</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1">
-        <f xml:space="preserve"> B6 / $D6</f>
-        <v>3.6887980760818579</v>
-      </c>
-      <c r="C16" s="1">
-        <f xml:space="preserve"> C6 / $D6</f>
-        <v>5.1628979549972689</v>
-      </c>
-      <c r="D16" s="1">
-        <f xml:space="preserve"> D6 / $D6</f>
-        <v>1</v>
-      </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="1">
-        <f xml:space="preserve"> B7 / $D7</f>
-        <v>3.4026799497747047</v>
+        <f t="shared" ref="B17:D17" si="4" xml:space="preserve"> B6 / $D6</f>
+        <v>3.5406524564091533</v>
       </c>
       <c r="C17" s="1">
-        <f xml:space="preserve"> C7 / $D7</f>
-        <v>0.98839528816958033</v>
+        <f t="shared" si="4"/>
+        <v>4.7982692196000176</v>
       </c>
       <c r="D17" s="1">
-        <f xml:space="preserve"> D7 / $D7</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1">
-        <f xml:space="preserve"> B8 / $D8</f>
-        <v>2.2959219069189705</v>
+        <f t="shared" ref="B18:D18" si="5" xml:space="preserve"> B7 / $D7</f>
+        <v>3.5412290949363032</v>
       </c>
       <c r="C18" s="1">
-        <f xml:space="preserve"> C8 / $D8</f>
-        <v>0.92379565755227477</v>
+        <f t="shared" si="5"/>
+        <v>1.0112483865019366</v>
       </c>
       <c r="D18" s="1">
-        <f xml:space="preserve"> D8 / $D8</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
-        <f xml:space="preserve"> B9 / $D9</f>
-        <v>8.8330365319782569</v>
-      </c>
-      <c r="C19" s="1" t="e">
-        <f xml:space="preserve"> C9 / $D9</f>
+        <f t="shared" ref="B19:D19" si="6" xml:space="preserve"> B8 / $D8</f>
+        <v>2.2878129842191046</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="6"/>
+        <v>0.93026050840057539</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" ref="B20:D21" si="7" xml:space="preserve"> B9 / $D9</f>
+        <v>8.6813645463175586</v>
+      </c>
+      <c r="C20" s="1" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D19" s="1">
-        <f xml:space="preserve"> D9 / $D9</f>
+      <c r="D20" s="1">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -6742,20 +6682,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B9C7172-2F08-433B-92F6-25D08187801E}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6763,152 +6703,125 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>149403.824730783</v>
+        <v>142008.388037928</v>
       </c>
       <c r="C2">
-        <v>5.7027225901397998</v>
+        <v>5.4635178004934701</v>
       </c>
       <c r="D2">
-        <v>4535.6355620866998</v>
-      </c>
-      <c r="E2">
-        <v>225758.29725829701</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4262.1504972790399</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>5447.7836213373403</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+        <v>5000.5586592178697</v>
+      </c>
+      <c r="C3">
+        <v>1.44378271070203</v>
       </c>
       <c r="D3">
-        <v>1256.6554180727401</v>
-      </c>
-      <c r="E3">
-        <v>6139.3939393939299</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1191.4353111957901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>5568.2363804247398</v>
+        <v>5470.67612999626</v>
       </c>
       <c r="C4">
-        <v>52.534900808229203</v>
+        <v>52.650756057569602</v>
       </c>
       <c r="D4">
-        <v>956.09756097560899</v>
-      </c>
-      <c r="E4">
-        <v>5818.3945284377196</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>980.59339428997896</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B5">
-        <v>2220.7815595173702</v>
-      </c>
-      <c r="C5" t="s">
+        <v>2229.7124015387399</v>
+      </c>
+      <c r="C5">
+        <v>1.0944910616563199</v>
+      </c>
+      <c r="D5">
+        <v>520.87250846182701</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>100.912506709608</v>
+      </c>
+      <c r="C6">
+        <v>2.7614138438880702</v>
+      </c>
+      <c r="D6">
+        <v>30.766396462785501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="D5">
-        <v>546.46633277684998</v>
-      </c>
-      <c r="E5">
-        <v>2260.4185960363002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7">
+        <v>260.65393093313702</v>
+      </c>
+      <c r="C7">
+        <v>32.910461481890003</v>
+      </c>
+      <c r="D7">
+        <v>78.568723968193794</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>401.92342587552099</v>
+      </c>
+      <c r="C8">
+        <v>2.5849335302806402</v>
+      </c>
+      <c r="D8">
+        <v>181.146025878003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>1263.3490737377399</v>
+      </c>
+      <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>2066.36931311329</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>506.87252871398903</v>
-      </c>
-      <c r="E6">
-        <v>1962.5570776255699</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <v>71.772997032640902</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>17.6514306949089</v>
-      </c>
-      <c r="E7">
-        <v>66.071096221849899</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>253.03827317250099</v>
-      </c>
-      <c r="C8">
-        <v>31.0833180062534</v>
-      </c>
-      <c r="D8">
-        <v>73.283004971460102</v>
-      </c>
-      <c r="E8">
-        <v>246.19335901669399</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>339.12248628884799</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
       <c r="D9">
-        <v>146.599777034559</v>
-      </c>
-      <c r="E9">
-        <v>414.25430560644901</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145.03957297993699</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -6916,19 +6829,19 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1">
         <f xml:space="preserve"> B2 / MIN($B2:$E2)</f>
-        <v>26198.683588275409</v>
+        <v>25992.115926684026</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" ref="C12:D12" si="0" xml:space="preserve"> C2 / MIN($B2:$E2)</f>
@@ -6936,35 +6849,35 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>795.34564243559157</v>
+        <v>780.11102972778428</v>
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" ref="B13:D19" si="1" xml:space="preserve"> B3 / MIN($B3:$E3)</f>
-        <v>4.3351451344492604</v>
-      </c>
-      <c r="C13" s="1" t="e">
+        <v>3463.5119413407992</v>
+      </c>
+      <c r="C13" s="1">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>825.21788241698937</v>
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="1"/>
-        <v>105.99118480780527</v>
+        <v>103.90498711954851</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="1"/>
@@ -6972,71 +6885,71 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" si="1"/>
-        <v>18.199283643186082</v>
+        <v>18.624488378054334</v>
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="1"/>
-        <v>4.0638945646158007</v>
-      </c>
-      <c r="C15" s="1" t="e">
+        <v>2037.213897539247</v>
+      </c>
+      <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>475.90384856462691</v>
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="1"/>
-        <v>4.0767040943330981</v>
-      </c>
-      <c r="C16" s="1" t="e">
+        <v>36.543782429772712</v>
+      </c>
+      <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>11.141537705723392</v>
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" si="1"/>
-        <v>4.0661291582071009</v>
-      </c>
-      <c r="C17" s="1" t="e">
+        <v>7.920093465616393</v>
+      </c>
+      <c r="C17" s="1">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.3873479869441714</v>
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="1"/>
-        <v>8.140645510289291</v>
+        <v>155.48694818155928</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="1"/>
@@ -7044,17 +6957,17 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" si="1"/>
-        <v>2.3576313492889303</v>
+        <v>70.077634011090566</v>
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" si="1"/>
-        <v>2.3132537657878176</v>
+        <v>8.7103750223568035</v>
       </c>
       <c r="C19" s="1" t="e">
         <f t="shared" si="1"/>
@@ -7076,48 +6989,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492AED1C-BF35-4801-93A4-FC7E4F2107AC}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2">
+        <v>152719.485693589</v>
+      </c>
+      <c r="C2" s="2">
+        <v>34128.503822351602</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4244.4074690330899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="2">
-        <v>109697.837837837</v>
-      </c>
-      <c r="C2" s="2">
-        <v>34672.289156626503</v>
-      </c>
-      <c r="D2" s="2">
-        <v>4352.6499174766104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
       </c>
       <c r="B3" s="2">
         <v>39485.635359116</v>
@@ -7129,9 +7042,9 @@
         <v>10555.514157973101</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2">
         <v>41142.381656804697</v>
@@ -7143,9 +7056,9 @@
         <v>14923.821940771</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2">
         <v>32103.674063295701</v>

</xml_diff>

<commit_message>
Close #135 and Fix #136
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE94BB40-BF19-470D-B08E-DEE6FA6ACCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8406932-3148-4D33-8305-5B0385DC3E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
+    <workbookView xWindow="14115" yWindow="-16455" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
   <sheets>
     <sheet name="assert" sheetId="1" r:id="rId1"/>
@@ -802,22 +802,22 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.1126582981806736</c:v>
+                  <c:v>2.0309147393559384</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.51580441874608</c:v>
+                  <c:v>1.8470740156776284</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.238712542860871</c:v>
+                  <c:v>12.492353844967141</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2646990371927758</c:v>
+                  <c:v>1.6278462686374255</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1331846395955001</c:v>
+                  <c:v>7.0902782185175601</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.979099468261982</c:v>
+                  <c:v>39.487882056163933</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -968,7 +968,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.4743434089763281</c:v>
+                  <c:v>1.6119307886419818</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -6070,14 +6070,14 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>22471.382289416801</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>22763.3756205184</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -6121,7 +6121,7 @@
         <v>2349.6708119970699</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -6132,7 +6132,7 @@
         <v>1568.1148748159001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -6143,7 +6143,7 @@
         <v>234.905487245366</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>34.906854765780402</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -6165,7 +6165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>1.1477596108528645</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -6191,7 +6191,7 @@
         <v>1.1084353191331768</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -6204,7 +6204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -6230,7 +6230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -6243,11 +6243,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
@@ -6263,17 +6263,17 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6287,54 +6287,54 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>99955.169920462693</v>
+        <v>108212.346125995</v>
       </c>
       <c r="C2" s="2">
-        <v>47312.511448983299</v>
+        <v>53282.564762079703</v>
       </c>
       <c r="D2" s="2">
-        <v>69754.889416925595</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85887.8066378066</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>67936.189775652805</v>
+        <v>87932.663690476096</v>
       </c>
       <c r="C3" s="2">
-        <v>44818.572195383698</v>
+        <v>47606.464572680699</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="2">
-        <v>13053.723601333801</v>
+        <v>15761.783901377799</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2">
-        <v>1161.4963503649601</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1261.71449328005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="2">
-        <v>14902.390438246999</v>
+        <v>15195.213430969799</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -6343,63 +6343,63 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>5735.9486986043003</v>
+        <v>7277.8394376618498</v>
       </c>
       <c r="C6" s="2">
-        <v>4535.4258443465396</v>
+        <v>4470.8395245170796</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="2">
-        <v>5173.0054838139004</v>
+        <v>7925.2662504590498</v>
       </c>
       <c r="C7" s="2">
-        <v>1007.75753202237</v>
+        <v>1117.7651999269599</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="2">
-        <v>5628.1022578839302</v>
+        <v>7013.8045278851396</v>
       </c>
       <c r="C8" s="2">
-        <v>1134.08635452723</v>
+        <v>1205.12344533135</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2">
-        <v>7411.7867165575299</v>
+        <v>11709.4732923878</v>
       </c>
       <c r="C9" s="2">
-        <v>274.72328071130403</v>
+        <v>296.53333333333302</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -6413,30 +6413,30 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="1">
         <f xml:space="preserve"> B2 / MIN($B2:$D2)</f>
-        <v>2.1126582981806736</v>
+        <v>2.0309147393559384</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" ref="C12:D13" si="0" xml:space="preserve"> C2 / MIN($B2:$D2)</f>
+        <f t="shared" ref="C12:D12" si="0" xml:space="preserve"> C2 / MIN($B2:$D2)</f>
         <v>1</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>1.4743434089763281</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.6119307886419818</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1">
         <f xml:space="preserve"> B3 / MIN($B3:$D3)</f>
-        <v>1.51580441874608</v>
+        <v>1.8470740156776284</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" ref="C13:D13" si="1" xml:space="preserve"> C3 / MIN($B3:$D3)</f>
@@ -6447,13 +6447,13 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="1">
         <f xml:space="preserve"> B4 / MIN($B4:$D4)</f>
-        <v>11.238712542860871</v>
+        <v>12.492353844967141</v>
       </c>
       <c r="C14" s="1" t="e">
         <f t="shared" ref="C14:D14" si="2" xml:space="preserve"> C4 / MIN($B4:$D4)</f>
@@ -6464,13 +6464,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="1">
         <f xml:space="preserve"> B6 / MIN($B6:$D6)</f>
-        <v>1.2646990371927758</v>
+        <v>1.6278462686374255</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" ref="C15:D15" si="3" xml:space="preserve"> C6 / MIN($B6:$D6)</f>
@@ -6481,13 +6481,13 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="1">
         <f xml:space="preserve"> B7 / MIN($B7:$D7)</f>
-        <v>5.1331846395955001</v>
+        <v>7.0902782185175601</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" ref="C16:D16" si="4" xml:space="preserve"> C7 / MIN($B7:$D7)</f>
@@ -6498,13 +6498,13 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="1">
         <f xml:space="preserve"> B9 / MIN($B9:$D9)</f>
-        <v>26.979099468261982</v>
+        <v>39.487882056163933</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" ref="C17:D17" si="5" xml:space="preserve"> C9 / MIN($B9:$D9)</f>
@@ -6515,11 +6515,11 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
@@ -6538,16 +6538,16 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6564,7 +6564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -6578,7 +6578,7 @@
         <v>4244.4074690330899</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -6592,7 +6592,7 @@
         <v>1232.90478852245</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -6606,7 +6606,7 @@
         <v>977.43800111877601</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -6620,7 +6620,7 @@
         <v>507.85531603945901</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>35.2720450281425</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -6648,7 +6648,7 @@
         <v>76.404084609773804</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>179.65052784856201</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -6676,10 +6676,10 @@
         <v>148.54602704204399</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -6694,7 +6694,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -6712,7 +6712,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -6730,7 +6730,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -6748,7 +6748,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -6766,7 +6766,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -6784,7 +6784,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -6802,7 +6802,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -6819,7 +6819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -6836,12 +6836,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -6861,16 +6861,16 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6884,7 +6884,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -6898,7 +6898,7 @@
         <v>4262.1504972790399</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -6912,7 +6912,7 @@
         <v>1191.4353111957901</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>980.59339428997896</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -6940,7 +6940,7 @@
         <v>520.87250846182701</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>30.766396462785501</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -6968,7 +6968,7 @@
         <v>78.568723968193794</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>181.146025878003</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -6996,7 +6996,7 @@
         <v>145.03957297993699</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -7010,7 +7010,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -7028,7 +7028,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -7046,7 +7046,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -7064,7 +7064,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -7082,7 +7082,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -7100,7 +7100,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -7118,7 +7118,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -7136,7 +7136,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -7168,14 +7168,14 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -7189,7 +7189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -7203,7 +7203,7 @@
         <v>4244.4074690330899</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -7217,7 +7217,7 @@
         <v>10555.514157973101</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>14923.821940771</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Close #228 - benchmark of `io-ts` and `zod`
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8AF042-B2C5-4054-8B24-E8E5683C0962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3273E2B-EA45-4164-831E-9B279431CA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8355" yWindow="-14685" windowWidth="21600" windowHeight="11235" activeTab="2" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
   <sheets>
-    <sheet name="assert" sheetId="1" r:id="rId1"/>
+    <sheet name="validate" sheetId="1" r:id="rId1"/>
     <sheet name="is" sheetId="2" r:id="rId2"/>
     <sheet name="stringify" sheetId="3" r:id="rId3"/>
     <sheet name="optimizer" sheetId="4" r:id="rId4"/>
@@ -37,15 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="26">
   <si>
     <t>Components</t>
   </si>
   <si>
     <t>typescript-json</t>
-  </si>
-  <si>
-    <t>typescript-is</t>
   </si>
   <si>
     <t>object (hierarchical)</t>
@@ -113,14 +110,21 @@
   <si>
     <t>Intel E5-2686 v4</t>
   </si>
+  <si>
+    <t>io-ts</t>
+  </si>
+  <si>
+    <t>zod</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="##,##0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -160,10 +164,11 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="백분율" xfId="1" builtinId="5"/>
@@ -222,7 +227,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
-              <a:t> type checker, </a:t>
+              <a:t> type checkers, </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="ko-KR" b="1" baseline="0">
@@ -230,7 +235,7 @@
                   <a:srgbClr val="7030A0"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>assertType()</a:t>
+              <a:t>validate()</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
@@ -281,7 +286,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>assert!$B$11</c:f>
+              <c:f>validate!$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -302,9 +307,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>assert!$A$12:$A$17</c:f>
+              <c:f>validate!$A$12:$A$19</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>object (hierarchical)</c:v>
                 </c:pt>
@@ -312,15 +317,21 @@
                   <c:v>object (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>object (union)</c:v>
+                  <c:v>object (union, explicit)</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>array (recursive)</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>array (union)</c:v>
-                </c:pt>
                 <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>ultimate union</c:v>
                 </c:pt>
               </c:strCache>
@@ -328,27 +339,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>assert!$B$12:$B$17</c:f>
+              <c:f>validate!$B$12:$B$19</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>34.547541526010903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>145.38984071038044</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.871178052716488</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.901547467780084</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83.800507007078579</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>482.88873626373538</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>407.10497153700175</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.9649752671990666</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0864403056801457</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12.855453268348597</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>128.10694791126352</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -364,11 +381,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>assert!$C$11</c:f>
+              <c:f>validate!$C$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>typescript-is</c:v>
+                  <c:v>io-ts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -385,9 +402,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>assert!$A$12:$A$17</c:f>
+              <c:f>validate!$A$12:$A$19</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>object (hierarchical)</c:v>
                 </c:pt>
@@ -395,15 +412,21 @@
                   <c:v>object (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>object (union)</c:v>
+                  <c:v>object (union, explicit)</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>array (recursive)</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>array (union)</c:v>
-                </c:pt>
                 <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>ultimate union</c:v>
                 </c:pt>
               </c:strCache>
@@ -411,27 +434,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>assert!$C$12:$C$17</c:f>
+              <c:f>validate!$C$12:$C$19</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.1477596108528645</c:v>
+                  <c:v>9.1791919173757286</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1084353191331768</c:v>
+                  <c:v>21.924209770114938</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>35.711539270040795</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>15.584902823150292</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>16.074244267243323</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>26.983885407341084</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.786208907354819</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -439,6 +468,101 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2080-459A-8C6D-0B6154CC0680}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>validate!$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>zod</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>validate!$A$12:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ultimate union</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>validate!$D$12:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3912-4FEA-81A6-1045CDC68000}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -526,7 +650,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="##,##0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -691,7 +815,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
-              <a:t> type checker, </a:t>
+              <a:t> type checkers, </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="ko-KR" b="1" baseline="0">
@@ -771,9 +895,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>is!$A$12:$A$17</c:f>
+              <c:f>is!$A$12:$A$19</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>object (hierarchical)</c:v>
                 </c:pt>
@@ -781,15 +905,21 @@
                   <c:v>object (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>object (union)</c:v>
+                  <c:v>object (union, explicit)</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>array (recursive)</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>array (union)</c:v>
-                </c:pt>
                 <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>ultimate union</c:v>
                 </c:pt>
               </c:strCache>
@@ -797,27 +927,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>is!$B$12:$B$17</c:f>
+              <c:f>is!$B$12:$B$19</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.0309147393559384</c:v>
+                  <c:v>285.78955071910411</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8470740156776284</c:v>
+                  <c:v>901.71460079033045</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.492353844967141</c:v>
+                  <c:v>422.24045561536002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6278462686374255</c:v>
+                  <c:v>271.29627274078285</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0902782185175601</c:v>
+                  <c:v>566.18240373496428</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39.487882056163933</c:v>
+                  <c:v>1161.7352281226636</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>891.56807840391821</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -837,7 +973,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>typescript-is</c:v>
+                  <c:v>io-ts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -854,9 +990,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>is!$A$12:$A$17</c:f>
+              <c:f>is!$A$12:$A$19</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>object (hierarchical)</c:v>
                 </c:pt>
@@ -864,15 +1000,21 @@
                   <c:v>object (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>object (union)</c:v>
+                  <c:v>object (union, explicit)</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>array (recursive)</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>array (union)</c:v>
-                </c:pt>
                 <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>ultimate union</c:v>
                 </c:pt>
               </c:strCache>
@@ -880,27 +1022,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>is!$C$12:$C$17</c:f>
+              <c:f>is!$C$12:$C$19</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>24.686748581252402</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>61.417791838196351</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>110.48324387994364</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>71.044544099691151</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>52.556967635424805</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>146.08439380224709</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>134.66523123010671</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -920,7 +1068,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ajv</c:v>
+                  <c:v>zod</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -937,9 +1085,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>is!$A$12:$A$17</c:f>
+              <c:f>is!$A$12:$A$19</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>object (hierarchical)</c:v>
                 </c:pt>
@@ -947,15 +1095,21 @@
                   <c:v>object (recursive)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>object (union)</c:v>
+                  <c:v>object (union, explicit)</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>array (recursive)</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>array (union)</c:v>
-                </c:pt>
                 <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>ultimate union</c:v>
                 </c:pt>
               </c:strCache>
@@ -963,26 +1117,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>is!$D$12:$D$17</c:f>
+              <c:f>is!$D$12:$D$19</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.6119307886419818</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -991,6 +1151,101 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-AE94-4DA0-AC65-7A634C8FAF91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>is!$E$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ajv</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>is!$A$12:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ultimate union</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>is!$E$12:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>216.24995217345088</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.488059156369793</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1E9D-4D32-926B-DCF95800B033}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1078,7 +1333,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="##,##0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5568,16 +5823,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>169544</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>188594</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5609,16 +5864,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>249554</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1904</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>249554</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>1905</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6066,20 +6321,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4DC42C-376D-41DF-9AD8-63D3F4858048}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6087,76 +6342,125 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>14331.255728689201</v>
+      </c>
+      <c r="C2">
+        <v>3807.7773682270499</v>
+      </c>
+      <c r="D2">
+        <v>414.827078734363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>19578.474514117999</v>
-      </c>
-      <c r="C2">
-        <v>22471.382289416801</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>10799.172215224</v>
+      </c>
+      <c r="C3">
+        <v>1628.4722222222199</v>
+      </c>
+      <c r="D3">
+        <v>74.277350896450699</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>2991.8181818181802</v>
+      </c>
+      <c r="C4">
+        <v>1102.9331390052801</v>
+      </c>
+      <c r="D4">
+        <v>30.884502923976601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>2732.98239244872</v>
+      </c>
+      <c r="C5">
+        <v>748.54317499558499</v>
+      </c>
+      <c r="D5">
+        <v>48.030018761725998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>767.231846664209</v>
+      </c>
+      <c r="C6">
+        <v>147.167034584253</v>
+      </c>
+      <c r="D6">
+        <v>9.1554559043348203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>1262.4542124542099</v>
+      </c>
+      <c r="C7">
+        <v>70.546105640107399</v>
+      </c>
+      <c r="D7">
+        <v>2.6143790849673199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>1304.3317972350201</v>
+      </c>
+      <c r="C8">
+        <v>92.228713046556905</v>
+      </c>
+      <c r="D8">
+        <v>3.2039200904636198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>127.202255109231</v>
+      </c>
+      <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>20536.4943065148</v>
-      </c>
-      <c r="C3">
-        <v>22763.3756205184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4">
-        <v>4617.0450316337901</v>
-      </c>
-      <c r="C4">
-        <v>2349.6708119970699</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>1703.66320393657</v>
-      </c>
-      <c r="C5">
-        <v>1568.1148748159001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>3019.8165137614601</v>
-      </c>
-      <c r="C6">
-        <v>234.905487245366</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7">
-        <v>4471.8106252258704</v>
-      </c>
-      <c r="C7">
-        <v>34.906854765780402</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -6164,94 +6468,147 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1">
-        <f t="shared" ref="B12:C17" si="0" xml:space="preserve"> B2/MIN($B2:$C2)</f>
-        <v>1</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" si="0"/>
-        <v>1.1477596108528645</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1">
+      <c r="B12" s="3">
+        <f xml:space="preserve"> B2/MIN($B2:$D2)</f>
+        <v>34.547541526010903</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ref="C12:D12" si="0" xml:space="preserve"> C2/MIN($B2:$D2)</f>
+        <v>9.1791919173757286</v>
+      </c>
+      <c r="D12" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C13" s="1">
-        <f t="shared" si="0"/>
-        <v>1.1084353191331768</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" ref="B13:D13" si="1" xml:space="preserve"> B3/MIN($B3:$D3)</f>
+        <v>145.38984071038044</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="1"/>
+        <v>21.924209770114938</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1">
-        <f t="shared" si="0"/>
-        <v>1.9649752671990666</v>
-      </c>
-      <c r="C14" s="1">
-        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" ref="B14:D14" si="2" xml:space="preserve"> B4/MIN($B4:$D4)</f>
+        <v>96.871178052716488</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="2"/>
+        <v>35.711539270040795</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="1">
-        <f t="shared" si="0"/>
-        <v>1.0864403056801457</v>
-      </c>
-      <c r="C15" s="1">
-        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" ref="B15:D15" si="3" xml:space="preserve"> B5/MIN($B5:$D5)</f>
+        <v>56.901547467780084</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="3"/>
+        <v>15.584902823150292</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1">
-        <f t="shared" si="0"/>
-        <v>12.855453268348597</v>
-      </c>
-      <c r="C16" s="1">
-        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" ref="B16:D16" si="4" xml:space="preserve"> B6/MIN($B6:$D6)</f>
+        <v>83.800507007078579</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="4"/>
+        <v>16.074244267243323</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <f t="shared" si="0"/>
-        <v>128.10694791126352</v>
-      </c>
-      <c r="C17" s="1">
-        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" ref="B17:D17" si="5" xml:space="preserve"> B7/MIN($B7:$D7)</f>
+        <v>482.88873626373538</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="5"/>
+        <v>26.983885407341084</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" ref="B18:D18" si="6" xml:space="preserve"> B8/MIN($B8:$D8)</f>
+        <v>407.10497153700175</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="6"/>
+        <v>28.786208907354819</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" ref="B19:D19" si="7" xml:space="preserve"> B9/MIN($B9:$D9)</f>
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6262,20 +6619,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AA11DE-36E1-4DB2-967D-EB7E691732BC}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6283,125 +6640,152 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" s="2">
+        <v>103477.36625514401</v>
+      </c>
+      <c r="C2" s="2">
+        <v>8938.4643985870898</v>
+      </c>
+      <c r="D2" s="2">
+        <v>362.07540126913</v>
+      </c>
+      <c r="E2">
+        <v>78298.788207632402</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>67138.165137614604</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4572.9301124838603</v>
+      </c>
+      <c r="D3" s="2">
+        <v>74.456114028507102</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2">
-        <v>108212.346125995</v>
-      </c>
-      <c r="C2" s="2">
-        <v>53282.564762079703</v>
-      </c>
-      <c r="D2" s="2">
-        <v>85887.8066378066</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B4" s="2">
+        <v>12969.0385659967</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3393.47268060139</v>
+      </c>
+      <c r="D4" s="2">
+        <v>30.714817572598601</v>
+      </c>
+      <c r="E4">
+        <v>1212.86853328388</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2">
+        <v>12926.197907104801</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3384.99245852187</v>
+      </c>
+      <c r="D5" s="2">
+        <v>47.646057855927403</v>
+      </c>
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
-        <v>87932.663690476096</v>
-      </c>
-      <c r="C3" s="2">
-        <v>47606.464572680699</v>
-      </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="2">
-        <v>15761.783901377799</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1261.71449328005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B6" s="2">
+        <v>5454.3450303141599</v>
+      </c>
+      <c r="C6" s="2">
+        <v>506.31003955547101</v>
+      </c>
+      <c r="D6" s="2">
+        <v>9.6335474121647096</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2">
-        <v>15195.213430969799</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>7277.8394376618498</v>
-      </c>
-      <c r="C6" s="2">
-        <v>4470.8395245170796</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7" s="2">
+        <v>3036.6492146596802</v>
+      </c>
+      <c r="C7" s="2">
+        <v>381.84867685426701</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.6138909634055199</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="2">
-        <v>7925.2662504590498</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1117.7651999269599</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
       <c r="B8" s="2">
-        <v>7013.8045278851396</v>
+        <v>3017.1508575428702</v>
       </c>
       <c r="C8" s="2">
-        <v>1205.12344533135</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>455.71990263995502</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3.3840947546531299</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
-        <v>11709.4732923878</v>
-      </c>
-      <c r="C9" s="2">
-        <v>296.53333333333302</v>
+        <v>593.20477502295603</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -6409,121 +6793,182 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12" s="3">
+        <f xml:space="preserve"> B2 / MIN($B2:$E2)</f>
+        <v>285.78955071910411</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ref="C12:E12" si="0" xml:space="preserve"> C2 / MIN($B2:$E2)</f>
+        <v>24.686748581252402</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>216.24995217345088</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="1">
-        <f xml:space="preserve"> B2 / MIN($B2:$D2)</f>
-        <v>2.0309147393559384</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" ref="C12:D12" si="0" xml:space="preserve"> C2 / MIN($B2:$D2)</f>
+      <c r="B13" s="3">
+        <f t="shared" ref="B13:E13" si="1" xml:space="preserve"> B3 / MIN($B3:$E3)</f>
+        <v>901.71460079033045</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="1"/>
+        <v>61.417791838196351</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>1.6119307886419818</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1">
-        <f xml:space="preserve"> B3 / MIN($B3:$D3)</f>
-        <v>1.8470740156776284</v>
-      </c>
-      <c r="C13" s="1">
-        <f t="shared" ref="C13:D13" si="1" xml:space="preserve"> C3 / MIN($B3:$D3)</f>
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="e">
+      <c r="E13" s="3" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1">
-        <f xml:space="preserve"> B4 / MIN($B4:$D4)</f>
-        <v>12.492353844967141</v>
-      </c>
-      <c r="C14" s="1" t="e">
-        <f t="shared" ref="C14:D14" si="2" xml:space="preserve"> C4 / MIN($B4:$D4)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D14" s="1">
+        <v>19</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" ref="B14:E14" si="2" xml:space="preserve"> B4 / MIN($B4:$E4)</f>
+        <v>422.24045561536002</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="2"/>
+        <v>110.48324387994364</v>
+      </c>
+      <c r="D14" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="3">
+        <f t="shared" si="2"/>
+        <v>39.488059156369793</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="1">
-        <f xml:space="preserve"> B6 / MIN($B6:$D6)</f>
-        <v>1.6278462686374255</v>
-      </c>
-      <c r="C15" s="1">
-        <f t="shared" ref="C15:D15" si="3" xml:space="preserve"> C6 / MIN($B6:$D6)</f>
+        <v>20</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" ref="B15:E15" si="3" xml:space="preserve"> B5 / MIN($B5:$E5)</f>
+        <v>271.29627274078285</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="3"/>
+        <v>71.044544099691151</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="D15" s="1" t="e">
+      <c r="E15" s="3" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1">
-        <f xml:space="preserve"> B7 / MIN($B7:$D7)</f>
-        <v>7.0902782185175601</v>
-      </c>
-      <c r="C16" s="1">
-        <f t="shared" ref="C16:D16" si="4" xml:space="preserve"> C7 / MIN($B7:$D7)</f>
+        <v>5</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" ref="B16:E16" si="4" xml:space="preserve"> B6 / MIN($B6:$E6)</f>
+        <v>566.18240373496428</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="4"/>
+        <v>52.556967635424805</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D16" s="1" t="e">
+      <c r="E16" s="3" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <f xml:space="preserve"> B9 / MIN($B9:$D9)</f>
-        <v>39.487882056163933</v>
-      </c>
-      <c r="C17" s="1">
-        <f t="shared" ref="C17:D17" si="5" xml:space="preserve"> C9 / MIN($B9:$D9)</f>
+        <v>21</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" ref="B17:E17" si="5" xml:space="preserve"> B7 / MIN($B7:$E7)</f>
+        <v>1161.7352281226636</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="5"/>
+        <v>146.08439380224709</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="D17" s="1" t="e">
+      <c r="E17" s="3" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" ref="B18:E18" si="6" xml:space="preserve"> B8 / MIN($B8:$E8)</f>
+        <v>891.56807840391821</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="6"/>
+        <v>134.66523123010671</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="3" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" ref="B19:E19" si="7" xml:space="preserve"> B9 / MIN($B9:$E9)</f>
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6536,20 +6981,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EFA07C-E270-4B85-8B26-6FA6BD53AA2B}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6557,18 +7002,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>153388.39848675899</v>
@@ -6580,9 +7025,9 @@
         <v>4226.6036707250496</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>5112.9676716309395</v>
@@ -6594,9 +7039,9 @@
         <v>1225.8186636380799</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>5599.7051234795399</v>
@@ -6608,9 +7053,9 @@
         <v>924.14831545266304</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2">
         <v>2150.9571558796702</v>
@@ -6622,9 +7067,9 @@
         <v>500.093510379652</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>381.49763722282802</v>
@@ -6636,9 +7081,9 @@
         <v>97.656982193064593</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>253.86313465783601</v>
@@ -6650,9 +7095,9 @@
         <v>70.606003398149895</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2">
         <v>392.47510143858301</v>
@@ -6664,24 +7109,24 @@
         <v>151.226656902233</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <v>1237.2001432151801</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2">
         <v>137.174721189591</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -6689,16 +7134,16 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>7</v>
-      </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>8</v>
       </c>
       <c r="B13" s="1">
         <f xml:space="preserve"> B2 / $D2</f>
@@ -6714,9 +7159,9 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" ref="B14:D14" si="1" xml:space="preserve"> B3 / $D3</f>
@@ -6732,9 +7177,9 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" ref="B15:D15" si="2" xml:space="preserve"> B4 / $D4</f>
@@ -6750,9 +7195,9 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" ref="B16:D16" si="3" xml:space="preserve"> B5 / $D5</f>
@@ -6768,9 +7213,9 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" ref="B17:D17" si="4" xml:space="preserve"> B6 / $D6</f>
@@ -6786,9 +7231,9 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" ref="B18:D18" si="5" xml:space="preserve"> B7 / $D7</f>
@@ -6804,9 +7249,9 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" ref="B19:D19" si="6" xml:space="preserve"> B8 / $D8</f>
@@ -6821,9 +7266,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1">
         <f t="shared" ref="B20:D20" si="7" xml:space="preserve"> B9 / $D9</f>
@@ -6838,12 +7283,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -6863,16 +7308,16 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6880,15 +7325,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
       </c>
       <c r="B2">
         <v>142008.388037928</v>
@@ -6900,9 +7345,9 @@
         <v>4262.1504972790399</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>5000.5586592178697</v>
@@ -6914,9 +7359,9 @@
         <v>1191.4353111957901</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>5470.67612999626</v>
@@ -6928,9 +7373,9 @@
         <v>980.59339428997896</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>2229.7124015387399</v>
@@ -6942,9 +7387,9 @@
         <v>520.87250846182701</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>100.912506709608</v>
@@ -6956,9 +7401,9 @@
         <v>30.766396462785501</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>260.65393093313702</v>
@@ -6970,9 +7415,9 @@
         <v>78.568723968193794</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>401.92342587552099</v>
@@ -6984,21 +7429,21 @@
         <v>181.146025878003</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>1263.3490737377399</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>145.03957297993699</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -7006,15 +7451,15 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>8</v>
       </c>
       <c r="B12" s="1">
         <f xml:space="preserve"> B2 / MIN($B2:$E2)</f>
@@ -7030,9 +7475,9 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" ref="B13:D19" si="1" xml:space="preserve"> B3 / MIN($B3:$E3)</f>
@@ -7048,9 +7493,9 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="1"/>
@@ -7066,9 +7511,9 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="1"/>
@@ -7084,9 +7529,9 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="1"/>
@@ -7102,9 +7547,9 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" si="1"/>
@@ -7120,9 +7565,9 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="1"/>
@@ -7138,9 +7583,9 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" si="1"/>
@@ -7170,30 +7615,30 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2">
         <v>153388.39848675899</v>
@@ -7205,23 +7650,23 @@
         <v>4226.6036707250496</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2">
         <v>58990.632318501099</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2">
         <v>5621.0191082802503</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2">
         <v>32103.674063295701</v>
@@ -7233,9 +7678,9 @@
         <v>5722.3155929038203</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2">
         <v>40660.655737704903</v>

</xml_diff>

<commit_message>
Benchmark #245 by AMD 5800H
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3273E2B-EA45-4164-831E-9B279431CA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA91064-C476-41BC-A11A-E67F31B7E87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
   <sheets>
     <sheet name="validate" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="28">
   <si>
     <t>Components</t>
   </si>
@@ -116,6 +116,12 @@
   <si>
     <t>zod</t>
   </si>
+  <si>
+    <t>class-validator</t>
+  </si>
+  <si>
+    <t>class-validatr</t>
+  </si>
 </sst>
 </file>
 
@@ -124,7 +130,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="##,##0%"/>
+    <numFmt numFmtId="165" formatCode="##,##0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -168,7 +174,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="백분율" xfId="1" builtinId="5"/>
@@ -344,25 +350,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>34.547541526010903</c:v>
+                  <c:v>180.81665526735807</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>145.38984071038044</c:v>
+                  <c:v>289.52621213475066</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96.871178052716488</c:v>
+                  <c:v>103.01753079363435</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.901547467780084</c:v>
+                  <c:v>73.714847791691994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>83.800507007078579</c:v>
+                  <c:v>171.84806722414336</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>482.88873626373538</c:v>
+                  <c:v>568.97534134909392</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>407.10497153700175</c:v>
+                  <c:v>445.75068946497305</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -385,7 +391,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>io-ts</c:v>
+                  <c:v>class-validator</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -439,25 +445,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>9.1791919173757286</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.924209770114938</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.711539270040795</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.584902823150292</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.074244267243323</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.983885407341084</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.786208907354819</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -480,7 +486,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>zod</c:v>
+                  <c:v>io-ts</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -534,25 +540,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>38.242355413178629</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>26.656482581916201</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>36.898599776344994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>16.413439129808197</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>27.625897533452559</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>25.837053156763425</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>30.860122927919498</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -563,6 +569,101 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3912-4FEA-81A6-1045CDC68000}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>validate!$E$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>zod</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>validate!$A$12:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ultimate union</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>validate!$E$12:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.2298354481337066</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0924739982300715</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6866228105190906</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-83BA-4704-941C-FD22C3C356F5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -932,25 +1033,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>285.78955071910411</c:v>
+                  <c:v>1040.8371146944341</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>901.71460079033045</c:v>
+                  <c:v>1162.6773986418757</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>422.24045561536002</c:v>
+                  <c:v>402.97851685267648</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>271.29627274078285</c:v>
+                  <c:v>269.52918236593331</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>566.18240373496428</c:v>
+                  <c:v>1387.7544368464478</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1161.7352281226636</c:v>
+                  <c:v>1303.3687616214222</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>891.56807840391821</c:v>
+                  <c:v>953.33491599707736</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -1027,25 +1128,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>24.686748581252402</c:v>
+                  <c:v>89.148994297215694</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>61.417791838196351</c:v>
+                  <c:v>73.286931818181756</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110.48324387994364</c:v>
+                  <c:v>98.464946900114825</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>71.044544099691151</c:v>
+                  <c:v>62.461725022909675</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52.556967635424805</c:v>
+                  <c:v>92.645439530189066</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>146.08439380224709</c:v>
+                  <c:v>136.61249290176056</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>134.66523123010671</c:v>
+                  <c:v>117.88817518248167</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1068,7 +1169,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>zod</c:v>
+                  <c:v>class-validatr</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1122,25 +1223,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1163,7 +1264,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ajv</c:v>
+                  <c:v>zod</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1217,25 +1318,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>216.24995217345088</c:v>
+                  <c:v>4.0051071233145734</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.0650411225514806</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.488059156369793</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.639145869191051</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1246,6 +1347,196 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1E9D-4D32-926B-DCF95800B033}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>is!$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ajv</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>is!$A$12:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ultimate union</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>is!$F$12:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>854.44079846613874</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35.33379836181058</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0079-472B-9DA3-A1B244DEE484}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>is!$G$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>class-validator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>is!$A$12:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ultimate union</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>is!$G$12:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0079-472B-9DA3-A1B244DEE484}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5864,16 +6155,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1904</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180022</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180023</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6321,20 +6612,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4DC42C-376D-41DF-9AD8-63D3F4858048}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="B12" sqref="B12:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6342,116 +6633,140 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>14331.255728689201</v>
+        <v>18456.513828238702</v>
       </c>
       <c r="C2">
-        <v>3807.7773682270499</v>
+        <v>102.07308503162299</v>
       </c>
       <c r="D2">
-        <v>414.827078734363</v>
+        <v>3903.51519589893</v>
+      </c>
+      <c r="E2">
+        <v>431.75235336712501</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>10799.172215224</v>
+        <v>19118.156682027598</v>
       </c>
       <c r="C3">
-        <v>1628.4722222222199</v>
+        <v>66.032558990305404</v>
       </c>
       <c r="D3">
-        <v>74.277350896450699</v>
+        <v>1760.19575856443</v>
+      </c>
+      <c r="E3">
+        <v>72.138853733502003</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4">
-        <v>2991.8181818181802</v>
-      </c>
-      <c r="C4">
-        <v>1102.9331390052801</v>
+        <v>3510.6532840288701</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>30.884502923976601</v>
+        <v>1257.4383164005801</v>
+      </c>
+      <c r="E4">
+        <v>34.078212290502698</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5">
-        <v>2732.98239244872</v>
-      </c>
-      <c r="C5">
-        <v>748.54317499558499</v>
+        <v>3848.0163903892699</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>48.030018761725998</v>
+        <v>856.804086099963</v>
+      </c>
+      <c r="E5">
+        <v>52.201374698123701</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>767.231846664209</v>
+        <v>729.64843015604401</v>
       </c>
       <c r="C6">
-        <v>147.167034584253</v>
+        <v>4.2458925604578104</v>
       </c>
       <c r="D6">
-        <v>9.1554559043348203</v>
+        <v>117.296592813256</v>
+      </c>
+      <c r="E6">
+        <v>7.1612192434814501</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
       <c r="B7">
-        <v>1262.4542124542099</v>
-      </c>
-      <c r="C7">
-        <v>70.546105640107399</v>
+        <v>1485.02139800285</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>2.6143790849673199</v>
+        <v>67.434516069106394</v>
+      </c>
+      <c r="E7">
+        <v>2.6099925428784401</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="B8">
-        <v>1304.3317972350201</v>
-      </c>
-      <c r="C8">
-        <v>92.228713046556905</v>
+        <v>1603.41974627688</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>3.2039200904636198</v>
+        <v>111.007636431365</v>
+      </c>
+      <c r="E8">
+        <v>3.5971223021582701</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9">
-        <v>127.202255109231</v>
+        <v>153.92819054390301</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -6459,8 +6774,11 @@
       <c r="D9" t="s">
         <v>4</v>
       </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -6468,137 +6786,168 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="3">
-        <f xml:space="preserve"> B2/MIN($B2:$D2)</f>
-        <v>34.547541526010903</v>
+        <f xml:space="preserve"> B2/MIN($B2:$E2)</f>
+        <v>180.81665526735807</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" ref="C12:D12" si="0" xml:space="preserve"> C2/MIN($B2:$D2)</f>
-        <v>9.1791919173757286</v>
+        <f t="shared" ref="C12:E12" si="0" xml:space="preserve"> C2/MIN($B2:$E2)</f>
+        <v>1</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>38.242355413178629</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>4.2298354481337066</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" ref="B13:D13" si="1" xml:space="preserve"> B3/MIN($B3:$D3)</f>
-        <v>145.38984071038044</v>
+        <f t="shared" ref="B13:E13" si="1" xml:space="preserve"> B3/MIN($B3:$E3)</f>
+        <v>289.52621213475066</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="1"/>
-        <v>21.924209770114938</v>
+        <v>1</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>26.656482581916201</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0924739982300715</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="3">
-        <f t="shared" ref="B14:D14" si="2" xml:space="preserve"> B4/MIN($B4:$D4)</f>
-        <v>96.871178052716488</v>
-      </c>
-      <c r="C14" s="3">
+        <f t="shared" ref="B14:E14" si="2" xml:space="preserve"> B4/MIN($B4:$E4)</f>
+        <v>103.01753079363435</v>
+      </c>
+      <c r="C14" s="3" t="e">
         <f t="shared" si="2"/>
-        <v>35.711539270040795</v>
+        <v>#VALUE!</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="2"/>
+        <v>36.898599776344994</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="3">
-        <f t="shared" ref="B15:D15" si="3" xml:space="preserve"> B5/MIN($B5:$D5)</f>
-        <v>56.901547467780084</v>
-      </c>
-      <c r="C15" s="3">
+        <f t="shared" ref="B15:E15" si="3" xml:space="preserve"> B5/MIN($B5:$E5)</f>
+        <v>73.714847791691994</v>
+      </c>
+      <c r="C15" s="3" t="e">
         <f t="shared" si="3"/>
-        <v>15.584902823150292</v>
+        <v>#VALUE!</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" si="3"/>
+        <v>16.413439129808197</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="3">
-        <f t="shared" ref="B16:D16" si="4" xml:space="preserve"> B6/MIN($B6:$D6)</f>
-        <v>83.800507007078579</v>
+        <f t="shared" ref="B16:E16" si="4" xml:space="preserve"> B6/MIN($B6:$E6)</f>
+        <v>171.84806722414336</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="4"/>
-        <v>16.074244267243323</v>
+        <v>1</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>27.625897533452559</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="4"/>
+        <v>1.6866228105190906</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" ref="B17:D17" si="5" xml:space="preserve"> B7/MIN($B7:$D7)</f>
-        <v>482.88873626373538</v>
-      </c>
-      <c r="C17" s="3">
+        <f t="shared" ref="B17:E17" si="5" xml:space="preserve"> B7/MIN($B7:$E7)</f>
+        <v>568.97534134909392</v>
+      </c>
+      <c r="C17" s="3" t="e">
         <f t="shared" si="5"/>
-        <v>26.983885407341084</v>
+        <v>#VALUE!</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="5"/>
+        <v>25.837053156763425</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" ref="B18:D18" si="6" xml:space="preserve"> B8/MIN($B8:$D8)</f>
-        <v>407.10497153700175</v>
-      </c>
-      <c r="C18" s="3">
+        <f t="shared" ref="B18:E18" si="6" xml:space="preserve"> B8/MIN($B8:$E8)</f>
+        <v>445.75068946497305</v>
+      </c>
+      <c r="C18" s="3" t="e">
         <f t="shared" si="6"/>
-        <v>28.786208907354819</v>
+        <v>#VALUE!</v>
       </c>
       <c r="D18" s="3">
         <f t="shared" si="6"/>
+        <v>30.860122927919498</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" ref="B19:D19" si="7" xml:space="preserve"> B9/MIN($B9:$D9)</f>
+        <f t="shared" ref="B19:E19" si="7" xml:space="preserve"> B9/MIN($B9:$E9)</f>
         <v>1</v>
       </c>
       <c r="C19" s="3" t="e">
@@ -6606,6 +6955,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="D19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E19" s="3" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
@@ -6619,20 +6972,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AA11DE-36E1-4DB2-967D-EB7E691732BC}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6643,137 +6996,185 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>103477.36625514401</v>
+        <v>103094.61187214599</v>
       </c>
       <c r="C2" s="2">
-        <v>8938.4643985870898</v>
-      </c>
-      <c r="D2" s="2">
-        <v>362.07540126913</v>
+        <v>8830.1818181818107</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="E2">
-        <v>78298.788207632402</v>
+        <v>396.70468948035398</v>
+      </c>
+      <c r="F2">
+        <v>84632.111251580194</v>
+      </c>
+      <c r="G2">
+        <v>99.049707602339097</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>67138.165137614604</v>
+        <v>74587.651598676894</v>
       </c>
       <c r="C3" s="2">
-        <v>4572.9301124838603</v>
-      </c>
-      <c r="D3" s="2">
-        <v>74.456114028507102</v>
-      </c>
-      <c r="E3" t="s">
+        <v>4701.47621651175</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E3">
+        <v>68.324125230202498</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>64.151631128120997</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="2">
-        <v>12969.0385659967</v>
+        <v>13381.1512620301</v>
       </c>
       <c r="C4" s="2">
-        <v>3393.47268060139</v>
-      </c>
-      <c r="D4" s="2">
-        <v>30.714817572598601</v>
+        <v>3269.5895522388</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>1212.86853328388</v>
+        <v>33.205619412515901</v>
+      </c>
+      <c r="F4">
+        <v>1173.28066080086</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="2">
-        <v>12926.197907104801</v>
+        <v>13568.746548868001</v>
       </c>
       <c r="C5" s="2">
-        <v>3384.99245852187</v>
-      </c>
-      <c r="D5" s="2">
-        <v>47.646057855927403</v>
-      </c>
-      <c r="E5" t="s">
+        <v>3144.4732937685399</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E5">
+        <v>50.342402369054199</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>5454.3450303141599</v>
+        <v>7331.5328739057504</v>
       </c>
       <c r="C6" s="2">
-        <v>506.31003955547101</v>
-      </c>
-      <c r="D6" s="2">
-        <v>9.6335474121647096</v>
-      </c>
-      <c r="E6" t="s">
+        <v>489.44760506514899</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E6">
+        <v>8.6596385542168601</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>5.28301886792452</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="2">
-        <v>3036.6492146596802</v>
+        <v>3689.4756415024099</v>
       </c>
       <c r="C7" s="2">
-        <v>381.84867685426701</v>
-      </c>
-      <c r="D7" s="2">
-        <v>2.6138909634055199</v>
-      </c>
-      <c r="E7" t="s">
+        <v>386.71209540033999</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E7">
+        <v>2.8307227778826101</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="2">
-        <v>3017.1508575428702</v>
+        <v>3594.7772096420699</v>
       </c>
       <c r="C8" s="2">
-        <v>455.71990263995502</v>
-      </c>
-      <c r="D8" s="2">
-        <v>3.3840947546531299</v>
-      </c>
-      <c r="E8" t="s">
+        <v>444.52554744525497</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E8">
+        <v>3.7707390648567101</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2">
-        <v>593.20477502295603</v>
+        <v>587.32471316700003</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
@@ -6784,8 +7185,14 @@
       <c r="E9" t="s">
         <v>4</v>
       </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -6796,165 +7203,227 @@
         <v>24</v>
       </c>
       <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
         <v>25</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>18</v>
       </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="3">
-        <f xml:space="preserve"> B2 / MIN($B2:$E2)</f>
-        <v>285.78955071910411</v>
+        <f xml:space="preserve"> B2 / MIN($B2:$G2)</f>
+        <v>1040.8371146944341</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" ref="C12:E12" si="0" xml:space="preserve"> C2 / MIN($B2:$E2)</f>
-        <v>24.686748581252402</v>
-      </c>
-      <c r="D12" s="3">
+        <f t="shared" ref="C12:G12" si="0" xml:space="preserve"> C2 / MIN($B2:$G2)</f>
+        <v>89.148994297215694</v>
+      </c>
+      <c r="D12" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>4.0051071233145734</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>854.44079846613874</v>
+      </c>
+      <c r="G12" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E12" s="3">
-        <f t="shared" si="0"/>
-        <v>216.24995217345088</v>
-      </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" ref="B13:E13" si="1" xml:space="preserve"> B3 / MIN($B3:$E3)</f>
-        <v>901.71460079033045</v>
+        <f t="shared" ref="B13:G13" si="1" xml:space="preserve"> B3 / MIN($B3:$G3)</f>
+        <v>1162.6773986418757</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="1"/>
-        <v>61.417791838196351</v>
-      </c>
-      <c r="D13" s="3">
+        <v>73.286931818181756</v>
+      </c>
+      <c r="D13" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0650411225514806</v>
+      </c>
+      <c r="F13" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G13" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E13" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="3">
-        <f t="shared" ref="B14:E14" si="2" xml:space="preserve"> B4 / MIN($B4:$E4)</f>
-        <v>422.24045561536002</v>
+        <f t="shared" ref="B14:G14" si="2" xml:space="preserve"> B4 / MIN($B4:$G4)</f>
+        <v>402.97851685267648</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="2"/>
-        <v>110.48324387994364</v>
-      </c>
-      <c r="D14" s="3">
+        <v>98.464946900114825</v>
+      </c>
+      <c r="D14" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E14" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E14" s="3">
+      <c r="F14" s="3">
         <f t="shared" si="2"/>
-        <v>39.488059156369793</v>
+        <v>35.33379836181058</v>
+      </c>
+      <c r="G14" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="3">
-        <f t="shared" ref="B15:E15" si="3" xml:space="preserve"> B5 / MIN($B5:$E5)</f>
-        <v>271.29627274078285</v>
+        <f t="shared" ref="B15:G15" si="3" xml:space="preserve"> B5 / MIN($B5:$G5)</f>
+        <v>269.52918236593331</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="3"/>
-        <v>71.044544099691151</v>
-      </c>
-      <c r="D15" s="3">
+        <v>62.461725022909675</v>
+      </c>
+      <c r="D15" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E15" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="E15" s="3" t="e">
+      <c r="F15" s="3" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G15" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="3">
-        <f t="shared" ref="B16:E16" si="4" xml:space="preserve"> B6 / MIN($B6:$E6)</f>
-        <v>566.18240373496428</v>
+        <f t="shared" ref="B16:G16" si="4" xml:space="preserve"> B6 / MIN($B6:$G6)</f>
+        <v>1387.7544368464478</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="4"/>
-        <v>52.556967635424805</v>
-      </c>
-      <c r="D16" s="3">
+        <v>92.645439530189066</v>
+      </c>
+      <c r="D16" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="4"/>
+        <v>1.639145869191051</v>
+      </c>
+      <c r="F16" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G16" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E16" s="3" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" ref="B17:E17" si="5" xml:space="preserve"> B7 / MIN($B7:$E7)</f>
-        <v>1161.7352281226636</v>
+        <f t="shared" ref="B17:G17" si="5" xml:space="preserve"> B7 / MIN($B7:$G7)</f>
+        <v>1303.3687616214222</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="5"/>
-        <v>146.08439380224709</v>
-      </c>
-      <c r="D17" s="3">
+        <v>136.61249290176056</v>
+      </c>
+      <c r="D17" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E17" s="3">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="E17" s="3" t="e">
+      <c r="F17" s="3" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G17" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" ref="B18:E18" si="6" xml:space="preserve"> B8 / MIN($B8:$E8)</f>
-        <v>891.56807840391821</v>
+        <f t="shared" ref="B18:G18" si="6" xml:space="preserve"> B8 / MIN($B8:$G8)</f>
+        <v>953.33491599707736</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="6"/>
-        <v>134.66523123010671</v>
-      </c>
-      <c r="D18" s="3">
+        <v>117.88817518248167</v>
+      </c>
+      <c r="D18" s="3" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E18" s="3">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="E18" s="3" t="e">
+      <c r="F18" s="3" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
+      <c r="G18" s="3" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" ref="B19:E19" si="7" xml:space="preserve"> B9 / MIN($B9:$E9)</f>
+        <f t="shared" ref="B19:G19" si="7" xml:space="preserve"> B9 / MIN($B9:$G9)</f>
         <v>1</v>
       </c>
       <c r="C19" s="3" t="e">
@@ -6966,6 +7435,14 @@
         <v>#VALUE!</v>
       </c>
       <c r="E19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G19" s="3" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
@@ -6985,16 +7462,16 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7011,7 +7488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -7025,7 +7502,7 @@
         <v>4226.6036707250496</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7039,7 +7516,7 @@
         <v>1225.8186636380799</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -7053,7 +7530,7 @@
         <v>924.14831545266304</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -7067,7 +7544,7 @@
         <v>500.093510379652</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -7081,7 +7558,7 @@
         <v>97.656982193064593</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -7095,7 +7572,7 @@
         <v>70.606003398149895</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -7109,7 +7586,7 @@
         <v>151.226656902233</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -7123,10 +7600,10 @@
         <v>137.174721189591</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -7141,7 +7618,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -7159,7 +7636,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -7177,7 +7654,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -7195,7 +7672,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -7213,7 +7690,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -7231,7 +7708,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -7249,7 +7726,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -7266,7 +7743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -7283,12 +7760,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -7308,16 +7785,16 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7331,7 +7808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -7345,7 +7822,7 @@
         <v>4262.1504972790399</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7359,7 +7836,7 @@
         <v>1191.4353111957901</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -7373,7 +7850,7 @@
         <v>980.59339428997896</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -7387,7 +7864,7 @@
         <v>520.87250846182701</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -7401,7 +7878,7 @@
         <v>30.766396462785501</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -7415,7 +7892,7 @@
         <v>78.568723968193794</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -7429,7 +7906,7 @@
         <v>181.146025878003</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -7443,7 +7920,7 @@
         <v>145.03957297993699</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -7457,7 +7934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -7475,7 +7952,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -7493,7 +7970,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -7511,7 +7988,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -7529,7 +8006,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -7547,7 +8024,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -7565,7 +8042,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -7583,7 +8060,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -7615,14 +8092,14 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -7636,7 +8113,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -7650,7 +8127,7 @@
         <v>4226.6036707250496</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -7664,7 +8141,7 @@
         <v>5621.0191082802503</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -7678,7 +8155,7 @@
         <v>5722.3155929038203</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Close #243 and Fix #244 - enhance json schema
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA91064-C476-41BC-A11A-E67F31B7E87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8331BFDE-4609-4054-8196-C7A4210C72E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="27">
   <si>
     <t>Components</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>class-validator</t>
-  </si>
-  <si>
-    <t>class-validatr</t>
   </si>
 </sst>
 </file>
@@ -350,25 +347,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>180.81665526735807</c:v>
+                  <c:v>177.88548762189333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>289.52621213475066</c:v>
+                  <c:v>285.48461640744574</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>103.01753079363435</c:v>
+                  <c:v>113.27678103719222</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>73.714847791691994</c:v>
+                  <c:v>77.113981680337389</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>171.84806722414336</c:v>
+                  <c:v>198.99574615142848</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>568.97534134909392</c:v>
+                  <c:v>602.86563445452919</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>445.75068946497305</c:v>
+                  <c:v>393.12995750365292</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -540,25 +537,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>38.242355413178629</c:v>
+                  <c:v>38.83132619263386</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.656482581916201</c:v>
+                  <c:v>28.653605551337947</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.898599776344994</c:v>
+                  <c:v>35.384448022409337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.413439129808197</c:v>
+                  <c:v>17.283504662034783</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.625897533452559</c:v>
+                  <c:v>30.199697138265559</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.837053156763425</c:v>
+                  <c:v>31.750136587142617</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.860122927919498</c:v>
+                  <c:v>28.448447557743187</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -635,10 +632,10 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4.2298354481337066</c:v>
+                  <c:v>3.9740258211279853</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0924739982300715</c:v>
+                  <c:v>1.1192706158507841</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -647,7 +644,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6866228105190906</c:v>
+                  <c:v>1.6080597014925375</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -1033,25 +1030,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1040.8371146944341</c:v>
+                  <c:v>1108.6873102375901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1162.6773986418757</c:v>
+                  <c:v>1233.2297047228265</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>402.97851685267648</c:v>
+                  <c:v>428.19534932994344</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>269.52918236593331</c:v>
+                  <c:v>275.31251958808286</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1387.7544368464478</c:v>
+                  <c:v>1350.8549775745043</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1303.3687616214222</c:v>
+                  <c:v>1430.2182727946602</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>953.33491599707736</c:v>
+                  <c:v>1070.4890094012503</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -1128,25 +1125,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>89.148994297215694</c:v>
+                  <c:v>86.62881990922078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73.286931818181756</c:v>
+                  <c:v>73.080754716981232</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.464946900114825</c:v>
+                  <c:v>89.079062084155566</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62.461725022909675</c:v>
+                  <c:v>58.912789142933512</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>92.645439530189066</c:v>
+                  <c:v>92.14933886440248</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>136.61249290176056</c:v>
+                  <c:v>135.82375238446852</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>117.88817518248167</c:v>
+                  <c:v>124.9910997163218</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1169,7 +1166,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>class-validatr</c:v>
+                  <c:v>class-validator</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1223,10 +1220,10 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1235,7 +1232,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1318,10 +1315,10 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4.0051071233145734</c:v>
+                  <c:v>3.9618587651742567</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0650411225514806</c:v>
+                  <c:v>1.0482333373899644</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -1330,7 +1327,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.639145869191051</c:v>
+                  <c:v>1.6545801035255354</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -1413,13 +1410,13 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>854.44079846613874</c:v>
+                  <c:v>873.92143609278594</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.33379836181058</c:v>
+                  <c:v>34.938444756116368</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1442,101 +1439,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0079-472B-9DA3-A1B244DEE484}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>is!$G$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>class-validator</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>is!$A$12:$A$19</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>object (hierarchical)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>object (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>object (union, explicit)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>object (union, implicit)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>array (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>array (union, explicit)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>array (union, implicit)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ultimate union</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>is!$G$12:$G$19</c:f>
-              <c:numCache>
-                <c:formatCode>##,##0%</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0079-472B-9DA3-A1B244DEE484}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6615,7 +6517,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:E19"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6647,16 +6549,16 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>18456.513828238702</v>
+        <v>17908.146223789201</v>
       </c>
       <c r="C2">
-        <v>102.07308503162299</v>
+        <v>100.672328379334</v>
       </c>
       <c r="D2">
-        <v>3903.51519589893</v>
+        <v>3909.2400218698699</v>
       </c>
       <c r="E2">
-        <v>431.75235336712501</v>
+        <v>400.07443245254899</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -6664,16 +6566,16 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>19118.156682027598</v>
+        <v>18673.663077203801</v>
       </c>
       <c r="C3">
-        <v>66.032558990305404</v>
+        <v>65.410400434861302</v>
       </c>
       <c r="D3">
-        <v>1760.19575856443</v>
+        <v>1874.2438130155799</v>
       </c>
       <c r="E3">
-        <v>72.138853733502003</v>
+        <v>73.211939177773601</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -6681,16 +6583,16 @@
         <v>19</v>
       </c>
       <c r="B4">
-        <v>3510.6532840288701</v>
+        <v>3883.53413654618</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4">
-        <v>1257.4383164005801</v>
+        <v>1213.10572687224</v>
       </c>
       <c r="E4">
-        <v>34.078212290502698</v>
+        <v>34.283584870504903</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -6698,16 +6600,16 @@
         <v>20</v>
       </c>
       <c r="B5">
-        <v>3848.0163903892699</v>
+        <v>4063.2131860170198</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5">
-        <v>856.804086099963</v>
+        <v>910.68522871090204</v>
       </c>
       <c r="E5">
-        <v>52.201374698123701</v>
+        <v>52.691004892736103</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -6715,16 +6617,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>729.64843015604401</v>
+        <v>1108.1998114985799</v>
       </c>
       <c r="C6">
-        <v>4.2458925604578104</v>
+        <v>5.56896231668832</v>
       </c>
       <c r="D6">
-        <v>117.296592813256</v>
+        <v>168.180975338401</v>
       </c>
       <c r="E6">
-        <v>7.1612192434814501</v>
+        <v>8.9552238805970106</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -6732,16 +6634,16 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>1485.02139800285</v>
+        <v>1590.6744972414999</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7">
-        <v>67.434516069106394</v>
+        <v>83.773447459479101</v>
       </c>
       <c r="E7">
-        <v>2.6099925428784401</v>
+        <v>2.63852242744063</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -6749,16 +6651,16 @@
         <v>22</v>
       </c>
       <c r="B8">
-        <v>1603.41974627688</v>
+        <v>1399.3010851572501</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8">
-        <v>111.007636431365</v>
+        <v>101.258992805755</v>
       </c>
       <c r="E8">
-        <v>3.5971223021582701</v>
+        <v>3.55938553765455</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -6766,7 +6668,7 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>153.92819054390301</v>
+        <v>127.03983154939399</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -6801,7 +6703,7 @@
       </c>
       <c r="B12" s="3">
         <f xml:space="preserve"> B2/MIN($B2:$E2)</f>
-        <v>180.81665526735807</v>
+        <v>177.88548762189333</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:E12" si="0" xml:space="preserve"> C2/MIN($B2:$E2)</f>
@@ -6809,11 +6711,11 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>38.242355413178629</v>
+        <v>38.83132619263386</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>4.2298354481337066</v>
+        <v>3.9740258211279853</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -6822,7 +6724,7 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" ref="B13:E13" si="1" xml:space="preserve"> B3/MIN($B3:$E3)</f>
-        <v>289.52621213475066</v>
+        <v>285.48461640744574</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="1"/>
@@ -6830,11 +6732,11 @@
       </c>
       <c r="D13" s="3">
         <f t="shared" si="1"/>
-        <v>26.656482581916201</v>
+        <v>28.653605551337947</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="1"/>
-        <v>1.0924739982300715</v>
+        <v>1.1192706158507841</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -6843,7 +6745,7 @@
       </c>
       <c r="B14" s="3">
         <f t="shared" ref="B14:E14" si="2" xml:space="preserve"> B4/MIN($B4:$E4)</f>
-        <v>103.01753079363435</v>
+        <v>113.27678103719222</v>
       </c>
       <c r="C14" s="3" t="e">
         <f t="shared" si="2"/>
@@ -6851,7 +6753,7 @@
       </c>
       <c r="D14" s="3">
         <f t="shared" si="2"/>
-        <v>36.898599776344994</v>
+        <v>35.384448022409337</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="2"/>
@@ -6864,7 +6766,7 @@
       </c>
       <c r="B15" s="3">
         <f t="shared" ref="B15:E15" si="3" xml:space="preserve"> B5/MIN($B5:$E5)</f>
-        <v>73.714847791691994</v>
+        <v>77.113981680337389</v>
       </c>
       <c r="C15" s="3" t="e">
         <f t="shared" si="3"/>
@@ -6872,7 +6774,7 @@
       </c>
       <c r="D15" s="3">
         <f t="shared" si="3"/>
-        <v>16.413439129808197</v>
+        <v>17.283504662034783</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" si="3"/>
@@ -6885,7 +6787,7 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" ref="B16:E16" si="4" xml:space="preserve"> B6/MIN($B6:$E6)</f>
-        <v>171.84806722414336</v>
+        <v>198.99574615142848</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="4"/>
@@ -6893,11 +6795,11 @@
       </c>
       <c r="D16" s="3">
         <f t="shared" si="4"/>
-        <v>27.625897533452559</v>
+        <v>30.199697138265559</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="4"/>
-        <v>1.6866228105190906</v>
+        <v>1.6080597014925375</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -6906,7 +6808,7 @@
       </c>
       <c r="B17" s="3">
         <f t="shared" ref="B17:E17" si="5" xml:space="preserve"> B7/MIN($B7:$E7)</f>
-        <v>568.97534134909392</v>
+        <v>602.86563445452919</v>
       </c>
       <c r="C17" s="3" t="e">
         <f t="shared" si="5"/>
@@ -6914,7 +6816,7 @@
       </c>
       <c r="D17" s="3">
         <f t="shared" si="5"/>
-        <v>25.837053156763425</v>
+        <v>31.750136587142617</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="5"/>
@@ -6927,7 +6829,7 @@
       </c>
       <c r="B18" s="3">
         <f t="shared" ref="B18:E18" si="6" xml:space="preserve"> B8/MIN($B8:$E8)</f>
-        <v>445.75068946497305</v>
+        <v>393.12995750365292</v>
       </c>
       <c r="C18" s="3" t="e">
         <f t="shared" si="6"/>
@@ -6935,7 +6837,7 @@
       </c>
       <c r="D18" s="3">
         <f t="shared" si="6"/>
-        <v>30.860122927919498</v>
+        <v>28.448447557743187</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" si="6"/>
@@ -6974,8 +6876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AA11DE-36E1-4DB2-967D-EB7E691732BC}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6996,16 +6898,13 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
         <v>25</v>
       </c>
       <c r="F1" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -7013,22 +6912,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>103094.61187214599</v>
+        <v>108502.454099254</v>
       </c>
       <c r="C2" s="2">
-        <v>8830.1818181818107</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
+        <v>8477.9896631616393</v>
+      </c>
+      <c r="D2">
+        <v>97.865694950546597</v>
       </c>
       <c r="E2">
-        <v>396.70468948035398</v>
+        <v>387.73006134969302</v>
       </c>
       <c r="F2">
-        <v>84632.111251580194</v>
-      </c>
-      <c r="G2">
-        <v>99.049707602339097</v>
+        <v>85526.928675400195</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -7036,22 +6932,19 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>74587.651598676894</v>
+        <v>81610.789283128106</v>
       </c>
       <c r="C3" s="2">
-        <v>4701.47621651175</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
+        <v>4836.2264150943402</v>
+      </c>
+      <c r="D3">
+        <v>66.176470588235205</v>
       </c>
       <c r="E3">
-        <v>68.324125230202498</v>
+        <v>69.368382621394602</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
-      </c>
-      <c r="G3">
-        <v>64.151631128120997</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -7059,22 +6952,19 @@
         <v>19</v>
       </c>
       <c r="B4" s="2">
-        <v>13381.1512620301</v>
+        <v>14748.9509213647</v>
       </c>
       <c r="C4" s="2">
-        <v>3269.5895522388</v>
-      </c>
-      <c r="D4" s="2" t="s">
+        <v>3068.27880512091</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
       </c>
       <c r="E4">
-        <v>33.205619412515901</v>
+        <v>34.4444444444444</v>
       </c>
       <c r="F4">
-        <v>1173.28066080086</v>
-      </c>
-      <c r="G4" t="s">
-        <v>4</v>
+        <v>1203.43531937734</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -7082,21 +6972,18 @@
         <v>20</v>
       </c>
       <c r="B5" s="2">
-        <v>13568.746548868001</v>
+        <v>14495.6411187795</v>
       </c>
       <c r="C5" s="2">
-        <v>3144.4732937685399</v>
-      </c>
-      <c r="D5" s="2" t="s">
+        <v>3101.8518518518499</v>
+      </c>
+      <c r="D5" t="s">
         <v>4</v>
       </c>
       <c r="E5">
-        <v>50.342402369054199</v>
+        <v>52.6515871507318</v>
       </c>
       <c r="F5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7105,22 +6992,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>7331.5328739057504</v>
+        <v>7164.3735094477997</v>
       </c>
       <c r="C6" s="2">
-        <v>489.44760506514899</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>4</v>
+        <v>488.72180451127798</v>
+      </c>
+      <c r="D6">
+        <v>5.3035844915874097</v>
       </c>
       <c r="E6">
-        <v>8.6596385542168601</v>
+        <v>8.7752053771471203</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
-      </c>
-      <c r="G6">
-        <v>5.28301886792452</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -7128,21 +7012,18 @@
         <v>21</v>
       </c>
       <c r="B7" s="2">
-        <v>3689.4756415024099</v>
+        <v>4025.7598220904301</v>
       </c>
       <c r="C7" s="2">
-        <v>386.71209540033999</v>
-      </c>
-      <c r="D7" s="2" t="s">
+        <v>382.31493446557101</v>
+      </c>
+      <c r="D7" t="s">
         <v>4</v>
       </c>
       <c r="E7">
-        <v>2.8307227778826101</v>
+        <v>2.81478701444924</v>
       </c>
       <c r="F7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7151,21 +7032,18 @@
         <v>22</v>
       </c>
       <c r="B8" s="2">
-        <v>3594.7772096420699</v>
+        <v>3832.5402635431901</v>
       </c>
       <c r="C8" s="2">
-        <v>444.52554744525497</v>
-      </c>
-      <c r="D8" s="2" t="s">
+        <v>447.49027597703201</v>
+      </c>
+      <c r="D8" t="s">
         <v>4</v>
       </c>
       <c r="E8">
-        <v>3.7707390648567101</v>
+        <v>3.5801771245524701</v>
       </c>
       <c r="F8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7174,21 +7052,18 @@
         <v>15</v>
       </c>
       <c r="B9" s="2">
-        <v>587.32471316700003</v>
+        <v>677.60973810402004</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>4</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7203,16 +7078,13 @@
         <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
       <c r="F11" t="s">
         <v>18</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -7220,70 +7092,64 @@
         <v>2</v>
       </c>
       <c r="B12" s="3">
-        <f xml:space="preserve"> B2 / MIN($B2:$G2)</f>
-        <v>1040.8371146944341</v>
+        <f xml:space="preserve"> B2 / MIN($B2:$F2)</f>
+        <v>1108.6873102375901</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" ref="C12:G12" si="0" xml:space="preserve"> C2 / MIN($B2:$G2)</f>
-        <v>89.148994297215694</v>
-      </c>
-      <c r="D12" s="3" t="e">
+        <f t="shared" ref="C12:F12" si="0" xml:space="preserve"> C2 / MIN($B2:$F2)</f>
+        <v>86.62881990922078</v>
+      </c>
+      <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>4.0051071233145734</v>
+        <v>3.9618587651742567</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
-        <v>854.44079846613874</v>
-      </c>
-      <c r="G12" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+        <v>873.92143609278594</v>
+      </c>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" ref="B13:G13" si="1" xml:space="preserve"> B3 / MIN($B3:$G3)</f>
-        <v>1162.6773986418757</v>
+        <f t="shared" ref="B13:F13" si="1" xml:space="preserve"> B3 / MIN($B3:$F3)</f>
+        <v>1233.2297047228265</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="1"/>
-        <v>73.286931818181756</v>
-      </c>
-      <c r="D13" s="3" t="e">
+        <v>73.080754716981232</v>
+      </c>
+      <c r="D13" s="3">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="1"/>
-        <v>1.0650411225514806</v>
+        <v>1.0482333373899644</v>
       </c>
       <c r="F13" s="3" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G13" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="3">
-        <f t="shared" ref="B14:G14" si="2" xml:space="preserve"> B4 / MIN($B4:$G4)</f>
-        <v>402.97851685267648</v>
+        <f t="shared" ref="B14:F14" si="2" xml:space="preserve"> B4 / MIN($B4:$F4)</f>
+        <v>428.19534932994344</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="2"/>
-        <v>98.464946900114825</v>
+        <v>89.079062084155566</v>
       </c>
       <c r="D14" s="3" t="e">
         <f t="shared" si="2"/>
@@ -7295,24 +7161,21 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" si="2"/>
-        <v>35.33379836181058</v>
-      </c>
-      <c r="G14" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
+        <v>34.938444756116368</v>
+      </c>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="3">
-        <f t="shared" ref="B15:G15" si="3" xml:space="preserve"> B5 / MIN($B5:$G5)</f>
-        <v>269.52918236593331</v>
+        <f t="shared" ref="B15:F15" si="3" xml:space="preserve"> B5 / MIN($B5:$F5)</f>
+        <v>275.31251958808286</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="3"/>
-        <v>62.461725022909675</v>
+        <v>58.912789142933512</v>
       </c>
       <c r="D15" s="3" t="e">
         <f t="shared" si="3"/>
@@ -7326,51 +7189,45 @@
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G15" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="3">
-        <f t="shared" ref="B16:G16" si="4" xml:space="preserve"> B6 / MIN($B6:$G6)</f>
-        <v>1387.7544368464478</v>
+        <f t="shared" ref="B16:F16" si="4" xml:space="preserve"> B6 / MIN($B6:$F6)</f>
+        <v>1350.8549775745043</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="4"/>
-        <v>92.645439530189066</v>
-      </c>
-      <c r="D16" s="3" t="e">
+        <v>92.14933886440248</v>
+      </c>
+      <c r="D16" s="3">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="4"/>
-        <v>1.639145869191051</v>
+        <v>1.6545801035255354</v>
       </c>
       <c r="F16" s="3" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G16" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" ref="B17:G17" si="5" xml:space="preserve"> B7 / MIN($B7:$G7)</f>
-        <v>1303.3687616214222</v>
+        <f t="shared" ref="B17:F17" si="5" xml:space="preserve"> B7 / MIN($B7:$F7)</f>
+        <v>1430.2182727946602</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="5"/>
-        <v>136.61249290176056</v>
+        <v>135.82375238446852</v>
       </c>
       <c r="D17" s="3" t="e">
         <f t="shared" si="5"/>
@@ -7384,22 +7241,19 @@
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G17" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" ref="B18:G18" si="6" xml:space="preserve"> B8 / MIN($B8:$G8)</f>
-        <v>953.33491599707736</v>
+        <f t="shared" ref="B18:F18" si="6" xml:space="preserve"> B8 / MIN($B8:$F8)</f>
+        <v>1070.4890094012503</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="6"/>
-        <v>117.88817518248167</v>
+        <v>124.9910997163218</v>
       </c>
       <c r="D18" s="3" t="e">
         <f t="shared" si="6"/>
@@ -7413,17 +7267,14 @@
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G18" s="3" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" ref="B19:G19" si="7" xml:space="preserve"> B9 / MIN($B9:$G9)</f>
+        <f t="shared" ref="B19:F19" si="7" xml:space="preserve"> B9 / MIN($B9:$F9)</f>
         <v>1</v>
       </c>
       <c r="C19" s="3" t="e">
@@ -7442,10 +7293,7 @@
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G19" s="3" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="G19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7458,7 +7306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EFA07C-E270-4B85-8B26-6FA6BD53AA2B}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Complement #245 - benchmark `class-validator` more
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8331BFDE-4609-4054-8196-C7A4210C72E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6071010E-0277-458A-950F-CD5616D99A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="27">
   <si>
     <t>Components</t>
   </si>
@@ -347,25 +347,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>177.88548762189333</c:v>
+                  <c:v>277.0537593206289</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>285.48461640744574</c:v>
+                  <c:v>470.42700480668395</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>113.27678103719222</c:v>
+                  <c:v>241.58858151500675</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>77.113981680337389</c:v>
+                  <c:v>247.19862036343636</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>198.99574615142848</c:v>
+                  <c:v>307.46560674566746</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>602.86563445452919</c:v>
+                  <c:v>626.64004248539538</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>393.12995750365292</c:v>
+                  <c:v>443.64047402005451</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -448,19 +448,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2.4140855192238595</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.3785394932935922</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -537,25 +537,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>38.83132619263386</c:v>
+                  <c:v>63.444003503928734</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.653605551337947</c:v>
+                  <c:v>47.629561720878471</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.384448022409337</c:v>
+                  <c:v>73.061093644532463</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.283504662034783</c:v>
+                  <c:v>55.327829116800743</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.199697138265559</c:v>
+                  <c:v>49.141991878979319</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.750136587142617</c:v>
+                  <c:v>30.336174863387999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.448447557743187</c:v>
+                  <c:v>30.962962962962866</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -632,19 +632,19 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3.9740258211279853</c:v>
+                  <c:v>6.7516210554317917</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1192706158507841</c:v>
+                  <c:v>1.8249885195646147</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2.1045117651291672</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>3.1575857303756871</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6080597014925375</c:v>
+                  <c:v>2.5979891986687647</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -1030,25 +1030,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1108.6873102375901</c:v>
+                  <c:v>1676.3226172957502</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1233.2297047228265</c:v>
+                  <c:v>1892.6915885261385</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>428.19534932994344</c:v>
+                  <c:v>931.51274001237221</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>275.31251958808286</c:v>
+                  <c:v>1036.1718452221298</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1350.8549775745043</c:v>
+                  <c:v>2032.2785219178759</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1430.2182727946602</c:v>
+                  <c:v>1403.3368362213507</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1070.4890094012503</c:v>
+                  <c:v>1053.8736342042746</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -1125,25 +1125,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>86.62881990922078</c:v>
+                  <c:v>142.81631758033251</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73.080754716981232</c:v>
+                  <c:v>120.78720089546175</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>89.079062084155566</c:v>
+                  <c:v>197.87720490244936</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58.912789142933512</c:v>
+                  <c:v>191.34169090362045</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>92.14933886440248</c:v>
+                  <c:v>138.259586225487</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>135.82375238446852</c:v>
+                  <c:v>140.10399698340873</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>124.9910997163218</c:v>
+                  <c:v>122.57903406963683</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1226,19 +1226,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2.4383333333333321</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.3012899607403248</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1315,19 +1315,19 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3.9618587651742567</c:v>
+                  <c:v>6.8021114057670244</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0482333373899644</c:v>
+                  <c:v>1.7399973783325062</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2.147612563395902</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>3.1023234082317517</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6545801035255354</c:v>
+                  <c:v>2.4634160873882833</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -1410,13 +1410,13 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>873.92143609278594</c:v>
+                  <c:v>1399.945837962613</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.938444756116368</c:v>
+                  <c:v>77.802401108203966</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1509,6 +1509,7 @@
         <c:axId val="480554528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2250"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6065,8 +6066,8 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>180023</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6517,7 +6518,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6549,16 +6550,16 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>17908.146223789201</v>
+        <v>17242.957746478802</v>
       </c>
       <c r="C2">
-        <v>100.672328379334</v>
+        <v>62.236866190737601</v>
       </c>
       <c r="D2">
-        <v>3909.2400218698699</v>
+        <v>3948.5559566787001</v>
       </c>
       <c r="E2">
-        <v>400.07443245254899</v>
+        <v>420.19973619747498</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -6566,16 +6567,16 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>18673.663077203801</v>
+        <v>18419.019857897601</v>
       </c>
       <c r="C3">
-        <v>65.410400434861302</v>
+        <v>39.153831879755003</v>
       </c>
       <c r="D3">
-        <v>1874.2438130155799</v>
+        <v>1864.8798521256899</v>
       </c>
       <c r="E3">
-        <v>73.211939177773601</v>
+        <v>71.455293677515897</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -6583,16 +6584,16 @@
         <v>19</v>
       </c>
       <c r="B4">
-        <v>3883.53413654618</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
+        <v>4059.18776179202</v>
+      </c>
+      <c r="C4">
+        <v>16.802067946824199</v>
       </c>
       <c r="D4">
-        <v>1213.10572687224</v>
+        <v>1227.57745968472</v>
       </c>
       <c r="E4">
-        <v>34.283584870504903</v>
+        <v>35.360149672591199</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -6600,16 +6601,16 @@
         <v>20</v>
       </c>
       <c r="B5">
-        <v>4063.2131860170198</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
+        <v>4099.18404351767</v>
+      </c>
+      <c r="C5">
+        <v>16.582552271088598</v>
       </c>
       <c r="D5">
-        <v>910.68522871090204</v>
+        <v>917.47661837520604</v>
       </c>
       <c r="E5">
-        <v>52.691004892736103</v>
+        <v>52.360830424398301</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -6617,16 +6618,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1108.1998114985799</v>
+        <v>1097.8850832865401</v>
       </c>
       <c r="C6">
-        <v>5.56896231668832</v>
+        <v>3.5707573764329998</v>
       </c>
       <c r="D6">
-        <v>168.180975338401</v>
+        <v>175.47412999447599</v>
       </c>
       <c r="E6">
-        <v>8.9552238805970106</v>
+        <v>9.2767890950397494</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -6634,16 +6635,16 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>1590.6744972414999</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
+        <v>1772.17206585236</v>
+      </c>
+      <c r="C7">
+        <v>6.8271649299317199</v>
       </c>
       <c r="D7">
-        <v>83.773447459479101</v>
+        <v>85.792349726775896</v>
       </c>
       <c r="E7">
-        <v>2.63852242744063</v>
+        <v>2.8280542986425301</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -6651,16 +6652,16 @@
         <v>22</v>
       </c>
       <c r="B8">
-        <v>1399.3010851572501</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
+        <v>1667.82133090246</v>
+      </c>
+      <c r="C8">
+        <v>8.9418777943368095</v>
       </c>
       <c r="D8">
-        <v>101.258992805755</v>
+        <v>116.40211640211599</v>
       </c>
       <c r="E8">
-        <v>3.55938553765455</v>
+        <v>3.7593984962406002</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -6668,7 +6669,7 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>127.03983154939399</v>
+        <v>162.08268465663301</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -6703,7 +6704,7 @@
       </c>
       <c r="B12" s="3">
         <f xml:space="preserve"> B2/MIN($B2:$E2)</f>
-        <v>177.88548762189333</v>
+        <v>277.0537593206289</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:E12" si="0" xml:space="preserve"> C2/MIN($B2:$E2)</f>
@@ -6711,11 +6712,11 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>38.83132619263386</v>
+        <v>63.444003503928734</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>3.9740258211279853</v>
+        <v>6.7516210554317917</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -6724,7 +6725,7 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" ref="B13:E13" si="1" xml:space="preserve"> B3/MIN($B3:$E3)</f>
-        <v>285.48461640744574</v>
+        <v>470.42700480668395</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="1"/>
@@ -6732,11 +6733,11 @@
       </c>
       <c r="D13" s="3">
         <f t="shared" si="1"/>
-        <v>28.653605551337947</v>
+        <v>47.629561720878471</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="1"/>
-        <v>1.1192706158507841</v>
+        <v>1.8249885195646147</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -6745,19 +6746,19 @@
       </c>
       <c r="B14" s="3">
         <f t="shared" ref="B14:E14" si="2" xml:space="preserve"> B4/MIN($B4:$E4)</f>
-        <v>113.27678103719222</v>
-      </c>
-      <c r="C14" s="3" t="e">
+        <v>241.58858151500675</v>
+      </c>
+      <c r="C14" s="3">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="2"/>
-        <v>35.384448022409337</v>
+        <v>73.061093644532463</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2.1045117651291672</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -6766,19 +6767,19 @@
       </c>
       <c r="B15" s="3">
         <f t="shared" ref="B15:E15" si="3" xml:space="preserve"> B5/MIN($B5:$E5)</f>
-        <v>77.113981680337389</v>
-      </c>
-      <c r="C15" s="3" t="e">
+        <v>247.19862036343636</v>
+      </c>
+      <c r="C15" s="3">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" si="3"/>
-        <v>17.283504662034783</v>
+        <v>55.327829116800743</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3.1575857303756871</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -6787,7 +6788,7 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" ref="B16:E16" si="4" xml:space="preserve"> B6/MIN($B6:$E6)</f>
-        <v>198.99574615142848</v>
+        <v>307.46560674566746</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="4"/>
@@ -6795,11 +6796,11 @@
       </c>
       <c r="D16" s="3">
         <f t="shared" si="4"/>
-        <v>30.199697138265559</v>
+        <v>49.141991878979319</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="4"/>
-        <v>1.6080597014925375</v>
+        <v>2.5979891986687647</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -6808,15 +6809,15 @@
       </c>
       <c r="B17" s="3">
         <f t="shared" ref="B17:E17" si="5" xml:space="preserve"> B7/MIN($B7:$E7)</f>
-        <v>602.86563445452919</v>
-      </c>
-      <c r="C17" s="3" t="e">
+        <v>626.64004248539538</v>
+      </c>
+      <c r="C17" s="3">
         <f t="shared" si="5"/>
-        <v>#VALUE!</v>
+        <v>2.4140855192238595</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="5"/>
-        <v>31.750136587142617</v>
+        <v>30.336174863387999</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="5"/>
@@ -6829,15 +6830,15 @@
       </c>
       <c r="B18" s="3">
         <f t="shared" ref="B18:E18" si="6" xml:space="preserve"> B8/MIN($B8:$E8)</f>
-        <v>393.12995750365292</v>
-      </c>
-      <c r="C18" s="3" t="e">
+        <v>443.64047402005451</v>
+      </c>
+      <c r="C18" s="3">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>2.3785394932935922</v>
       </c>
       <c r="D18" s="3">
         <f t="shared" si="6"/>
-        <v>28.448447557743187</v>
+        <v>30.962962962962866</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" si="6"/>
@@ -6876,8 +6877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AA11DE-36E1-4DB2-967D-EB7E691732BC}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6912,19 +6913,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>108502.454099254</v>
+        <v>105018.208040382</v>
       </c>
       <c r="C2" s="2">
-        <v>8477.9896631616393</v>
+        <v>8947.1522942331703</v>
       </c>
       <c r="D2">
-        <v>97.865694950546597</v>
+        <v>62.647969404480001</v>
       </c>
       <c r="E2">
-        <v>387.73006134969302</v>
+        <v>426.13846723435699</v>
       </c>
       <c r="F2">
-        <v>85526.928675400195</v>
+        <v>87703.764024610893</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -6932,16 +6933,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>81610.789283128106</v>
+        <v>76773.376159885796</v>
       </c>
       <c r="C3" s="2">
-        <v>4836.2264150943402</v>
+        <v>4899.4993510105696</v>
       </c>
       <c r="D3">
-        <v>66.176470588235205</v>
+        <v>40.563067234672999</v>
       </c>
       <c r="E3">
-        <v>69.368382621394602</v>
+        <v>70.579630645456206</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
@@ -6952,19 +6953,19 @@
         <v>19</v>
       </c>
       <c r="B4" s="2">
-        <v>14748.9509213647</v>
+        <v>14951.2414537603</v>
       </c>
       <c r="C4" s="2">
-        <v>3068.27880512091</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
+        <v>3176.0272743585101</v>
+      </c>
+      <c r="D4">
+        <v>16.050495942290301</v>
       </c>
       <c r="E4">
-        <v>34.4444444444444</v>
+        <v>34.470246734397598</v>
       </c>
       <c r="F4">
-        <v>1203.43531937734</v>
+        <v>1248.7671232876701</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -6972,16 +6973,16 @@
         <v>20</v>
       </c>
       <c r="B5" s="2">
-        <v>14495.6411187795</v>
+        <v>17336.208478619901</v>
       </c>
       <c r="C5" s="2">
-        <v>3101.8518518518499</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
+        <v>3201.3410318494998</v>
+      </c>
+      <c r="D5">
+        <v>16.731016731016702</v>
       </c>
       <c r="E5">
-        <v>52.6515871507318</v>
+        <v>51.905024848150198</v>
       </c>
       <c r="F5" t="s">
         <v>4</v>
@@ -6992,16 +6993,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>7164.3735094477997</v>
+        <v>7315.8946412352398</v>
       </c>
       <c r="C6" s="2">
-        <v>488.72180451127798</v>
+        <v>497.71355405158198</v>
       </c>
       <c r="D6">
-        <v>5.3035844915874097</v>
+        <v>3.5998484274346301</v>
       </c>
       <c r="E6">
-        <v>8.7752053771471203</v>
+        <v>8.8679245283018808</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
@@ -7012,16 +7013,16 @@
         <v>21</v>
       </c>
       <c r="B7" s="2">
-        <v>4025.7598220904301</v>
+        <v>3961.9899385131298</v>
       </c>
       <c r="C7" s="2">
-        <v>382.31493446557101</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
+        <v>395.550527903469</v>
+      </c>
+      <c r="D7">
+        <v>6.8840579710144896</v>
       </c>
       <c r="E7">
-        <v>2.81478701444924</v>
+        <v>2.8232636928289101</v>
       </c>
       <c r="F7" t="s">
         <v>4</v>
@@ -7032,16 +7033,16 @@
         <v>22</v>
       </c>
       <c r="B8" s="2">
-        <v>3832.5402635431901</v>
+        <v>3938.2422802850301</v>
       </c>
       <c r="C8" s="2">
-        <v>447.49027597703201</v>
-      </c>
-      <c r="D8" t="s">
-        <v>4</v>
+        <v>458.06813927368</v>
+      </c>
+      <c r="D8">
+        <v>8.5997382688352904</v>
       </c>
       <c r="E8">
-        <v>3.5801771245524701</v>
+        <v>3.7369207772795199</v>
       </c>
       <c r="F8" t="s">
         <v>4</v>
@@ -7052,7 +7053,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="2">
-        <v>677.60973810402004</v>
+        <v>683.81818181818096</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
@@ -7093,11 +7094,11 @@
       </c>
       <c r="B12" s="3">
         <f xml:space="preserve"> B2 / MIN($B2:$F2)</f>
-        <v>1108.6873102375901</v>
+        <v>1676.3226172957502</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:F12" si="0" xml:space="preserve"> C2 / MIN($B2:$F2)</f>
-        <v>86.62881990922078</v>
+        <v>142.81631758033251</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
@@ -7105,11 +7106,11 @@
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>3.9618587651742567</v>
+        <v>6.8021114057670244</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
-        <v>873.92143609278594</v>
+        <v>1399.945837962613</v>
       </c>
       <c r="G12" s="3"/>
     </row>
@@ -7119,11 +7120,11 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" ref="B13:F13" si="1" xml:space="preserve"> B3 / MIN($B3:$F3)</f>
-        <v>1233.2297047228265</v>
+        <v>1892.6915885261385</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="1"/>
-        <v>73.080754716981232</v>
+        <v>120.78720089546175</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="1"/>
@@ -7131,7 +7132,7 @@
       </c>
       <c r="E13" s="3">
         <f t="shared" si="1"/>
-        <v>1.0482333373899644</v>
+        <v>1.7399973783325062</v>
       </c>
       <c r="F13" s="3" t="e">
         <f t="shared" si="1"/>
@@ -7145,23 +7146,23 @@
       </c>
       <c r="B14" s="3">
         <f t="shared" ref="B14:F14" si="2" xml:space="preserve"> B4 / MIN($B4:$F4)</f>
-        <v>428.19534932994344</v>
+        <v>931.51274001237221</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="2"/>
-        <v>89.079062084155566</v>
-      </c>
-      <c r="D14" s="3" t="e">
+        <v>197.87720490244936</v>
+      </c>
+      <c r="D14" s="3">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2.147612563395902</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="2"/>
-        <v>34.938444756116368</v>
+        <v>77.802401108203966</v>
       </c>
       <c r="G14" s="3"/>
     </row>
@@ -7171,19 +7172,19 @@
       </c>
       <c r="B15" s="3">
         <f t="shared" ref="B15:F15" si="3" xml:space="preserve"> B5 / MIN($B5:$F5)</f>
-        <v>275.31251958808286</v>
+        <v>1036.1718452221298</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="3"/>
-        <v>58.912789142933512</v>
-      </c>
-      <c r="D15" s="3" t="e">
+        <v>191.34169090362045</v>
+      </c>
+      <c r="D15" s="3">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3.1023234082317517</v>
       </c>
       <c r="F15" s="3" t="e">
         <f t="shared" si="3"/>
@@ -7197,11 +7198,11 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" ref="B16:F16" si="4" xml:space="preserve"> B6 / MIN($B6:$F6)</f>
-        <v>1350.8549775745043</v>
+        <v>2032.2785219178759</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="4"/>
-        <v>92.14933886440248</v>
+        <v>138.259586225487</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="4"/>
@@ -7209,7 +7210,7 @@
       </c>
       <c r="E16" s="3">
         <f t="shared" si="4"/>
-        <v>1.6545801035255354</v>
+        <v>2.4634160873882833</v>
       </c>
       <c r="F16" s="3" t="e">
         <f t="shared" si="4"/>
@@ -7223,15 +7224,15 @@
       </c>
       <c r="B17" s="3">
         <f t="shared" ref="B17:F17" si="5" xml:space="preserve"> B7 / MIN($B7:$F7)</f>
-        <v>1430.2182727946602</v>
+        <v>1403.3368362213507</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="5"/>
-        <v>135.82375238446852</v>
-      </c>
-      <c r="D17" s="3" t="e">
+        <v>140.10399698340873</v>
+      </c>
+      <c r="D17" s="3">
         <f t="shared" si="5"/>
-        <v>#VALUE!</v>
+        <v>2.4383333333333321</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="5"/>
@@ -7249,15 +7250,15 @@
       </c>
       <c r="B18" s="3">
         <f t="shared" ref="B18:F18" si="6" xml:space="preserve"> B8 / MIN($B8:$F8)</f>
-        <v>1070.4890094012503</v>
+        <v>1053.8736342042746</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="6"/>
-        <v>124.9910997163218</v>
-      </c>
-      <c r="D18" s="3" t="e">
+        <v>122.57903406963683</v>
+      </c>
+      <c r="D18" s="3">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>2.3012899607403248</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" si="6"/>
@@ -7307,7 +7308,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Complement #245 - add `assertType()` benchmarker
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6071010E-0277-458A-950F-CD5616D99A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF6F7A5-3ECE-4377-94CE-326833152AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
   <sheets>
-    <sheet name="validate" sheetId="1" r:id="rId1"/>
-    <sheet name="is" sheetId="2" r:id="rId2"/>
-    <sheet name="stringify" sheetId="3" r:id="rId3"/>
-    <sheet name="optimizer" sheetId="4" r:id="rId4"/>
-    <sheet name="cpus" sheetId="5" r:id="rId5"/>
+    <sheet name="is" sheetId="2" r:id="rId1"/>
+    <sheet name="assert" sheetId="6" r:id="rId2"/>
+    <sheet name="validate" sheetId="1" r:id="rId3"/>
+    <sheet name="stringify" sheetId="3" r:id="rId4"/>
+    <sheet name="optimizer" sheetId="4" r:id="rId5"/>
+    <sheet name="cpus" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="28">
   <si>
     <t>Components</t>
   </si>
@@ -118,6 +119,9 @@
   </si>
   <si>
     <t>class-validator</t>
+  </si>
+  <si>
+    <t>Measured by AMD 5800H</t>
   </si>
 </sst>
 </file>
@@ -238,6 +242,1469 @@
                   <a:srgbClr val="7030A0"/>
                 </a:solidFill>
               </a:rPr>
+              <a:t>is()</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
+              <a:t> function</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>is!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>typescript-json</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>is!$A$12:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ultimate union</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>is!$B$12:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1885.2411840771579</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2035.5897843152793</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1046.3862651535908</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>926.89567157730824</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1840.6355551463826</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1434.0300085564093</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1067.104121032113</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-19A9-4E7A-A359-D13A8B7C2CDC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>is!$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>io-ts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>is!$A$12:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ultimate union</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>is!$C$12:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>155.12986242884242</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>121.25522186750867</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200.37198046036829</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>193.54095847617191</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>135.9729296949024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>135.04490874159455</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120.71805760708993</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-19A9-4E7A-A359-D13A8B7C2CDC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>is!$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>class-validator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>is!$A$12:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ultimate union</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>is!$D$12:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5844398728258815</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3206575342465765</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AE94-4DA0-AC65-7A634C8FAF91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>is!$E$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>zod</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>is!$A$12:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ultimate union</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>is!$E$12:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6.7933906962394186</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7456229661508271</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1171926664884477</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.225165456788933</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3666172106824934</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1E9D-4D32-926B-DCF95800B033}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>is!$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ajv</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>is!$A$12:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ultimate union</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>is!$F$12:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1481.2023877437</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73.339569052251761</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0079-472B-9DA3-A1B244DEE484}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="249741552"/>
+        <c:axId val="480554528"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="249741552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="480554528"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="480554528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2250"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="##,##0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="249741552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:t>Runtime</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
+              <a:t> type checkers, </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" b="1" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>assert()</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
+              <a:t> function</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>assert!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>typescript-json</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>assert!$A$12:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ultimate union</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>assert!$B$12:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>371.89452250275474</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>818.68043464864797</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>301.24775200180926</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>269.65532622974769</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>451.12895232711332</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>726.62424918092529</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>511.63374411018282</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1827-4E54-BD99-1254018CEC6B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>assert!$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>class-validator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>assert!$A$12:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ultimate union</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>assert!$C$12:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3611339171684032</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3712413405729253</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1827-4E54-BD99-1254018CEC6B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>assert!$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>io-ts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>assert!$A$12:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ultimate union</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>assert!$D$12:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>63.943991040328974</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42.621749795068474</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.746037069867171</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.875396603349138</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47.028513071895269</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.178002563163748</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.841526845637556</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1827-4E54-BD99-1254018CEC6B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>assert!$E$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>zod</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>assert!$A$12:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ultimate union</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>assert!$E$12:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6.7197221105754403</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8065534008033433</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0498726778459528</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0663115909720839</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4091237407337003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1827-4E54-BD99-1254018CEC6B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="381772224"/>
+        <c:axId val="381772640"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="381772224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="381772640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="381772640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="##,##0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="381772224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:t>Runtime</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
+              <a:t> type checkers, </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" b="1" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>validate()</a:t>
             </a:r>
             <a:r>
@@ -347,25 +1814,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>277.0537593206289</c:v>
+                  <c:v>289.65993536893467</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>470.42700480668395</c:v>
+                  <c:v>456.49056540760751</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>241.58858151500675</c:v>
+                  <c:v>248.80030620158954</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>247.19862036343636</c:v>
+                  <c:v>249.41086556169481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>307.46560674566746</c:v>
+                  <c:v>310.30780959169925</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>626.64004248539538</c:v>
+                  <c:v>651.19550466497071</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>443.64047402005451</c:v>
+                  <c:v>432.37878680383005</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -457,10 +1924,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.4140855192238595</c:v>
+                  <c:v>2.5061097939084509</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3785394932935922</c:v>
+                  <c:v>2.3834729201563398</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -537,25 +2004,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>63.444003503928734</c:v>
+                  <c:v>61.457142533023699</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47.629561720878471</c:v>
+                  <c:v>45.092337422853667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>73.061093644532463</c:v>
+                  <c:v>73.504954195527205</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55.327829116800743</c:v>
+                  <c:v>54.418682111253425</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49.141991878979319</c:v>
+                  <c:v>51.047313304388936</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30.336174863387999</c:v>
+                  <c:v>30.853115819738797</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.962962962962866</c:v>
+                  <c:v>31.416931797403478</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -632,19 +2099,19 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.7516210554317917</c:v>
+                  <c:v>6.7501614846109517</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8249885195646147</c:v>
+                  <c:v>1.8076063811219343</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1045117651291672</c:v>
+                  <c:v>2.1216694474453273</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.1575857303756871</c:v>
+                  <c:v>3.1386775305300318</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5979891986687647</c:v>
+                  <c:v>2.5826379974326108</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -874,786 +2341,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="ko-KR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR"/>
-              <a:t>Runtime</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
-              <a:t> type checkers, </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR" b="1" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="7030A0"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>is()</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
-              <a:t> function</a:t>
-            </a:r>
-            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>is!$B$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>typescript-json</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>is!$A$12:$A$19</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>object (hierarchical)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>object (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>object (union, explicit)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>object (union, implicit)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>array (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>array (union, explicit)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>array (union, implicit)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ultimate union</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>is!$B$12:$B$19</c:f>
-              <c:numCache>
-                <c:formatCode>##,##0%</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1676.3226172957502</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1892.6915885261385</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>931.51274001237221</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1036.1718452221298</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2032.2785219178759</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1403.3368362213507</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1053.8736342042746</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-19A9-4E7A-A359-D13A8B7C2CDC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>is!$C$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>io-ts</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>is!$A$12:$A$19</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>object (hierarchical)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>object (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>object (union, explicit)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>object (union, implicit)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>array (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>array (union, explicit)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>array (union, implicit)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ultimate union</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>is!$C$12:$C$19</c:f>
-              <c:numCache>
-                <c:formatCode>##,##0%</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>142.81631758033251</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>120.78720089546175</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>197.87720490244936</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>191.34169090362045</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>138.259586225487</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>140.10399698340873</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>122.57903406963683</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-19A9-4E7A-A359-D13A8B7C2CDC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>is!$D$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>class-validator</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>is!$A$12:$A$19</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>object (hierarchical)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>object (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>object (union, explicit)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>object (union, implicit)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>array (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>array (union, explicit)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>array (union, implicit)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ultimate union</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>is!$D$12:$D$19</c:f>
-              <c:numCache>
-                <c:formatCode>##,##0%</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.4383333333333321</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.3012899607403248</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AE94-4DA0-AC65-7A634C8FAF91}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>is!$E$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>zod</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>is!$A$12:$A$19</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>object (hierarchical)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>object (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>object (union, explicit)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>object (union, implicit)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>array (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>array (union, explicit)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>array (union, implicit)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ultimate union</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>is!$E$12:$E$19</c:f>
-              <c:numCache>
-                <c:formatCode>##,##0%</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>6.8021114057670244</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7399973783325062</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.147612563395902</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.1023234082317517</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.4634160873882833</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1E9D-4D32-926B-DCF95800B033}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>is!$F$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ajv</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>is!$A$12:$A$19</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>object (hierarchical)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>object (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>object (union, explicit)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>object (union, implicit)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>array (recursive)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>array (union, explicit)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>array (union, implicit)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ultimate union</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>is!$F$12:$F$19</c:f>
-              <c:numCache>
-                <c:formatCode>##,##0%</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1399.945837962613</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>77.802401108203966</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0079-472B-9DA3-A1B244DEE484}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="249741552"/>
-        <c:axId val="480554528"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="249741552"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="480554528"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="480554528"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="2250"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="##,##0%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="249741552"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:dTable>
-        <c:showHorzBorder val="1"/>
-        <c:showVertBorder val="1"/>
-        <c:showOutline val="1"/>
-        <c:showKeys val="1"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr rtl="0">
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-      </c:dTable>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ko-KR"/>
@@ -2233,7 +2921,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ko-KR"/>
@@ -2795,7 +3483,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ko-KR"/>
@@ -3496,6 +4184,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5006,7 +5734,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5210,23 +5938,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -5331,8 +6058,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5464,20 +6191,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5511,7 +6237,7 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5715,6 +6441,511 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
@@ -6017,16 +7248,100 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7159</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>728</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>5255</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>5863</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="차트 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA5D48CF-3597-F49B-E0D7-3D624C52CD47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2069</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>6625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="차트 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE057987-BAF7-4497-BA52-3761F4E51E17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>188594</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2069</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>185529</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6054,48 +7369,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1904</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>180022</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="차트 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA5D48CF-3597-F49B-E0D7-3D624C52CD47}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6136,7 +7410,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6177,7 +7451,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6514,11 +7788,446 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4DC42C-376D-41DF-9AD8-63D3F4858048}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AA11DE-36E1-4DB2-967D-EB7E691732BC}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>109854.27952329299</v>
+      </c>
+      <c r="C2" s="2">
+        <v>9039.5220588235206</v>
+      </c>
+      <c r="D2">
+        <v>58.2706766917293</v>
+      </c>
+      <c r="E2">
+        <v>395.85547290116898</v>
+      </c>
+      <c r="F2">
+        <v>86310.665451230598</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>80738.984316654198</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4809.4284674190003</v>
+      </c>
+      <c r="D3">
+        <v>39.6636812282946</v>
+      </c>
+      <c r="E3">
+        <v>69.237832874196499</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2">
+        <v>17086.1564918314</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3271.8195266272101</v>
+      </c>
+      <c r="D4">
+        <v>16.3287277947245</v>
+      </c>
+      <c r="E4">
+        <v>34.571062740076798</v>
+      </c>
+      <c r="F4">
+        <v>1197.5418596366201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2">
+        <v>15526.170291190499</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3241.9504932067698</v>
+      </c>
+      <c r="D5">
+        <v>16.750720461095099</v>
+      </c>
+      <c r="E5">
+        <v>54.023845007451499</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>6923.5868164242302</v>
+      </c>
+      <c r="C6" s="2">
+        <v>511.46484745120301</v>
+      </c>
+      <c r="D6">
+        <v>3.7615196539401898</v>
+      </c>
+      <c r="E6">
+        <v>8.9020771513353107</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4047.1213788045402</v>
+      </c>
+      <c r="C7" s="2">
+        <v>381.12391930835702</v>
+      </c>
+      <c r="D7">
+        <v>7.2938096128670198</v>
+      </c>
+      <c r="E7">
+        <v>2.8222013170272802</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4031.37182105067</v>
+      </c>
+      <c r="C8" s="2">
+        <v>456.05612998522798</v>
+      </c>
+      <c r="D8">
+        <v>8.7671232876712306</v>
+      </c>
+      <c r="E8">
+        <v>3.7778617302606698</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2">
+        <v>682.35294117647004</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3">
+        <f xml:space="preserve"> B2 / MIN($B2:$F2)</f>
+        <v>1885.2411840771579</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ref="C12:F12" si="0" xml:space="preserve"> C2 / MIN($B2:$F2)</f>
+        <v>155.12986242884242</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>6.7933906962394186</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>1481.2023877437</v>
+      </c>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" ref="B13:F13" si="1" xml:space="preserve"> B3 / MIN($B3:$F3)</f>
+        <v>2035.5897843152793</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="1"/>
+        <v>121.25522186750867</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>1.7456229661508271</v>
+      </c>
+      <c r="F13" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" ref="B14:F14" si="2" xml:space="preserve"> B4 / MIN($B4:$F4)</f>
+        <v>1046.3862651535908</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="2"/>
+        <v>200.37198046036829</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="2"/>
+        <v>2.1171926664884477</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="2"/>
+        <v>73.339569052251761</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" ref="B15:F15" si="3" xml:space="preserve"> B5 / MIN($B5:$F5)</f>
+        <v>926.89567157730824</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="3"/>
+        <v>193.54095847617191</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="3"/>
+        <v>3.225165456788933</v>
+      </c>
+      <c r="F15" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" ref="B16:F16" si="4" xml:space="preserve"> B6 / MIN($B6:$F6)</f>
+        <v>1840.6355551463826</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="4"/>
+        <v>135.9729296949024</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="4"/>
+        <v>2.3666172106824934</v>
+      </c>
+      <c r="F16" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" ref="B17:F17" si="5" xml:space="preserve"> B7 / MIN($B7:$F7)</f>
+        <v>1434.0300085564093</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="5"/>
+        <v>135.04490874159455</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="5"/>
+        <v>2.5844398728258815</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F17" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" ref="B18:F18" si="6" xml:space="preserve"> B8 / MIN($B8:$F8)</f>
+        <v>1067.104121032113</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="6"/>
+        <v>120.71805760708993</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="6"/>
+        <v>2.3206575342465765</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F18" s="3" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" ref="B19:F19" si="7" xml:space="preserve"> B9 / MIN($B9:$F9)</f>
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050C2C99-5EE7-403C-9AB2-DBCB91E8248D}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6550,16 +8259,16 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>17242.957746478802</v>
+        <v>22726.5139406854</v>
       </c>
       <c r="C2">
-        <v>62.236866190737601</v>
+        <v>61.110106671487898</v>
       </c>
       <c r="D2">
-        <v>3948.5559566787001</v>
+        <v>3907.6241134751699</v>
       </c>
       <c r="E2">
-        <v>420.19973619747498</v>
+        <v>410.64293498002098</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -6567,16 +8276,16 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>18419.019857897601</v>
+        <v>32424.4669316949</v>
       </c>
       <c r="C3">
-        <v>39.153831879755003</v>
+        <v>39.605767475816698</v>
       </c>
       <c r="D3">
-        <v>1864.8798521256899</v>
+        <v>1688.06711179592</v>
       </c>
       <c r="E3">
-        <v>71.455293677515897</v>
+        <v>71.549933924863097</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -6584,16 +8293,16 @@
         <v>19</v>
       </c>
       <c r="B4">
-        <v>4059.18776179202</v>
+        <v>4944.8635057471201</v>
       </c>
       <c r="C4">
-        <v>16.802067946824199</v>
+        <v>16.4146071560309</v>
       </c>
       <c r="D4">
-        <v>1227.57745968472</v>
+        <v>1177.6830135038999</v>
       </c>
       <c r="E4">
-        <v>35.360149672591199</v>
+        <v>33.6478547267224</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -6601,16 +8310,16 @@
         <v>20</v>
       </c>
       <c r="B5">
-        <v>4099.18404351767</v>
+        <v>4664.7963800904899</v>
       </c>
       <c r="C5">
-        <v>16.582552271088598</v>
+        <v>17.2991071428571</v>
       </c>
       <c r="D5">
-        <v>917.47661837520604</v>
+        <v>897.39804391954203</v>
       </c>
       <c r="E5">
-        <v>52.360830424398301</v>
+        <v>53.044452745610698</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -6618,16 +8327,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1097.8850832865401</v>
+        <v>1708.49820991143</v>
       </c>
       <c r="C6">
-        <v>3.5707573764329998</v>
+        <v>3.7871615224389301</v>
       </c>
       <c r="D6">
-        <v>175.47412999447599</v>
+        <v>178.10457516339801</v>
       </c>
       <c r="E6">
-        <v>9.2767890950397494</v>
+        <v>9.1237407337008101</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -6635,16 +8344,16 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>1772.17206585236</v>
+        <v>2133.60029122679</v>
       </c>
       <c r="C7">
-        <v>6.8271649299317199</v>
+        <v>6.9330414158000302</v>
       </c>
       <c r="D7">
-        <v>85.792349726775896</v>
+        <v>88.612229952398394</v>
       </c>
       <c r="E7">
-        <v>2.8280542986425301</v>
+        <v>2.9363185905670699</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -6652,16 +8361,16 @@
         <v>22</v>
       </c>
       <c r="B8">
-        <v>1667.82133090246</v>
+        <v>1939.1083725987601</v>
       </c>
       <c r="C8">
-        <v>8.9418777943368095</v>
+        <v>8.9870810709604907</v>
       </c>
       <c r="D8">
-        <v>116.40211640211599</v>
+        <v>116.890380313199</v>
       </c>
       <c r="E8">
-        <v>3.7593984962406002</v>
+        <v>3.7900322152738299</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -6669,7 +8378,7 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>162.08268465663301</v>
+        <v>276.25201938610599</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -6704,7 +8413,7 @@
       </c>
       <c r="B12" s="3">
         <f xml:space="preserve"> B2/MIN($B2:$E2)</f>
-        <v>277.0537593206289</v>
+        <v>371.89452250275474</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:E12" si="0" xml:space="preserve"> C2/MIN($B2:$E2)</f>
@@ -6712,11 +8421,11 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>63.444003503928734</v>
+        <v>63.943991040328974</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>6.7516210554317917</v>
+        <v>6.7197221105754403</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -6724,8 +8433,8 @@
         <v>3</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" ref="B13:E13" si="1" xml:space="preserve"> B3/MIN($B3:$E3)</f>
-        <v>470.42700480668395</v>
+        <f t="shared" ref="B13:E19" si="1" xml:space="preserve"> B3/MIN($B3:$E3)</f>
+        <v>818.68043464864797</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="1"/>
@@ -6733,11 +8442,11 @@
       </c>
       <c r="D13" s="3">
         <f t="shared" si="1"/>
-        <v>47.629561720878471</v>
+        <v>42.621749795068474</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="1"/>
-        <v>1.8249885195646147</v>
+        <v>1.8065534008033433</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -6745,20 +8454,20 @@
         <v>19</v>
       </c>
       <c r="B14" s="3">
-        <f t="shared" ref="B14:E14" si="2" xml:space="preserve"> B4/MIN($B4:$E4)</f>
-        <v>241.58858151500675</v>
+        <f t="shared" si="1"/>
+        <v>301.24775200180926</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="2"/>
-        <v>73.061093644532463</v>
+        <f t="shared" si="1"/>
+        <v>71.746037069867171</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="2"/>
-        <v>2.1045117651291672</v>
+        <f t="shared" si="1"/>
+        <v>2.0498726778459528</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -6766,20 +8475,20 @@
         <v>20</v>
       </c>
       <c r="B15" s="3">
-        <f t="shared" ref="B15:E15" si="3" xml:space="preserve"> B5/MIN($B5:$E5)</f>
-        <v>247.19862036343636</v>
+        <f t="shared" si="1"/>
+        <v>269.65532622974769</v>
       </c>
       <c r="C15" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="3"/>
-        <v>55.327829116800743</v>
+        <f t="shared" si="1"/>
+        <v>51.875396603349138</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="3"/>
-        <v>3.1575857303756871</v>
+        <f t="shared" si="1"/>
+        <v>3.0663115909720839</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -6787,20 +8496,20 @@
         <v>5</v>
       </c>
       <c r="B16" s="3">
-        <f t="shared" ref="B16:E16" si="4" xml:space="preserve"> B6/MIN($B6:$E6)</f>
-        <v>307.46560674566746</v>
+        <f t="shared" si="1"/>
+        <v>451.12895232711332</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="4"/>
-        <v>49.141991878979319</v>
+        <f t="shared" si="1"/>
+        <v>47.028513071895269</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="4"/>
-        <v>2.5979891986687647</v>
+        <f t="shared" si="1"/>
+        <v>2.4091237407337003</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -6808,19 +8517,19 @@
         <v>21</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" ref="B17:E17" si="5" xml:space="preserve"> B7/MIN($B7:$E7)</f>
-        <v>626.64004248539538</v>
+        <f t="shared" si="1"/>
+        <v>726.62424918092529</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="5"/>
-        <v>2.4140855192238595</v>
+        <f t="shared" si="1"/>
+        <v>2.3611339171684032</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="5"/>
-        <v>30.336174863387999</v>
+        <f t="shared" si="1"/>
+        <v>30.178002563163748</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6829,19 +8538,19 @@
         <v>22</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" ref="B18:E18" si="6" xml:space="preserve"> B8/MIN($B8:$E8)</f>
-        <v>443.64047402005451</v>
+        <f t="shared" si="1"/>
+        <v>511.63374411018282</v>
       </c>
       <c r="C18" s="3">
-        <f t="shared" si="6"/>
-        <v>2.3785394932935922</v>
+        <f t="shared" si="1"/>
+        <v>2.3712413405729253</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" si="6"/>
-        <v>30.962962962962866</v>
+        <f t="shared" si="1"/>
+        <v>30.841526845637556</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6850,451 +8559,21 @@
         <v>15</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" ref="B19:E19" si="7" xml:space="preserve"> B9/MIN($B9:$E9)</f>
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D19" s="3" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E19" s="3" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AA11DE-36E1-4DB2-967D-EB7E691732BC}">
-  <dimension ref="A1:G19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>105018.208040382</v>
-      </c>
-      <c r="C2" s="2">
-        <v>8947.1522942331703</v>
-      </c>
-      <c r="D2">
-        <v>62.647969404480001</v>
-      </c>
-      <c r="E2">
-        <v>426.13846723435699</v>
-      </c>
-      <c r="F2">
-        <v>87703.764024610893</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>76773.376159885796</v>
-      </c>
-      <c r="C3" s="2">
-        <v>4899.4993510105696</v>
-      </c>
-      <c r="D3">
-        <v>40.563067234672999</v>
-      </c>
-      <c r="E3">
-        <v>70.579630645456206</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2">
-        <v>14951.2414537603</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3176.0272743585101</v>
-      </c>
-      <c r="D4">
-        <v>16.050495942290301</v>
-      </c>
-      <c r="E4">
-        <v>34.470246734397598</v>
-      </c>
-      <c r="F4">
-        <v>1248.7671232876701</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="2">
-        <v>17336.208478619901</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3201.3410318494998</v>
-      </c>
-      <c r="D5">
-        <v>16.731016731016702</v>
-      </c>
-      <c r="E5">
-        <v>51.905024848150198</v>
-      </c>
-      <c r="F5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>7315.8946412352398</v>
-      </c>
-      <c r="C6" s="2">
-        <v>497.71355405158198</v>
-      </c>
-      <c r="D6">
-        <v>3.5998484274346301</v>
-      </c>
-      <c r="E6">
-        <v>8.8679245283018808</v>
-      </c>
-      <c r="F6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2">
-        <v>3961.9899385131298</v>
-      </c>
-      <c r="C7" s="2">
-        <v>395.550527903469</v>
-      </c>
-      <c r="D7">
-        <v>6.8840579710144896</v>
-      </c>
-      <c r="E7">
-        <v>2.8232636928289101</v>
-      </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="2">
-        <v>3938.2422802850301</v>
-      </c>
-      <c r="C8" s="2">
-        <v>458.06813927368</v>
-      </c>
-      <c r="D8">
-        <v>8.5997382688352904</v>
-      </c>
-      <c r="E8">
-        <v>3.7369207772795199</v>
-      </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2">
-        <v>683.81818181818096</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="3">
-        <f xml:space="preserve"> B2 / MIN($B2:$F2)</f>
-        <v>1676.3226172957502</v>
-      </c>
-      <c r="C12" s="3">
-        <f t="shared" ref="C12:F12" si="0" xml:space="preserve"> C2 / MIN($B2:$F2)</f>
-        <v>142.81631758033251</v>
-      </c>
-      <c r="D12" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E12" s="3">
-        <f t="shared" si="0"/>
-        <v>6.8021114057670244</v>
-      </c>
-      <c r="F12" s="3">
-        <f t="shared" si="0"/>
-        <v>1399.945837962613</v>
-      </c>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="3">
-        <f t="shared" ref="B13:F13" si="1" xml:space="preserve"> B3 / MIN($B3:$F3)</f>
-        <v>1892.6915885261385</v>
-      </c>
-      <c r="C13" s="3">
-        <f t="shared" si="1"/>
-        <v>120.78720089546175</v>
-      </c>
-      <c r="D13" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E13" s="3">
-        <f t="shared" si="1"/>
-        <v>1.7399973783325062</v>
-      </c>
-      <c r="F13" s="3" t="e">
+      <c r="C19" s="3" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="3">
-        <f t="shared" ref="B14:F14" si="2" xml:space="preserve"> B4 / MIN($B4:$F4)</f>
-        <v>931.51274001237221</v>
-      </c>
-      <c r="C14" s="3">
-        <f t="shared" si="2"/>
-        <v>197.87720490244936</v>
-      </c>
-      <c r="D14" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E14" s="3">
-        <f t="shared" si="2"/>
-        <v>2.147612563395902</v>
-      </c>
-      <c r="F14" s="3">
-        <f t="shared" si="2"/>
-        <v>77.802401108203966</v>
-      </c>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="3">
-        <f t="shared" ref="B15:F15" si="3" xml:space="preserve"> B5 / MIN($B5:$F5)</f>
-        <v>1036.1718452221298</v>
-      </c>
-      <c r="C15" s="3">
-        <f t="shared" si="3"/>
-        <v>191.34169090362045</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="E15" s="3">
-        <f t="shared" si="3"/>
-        <v>3.1023234082317517</v>
-      </c>
-      <c r="F15" s="3" t="e">
-        <f t="shared" si="3"/>
+      <c r="D19" s="3" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="3">
-        <f t="shared" ref="B16:F16" si="4" xml:space="preserve"> B6 / MIN($B6:$F6)</f>
-        <v>2032.2785219178759</v>
-      </c>
-      <c r="C16" s="3">
-        <f t="shared" si="4"/>
-        <v>138.259586225487</v>
-      </c>
-      <c r="D16" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="shared" si="4"/>
-        <v>2.4634160873882833</v>
-      </c>
-      <c r="F16" s="3" t="e">
-        <f t="shared" si="4"/>
+      <c r="E19" s="3" t="e">
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="3">
-        <f t="shared" ref="B17:F17" si="5" xml:space="preserve"> B7 / MIN($B7:$F7)</f>
-        <v>1403.3368362213507</v>
-      </c>
-      <c r="C17" s="3">
-        <f t="shared" si="5"/>
-        <v>140.10399698340873</v>
-      </c>
-      <c r="D17" s="3">
-        <f t="shared" si="5"/>
-        <v>2.4383333333333321</v>
-      </c>
-      <c r="E17" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="F17" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="3">
-        <f t="shared" ref="B18:F18" si="6" xml:space="preserve"> B8 / MIN($B8:$F8)</f>
-        <v>1053.8736342042746</v>
-      </c>
-      <c r="C18" s="3">
-        <f t="shared" si="6"/>
-        <v>122.57903406963683</v>
-      </c>
-      <c r="D18" s="3">
-        <f t="shared" si="6"/>
-        <v>2.3012899607403248</v>
-      </c>
-      <c r="E18" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="F18" s="3" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3">
-        <f t="shared" ref="B19:F19" si="7" xml:space="preserve"> B9 / MIN($B9:$F9)</f>
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D19" s="3" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E19" s="3" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F19" s="3" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7304,6 +8583,366 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4DC42C-376D-41DF-9AD8-63D3F4858048}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>18051.118792068399</v>
+      </c>
+      <c r="C2">
+        <v>62.3183139534883</v>
+      </c>
+      <c r="D2">
+        <v>3829.9055030572499</v>
+      </c>
+      <c r="E2">
+        <v>420.65868263472998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>18327.502254283099</v>
+      </c>
+      <c r="C3">
+        <v>40.148698884758304</v>
+      </c>
+      <c r="D3">
+        <v>1810.3986772000701</v>
+      </c>
+      <c r="E3">
+        <v>72.573044297832197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>4140.6049495875304</v>
+      </c>
+      <c r="C4">
+        <v>16.642282370153598</v>
+      </c>
+      <c r="D4">
+        <v>1223.29020332717</v>
+      </c>
+      <c r="E4">
+        <v>35.309422040512899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>4275.8747697974204</v>
+      </c>
+      <c r="C5">
+        <v>17.143899325186901</v>
+      </c>
+      <c r="D5">
+        <v>932.94840752467803</v>
+      </c>
+      <c r="E5">
+        <v>53.809171597633103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1098.9465763732101</v>
+      </c>
+      <c r="C6">
+        <v>3.5414725069897401</v>
+      </c>
+      <c r="D6">
+        <v>180.78265662318501</v>
+      </c>
+      <c r="E6">
+        <v>9.1463414634146307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>1848.2370047255499</v>
+      </c>
+      <c r="C7">
+        <v>7.1128944008754296</v>
+      </c>
+      <c r="D7">
+        <v>87.5679729983123</v>
+      </c>
+      <c r="E7">
+        <v>2.8382213812677302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>1620.61014544164</v>
+      </c>
+      <c r="C8">
+        <v>8.9335566722501394</v>
+      </c>
+      <c r="D8">
+        <v>117.754616931797</v>
+      </c>
+      <c r="E8">
+        <v>3.7481259370314799</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>165.993325136132</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3">
+        <f xml:space="preserve"> B2/MIN($B2:$E2)</f>
+        <v>289.65993536893467</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ref="C12:E12" si="0" xml:space="preserve"> C2/MIN($B2:$E2)</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>61.457142533023699</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>6.7501614846109517</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" ref="B13:E13" si="1" xml:space="preserve"> B3/MIN($B3:$E3)</f>
+        <v>456.49056540760751</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="1"/>
+        <v>45.092337422853667</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>1.8076063811219343</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" ref="B14:E14" si="2" xml:space="preserve"> B4/MIN($B4:$E4)</f>
+        <v>248.80030620158954</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="2"/>
+        <v>73.504954195527205</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="2"/>
+        <v>2.1216694474453273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" ref="B15:E15" si="3" xml:space="preserve"> B5/MIN($B5:$E5)</f>
+        <v>249.41086556169481</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="3"/>
+        <v>54.418682111253425</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="3"/>
+        <v>3.1386775305300318</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" ref="B16:E16" si="4" xml:space="preserve"> B6/MIN($B6:$E6)</f>
+        <v>310.30780959169925</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="4"/>
+        <v>51.047313304388936</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="4"/>
+        <v>2.5826379974326108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" ref="B17:E17" si="5" xml:space="preserve"> B7/MIN($B7:$E7)</f>
+        <v>651.19550466497071</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="5"/>
+        <v>2.5061097939084509</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="5"/>
+        <v>30.853115819738797</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" ref="B18:E18" si="6" xml:space="preserve"> B8/MIN($B8:$E8)</f>
+        <v>432.37878680383005</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="6"/>
+        <v>2.3834729201563398</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="6"/>
+        <v>31.416931797403478</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" ref="B19:E19" si="7" xml:space="preserve"> B9/MIN($B9:$E9)</f>
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EFA07C-E270-4B85-8B26-6FA6BD53AA2B}">
   <dimension ref="A1:E23"/>
   <sheetViews>
@@ -7626,7 +9265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B9C7172-2F08-433B-92F6-25D08187801E}">
   <dimension ref="A1:E19"/>
   <sheetViews>
@@ -7933,7 +9572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492AED1C-BF35-4801-93A4-FC7E4F2107AC}">
   <dimension ref="A1:D5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Complement #245 - i5-1135g4, SP8
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF6F7A5-3ECE-4377-94CE-326833152AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243399A9-156F-4A09-954C-E952389B5796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
   <sheets>
     <sheet name="is" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="29">
   <si>
     <t>Components</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>Measured by AMD 5800H</t>
+  </si>
+  <si>
+    <t>Measure by i5-1135g4, Surface Pro 8</t>
   </si>
 </sst>
 </file>
@@ -1814,25 +1817,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>289.65993536893467</c:v>
+                  <c:v>303.08114729860966</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>456.49056540760751</c:v>
+                  <c:v>712.32011527483655</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>248.80030620158954</c:v>
+                  <c:v>255.95040305610445</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>249.41086556169481</c:v>
+                  <c:v>229.10224009840329</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>310.30780959169925</c:v>
+                  <c:v>371.79014667167951</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>651.19550466497071</c:v>
+                  <c:v>704.79510000607956</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>432.37878680383005</c:v>
+                  <c:v>482.49087828405766</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -1924,10 +1927,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5061097939084509</c:v>
+                  <c:v>2.6875429553264638</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3834729201563398</c:v>
+                  <c:v>2.5763880748642238</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2004,25 +2007,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>61.457142533023699</c:v>
+                  <c:v>55.811156701380639</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45.092337422853667</c:v>
+                  <c:v>37.183943513548755</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>73.504954195527205</c:v>
+                  <c:v>65.826350414170548</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54.418682111253425</c:v>
+                  <c:v>43.225806697834315</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51.047313304388936</c:v>
+                  <c:v>42.073821796760022</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30.853115819738797</c:v>
+                  <c:v>26.718033186920472</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31.416931797403478</c:v>
+                  <c:v>26.109395781873477</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2099,19 +2102,19 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.7501614846109517</c:v>
+                  <c:v>6.30901294482707</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8076063811219343</c:v>
+                  <c:v>1.8024126823722624</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1216694474453273</c:v>
+                  <c:v>1.9993494930111142</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.1386775305300318</c:v>
+                  <c:v>2.9782353728324003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5826379974326108</c:v>
+                  <c:v>2.4709203036053169</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -7791,18 +7794,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AA11DE-36E1-4DB2-967D-EB7E691732BC}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7822,7 +7823,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -7842,7 +7843,7 @@
         <v>86310.665451230598</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -7862,7 +7863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -7882,7 +7883,7 @@
         <v>1197.5418596366201</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -7902,7 +7903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -7922,7 +7923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -7942,7 +7943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -7962,7 +7963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -7982,7 +7983,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -8002,7 +8003,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -8028,7 +8029,7 @@
       </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -8054,7 +8055,7 @@
       </c>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -8080,7 +8081,7 @@
       </c>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -8106,7 +8107,7 @@
       </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -8132,7 +8133,7 @@
       </c>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -8158,7 +8159,7 @@
       </c>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -8184,7 +8185,7 @@
       </c>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -8210,7 +8211,7 @@
       </c>
       <c r="G19" s="3"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
         <v>27</v>
       </c>
@@ -8226,18 +8227,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050C2C99-5EE7-403C-9AB2-DBCB91E8248D}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8254,7 +8255,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -8271,7 +8272,7 @@
         <v>410.64293498002098</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -8288,7 +8289,7 @@
         <v>71.549933924863097</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -8305,7 +8306,7 @@
         <v>33.6478547267224</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -8322,7 +8323,7 @@
         <v>53.044452745610698</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -8339,7 +8340,7 @@
         <v>9.1237407337008101</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -8356,7 +8357,7 @@
         <v>2.9363185905670699</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -8373,7 +8374,7 @@
         <v>3.7900322152738299</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -8390,7 +8391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -8407,7 +8408,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -8428,7 +8429,7 @@
         <v>6.7197221105754403</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -8449,7 +8450,7 @@
         <v>1.8065534008033433</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -8470,7 +8471,7 @@
         <v>2.0498726778459528</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -8491,7 +8492,7 @@
         <v>3.0663115909720839</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -8512,7 +8513,7 @@
         <v>2.4091237407337003</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -8533,7 +8534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -8554,7 +8555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -8584,20 +8585,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4DC42C-376D-41DF-9AD8-63D3F4858048}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:E9"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8614,131 +8615,131 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>18051.118792068399</v>
+        <v>19591.433278418401</v>
       </c>
       <c r="C2">
-        <v>62.3183139534883</v>
+        <v>64.640883977900501</v>
       </c>
       <c r="D2">
-        <v>3829.9055030572499</v>
+        <v>3607.6825050063699</v>
       </c>
       <c r="E2">
-        <v>420.65868263472998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>407.82017378163903</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>18327.502254283099</v>
+        <v>29092.927785034499</v>
       </c>
       <c r="C3">
-        <v>40.148698884758304</v>
+        <v>40.842490842490797</v>
       </c>
       <c r="D3">
-        <v>1810.3986772000701</v>
+        <v>1518.6848724398101</v>
       </c>
       <c r="E3">
-        <v>72.573044297832197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73.6150234741784</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4">
-        <v>4140.6049495875304</v>
+        <v>4357.4087862993301</v>
       </c>
       <c r="C4">
-        <v>16.642282370153598</v>
+        <v>17.024426350851201</v>
       </c>
       <c r="D4">
-        <v>1223.29020332717</v>
+        <v>1120.6558545713699</v>
       </c>
       <c r="E4">
-        <v>35.309422040512899</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>34.037778193379403</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5">
-        <v>4275.8747697974204</v>
+        <v>3955.8432346160598</v>
       </c>
       <c r="C5">
-        <v>17.143899325186901</v>
+        <v>17.266715650257101</v>
       </c>
       <c r="D5">
-        <v>932.94840752467803</v>
+        <v>746.36771300448402</v>
       </c>
       <c r="E5">
-        <v>53.809171597633103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>51.424343322234499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1098.9465763732101</v>
+        <v>1399.0221887927701</v>
       </c>
       <c r="C6">
-        <v>3.5414725069897401</v>
+        <v>3.7629350893696998</v>
       </c>
       <c r="D6">
-        <v>180.78265662318501</v>
+        <v>158.32106038291599</v>
       </c>
       <c r="E6">
-        <v>9.1463414634146307</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9.2979127134724795</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
       <c r="B7">
-        <v>1848.2370047255499</v>
+        <v>1979.3908444282299</v>
       </c>
       <c r="C7">
-        <v>7.1128944008754296</v>
+        <v>7.5478645066273904</v>
       </c>
       <c r="D7">
-        <v>87.5679729983123</v>
+        <v>75.036603221083396</v>
       </c>
       <c r="E7">
-        <v>2.8382213812677302</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.8084628346751499</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="B8">
-        <v>1620.61014544164</v>
+        <v>1737.88183647338</v>
       </c>
       <c r="C8">
-        <v>8.9335566722501394</v>
+        <v>9.2798812175204102</v>
       </c>
       <c r="D8">
-        <v>117.754616931797</v>
+        <v>94.043321299638905</v>
       </c>
       <c r="E8">
-        <v>3.7481259370314799</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.6018957345971501</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9">
-        <v>165.993325136132</v>
+        <v>249.23409623355499</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -8750,7 +8751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -8767,13 +8768,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="3">
         <f xml:space="preserve"> B2/MIN($B2:$E2)</f>
-        <v>289.65993536893467</v>
+        <v>303.08114729860966</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:E12" si="0" xml:space="preserve"> C2/MIN($B2:$E2)</f>
@@ -8781,20 +8782,20 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>61.457142533023699</v>
+        <v>55.811156701380639</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>6.7501614846109517</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6.30901294482707</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="3">
         <f t="shared" ref="B13:E13" si="1" xml:space="preserve"> B3/MIN($B3:$E3)</f>
-        <v>456.49056540760751</v>
+        <v>712.32011527483655</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="1"/>
@@ -8802,20 +8803,20 @@
       </c>
       <c r="D13" s="3">
         <f t="shared" si="1"/>
-        <v>45.092337422853667</v>
+        <v>37.183943513548755</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="1"/>
-        <v>1.8076063811219343</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.8024126823722624</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="3">
         <f t="shared" ref="B14:E14" si="2" xml:space="preserve"> B4/MIN($B4:$E4)</f>
-        <v>248.80030620158954</v>
+        <v>255.95040305610445</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="2"/>
@@ -8823,20 +8824,20 @@
       </c>
       <c r="D14" s="3">
         <f t="shared" si="2"/>
-        <v>73.504954195527205</v>
+        <v>65.826350414170548</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="2"/>
-        <v>2.1216694474453273</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.9993494930111142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="3">
         <f t="shared" ref="B15:E15" si="3" xml:space="preserve"> B5/MIN($B5:$E5)</f>
-        <v>249.41086556169481</v>
+        <v>229.10224009840329</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="3"/>
@@ -8844,20 +8845,20 @@
       </c>
       <c r="D15" s="3">
         <f t="shared" si="3"/>
-        <v>54.418682111253425</v>
+        <v>43.225806697834315</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" si="3"/>
-        <v>3.1386775305300318</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.9782353728324003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="3">
         <f t="shared" ref="B16:E16" si="4" xml:space="preserve"> B6/MIN($B6:$E6)</f>
-        <v>310.30780959169925</v>
+        <v>371.79014667167951</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="4"/>
@@ -8865,56 +8866,56 @@
       </c>
       <c r="D16" s="3">
         <f t="shared" si="4"/>
-        <v>51.047313304388936</v>
+        <v>42.073821796760022</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="4"/>
-        <v>2.5826379974326108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.4709203036053169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="3">
         <f t="shared" ref="B17:E17" si="5" xml:space="preserve"> B7/MIN($B7:$E7)</f>
-        <v>651.19550466497071</v>
+        <v>704.79510000607956</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="5"/>
-        <v>2.5061097939084509</v>
+        <v>2.6875429553264638</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="5"/>
-        <v>30.853115819738797</v>
+        <v>26.718033186920472</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="3">
         <f t="shared" ref="B18:E18" si="6" xml:space="preserve"> B8/MIN($B8:$E8)</f>
-        <v>432.37878680383005</v>
+        <v>482.49087828405766</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="6"/>
-        <v>2.3834729201563398</v>
+        <v>2.5763880748642238</v>
       </c>
       <c r="D18" s="3">
         <f t="shared" si="6"/>
-        <v>31.416931797403478</v>
+        <v>26.109395781873477</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -8933,6 +8934,11 @@
       <c r="E19" s="3" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -8950,16 +8956,16 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8976,7 +8982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -8990,7 +8996,7 @@
         <v>4226.6036707250496</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9004,7 +9010,7 @@
         <v>1225.8186636380799</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -9018,7 +9024,7 @@
         <v>924.14831545266304</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -9032,7 +9038,7 @@
         <v>500.093510379652</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -9046,7 +9052,7 @@
         <v>97.656982193064593</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -9060,7 +9066,7 @@
         <v>70.606003398149895</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -9074,7 +9080,7 @@
         <v>151.226656902233</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -9088,10 +9094,10 @@
         <v>137.174721189591</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -9106,7 +9112,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -9124,7 +9130,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -9142,7 +9148,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -9160,7 +9166,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -9178,7 +9184,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -9196,7 +9202,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -9214,7 +9220,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -9231,7 +9237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -9248,12 +9254,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -9273,16 +9279,16 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9296,7 +9302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -9310,7 +9316,7 @@
         <v>4262.1504972790399</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9324,7 +9330,7 @@
         <v>1191.4353111957901</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -9338,7 +9344,7 @@
         <v>980.59339428997896</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -9352,7 +9358,7 @@
         <v>520.87250846182701</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -9366,7 +9372,7 @@
         <v>30.766396462785501</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -9380,7 +9386,7 @@
         <v>78.568723968193794</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -9394,7 +9400,7 @@
         <v>181.146025878003</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -9408,7 +9414,7 @@
         <v>145.03957297993699</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -9422,7 +9428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -9440,7 +9446,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -9458,7 +9464,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -9476,7 +9482,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -9494,7 +9500,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -9512,7 +9518,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -9530,7 +9536,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -9548,7 +9554,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -9580,14 +9586,14 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -9601,7 +9607,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -9615,7 +9621,7 @@
         <v>4226.6036707250496</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -9629,7 +9635,7 @@
         <v>5621.0191082802503</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -9643,7 +9649,7 @@
         <v>5722.3155929038203</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Complement #245 - measured by AMD-5900HX
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243399A9-156F-4A09-954C-E952389B5796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53C7925-EA56-4188-8697-803A3BCA28CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
   <sheets>
     <sheet name="is" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="30">
   <si>
     <t>Components</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Measure by i5-1135g4, Surface Pro 8</t>
+  </si>
+  <si>
+    <t>Measured by AMD-5900HX</t>
   </si>
 </sst>
 </file>
@@ -1134,25 +1137,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>371.89452250275474</c:v>
+                  <c:v>375.11770154231999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>818.68043464864797</c:v>
+                  <c:v>780.42680202708357</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>301.24775200180926</c:v>
+                  <c:v>293.83702948784764</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>269.65532622974769</c:v>
+                  <c:v>271.9452044519382</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>451.12895232711332</c:v>
+                  <c:v>434.5201546107121</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>726.62424918092529</c:v>
+                  <c:v>779.3709885651034</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>511.63374411018282</c:v>
+                  <c:v>485.05739654610693</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -1244,10 +1247,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.3611339171684032</c:v>
+                  <c:v>2.7272111913357451</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3712413405729253</c:v>
+                  <c:v>2.4309745840190122</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1324,25 +1327,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>63.943991040328974</c:v>
+                  <c:v>59.141782963045557</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.621749795068474</c:v>
+                  <c:v>44.849748747493095</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.746037069867171</c:v>
+                  <c:v>72.624244222184501</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51.875396603349138</c:v>
+                  <c:v>47.919221503871036</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47.028513071895269</c:v>
+                  <c:v>46.509989648033134</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30.178002563163748</c:v>
+                  <c:v>30.617362757614483</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.841526845637556</c:v>
+                  <c:v>31.298270013568445</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1419,19 +1422,19 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.7197221105754403</c:v>
+                  <c:v>6.5085911252672384</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8065534008033433</c:v>
+                  <c:v>1.677367516755442</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0498726778459528</c:v>
+                  <c:v>2.0273769885312669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0663115909720839</c:v>
+                  <c:v>2.8370154366490432</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4091237407337003</c:v>
+                  <c:v>2.5025479494211664</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -7794,7 +7797,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AA11DE-36E1-4DB2-967D-EB7E691732BC}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8225,10 +8230,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050C2C99-5EE7-403C-9AB2-DBCB91E8248D}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8260,16 +8265,16 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>22726.5139406854</v>
+        <v>26022.039061100098</v>
       </c>
       <c r="C2">
-        <v>61.110106671487898</v>
+        <v>69.370330843116307</v>
       </c>
       <c r="D2">
-        <v>3907.6241134751699</v>
+        <v>4102.6850507982499</v>
       </c>
       <c r="E2">
-        <v>410.64293498002098</v>
+        <v>451.503119682359</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -8277,16 +8282,16 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>32424.4669316949</v>
+        <v>35776.804027596401</v>
       </c>
       <c r="C3">
-        <v>39.605767475816698</v>
+        <v>45.842613214550802</v>
       </c>
       <c r="D3">
-        <v>1688.06711179592</v>
+        <v>2056.0296846011101</v>
       </c>
       <c r="E3">
-        <v>71.549933924863097</v>
+        <v>76.894910289271294</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -8294,16 +8299,16 @@
         <v>19</v>
       </c>
       <c r="B4">
-        <v>4944.8635057471201</v>
+        <v>5469.2293809781604</v>
       </c>
       <c r="C4">
-        <v>16.4146071560309</v>
+        <v>18.6131386861313</v>
       </c>
       <c r="D4">
-        <v>1177.6830135038999</v>
+        <v>1351.7651296829899</v>
       </c>
       <c r="E4">
-        <v>33.6478547267224</v>
+        <v>37.735849056603698</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -8311,16 +8316,16 @@
         <v>20</v>
       </c>
       <c r="B5">
-        <v>4664.7963800904899</v>
+        <v>5295.3194650817204</v>
       </c>
       <c r="C5">
-        <v>17.2991071428571</v>
+        <v>19.472008987081001</v>
       </c>
       <c r="D5">
-        <v>897.39804391954203</v>
+        <v>933.08351177730196</v>
       </c>
       <c r="E5">
-        <v>53.044452745610698</v>
+        <v>55.242390078917701</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -8328,16 +8333,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1708.49820991143</v>
+        <v>1716.1789066813899</v>
       </c>
       <c r="C6">
-        <v>3.7871615224389301</v>
+        <v>3.9495956366371998</v>
       </c>
       <c r="D6">
-        <v>178.10457516339801</v>
+        <v>183.695652173913</v>
       </c>
       <c r="E6">
-        <v>9.1237407337008101</v>
+        <v>9.88405246150921</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -8345,16 +8350,16 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>2133.60029122679</v>
+        <v>2321.2836591663499</v>
       </c>
       <c r="C7">
-        <v>6.9330414158000302</v>
+        <v>8.1227436823104693</v>
       </c>
       <c r="D7">
-        <v>88.612229952398394</v>
+        <v>91.190953857377295</v>
       </c>
       <c r="E7">
-        <v>2.9363185905670699</v>
+        <v>2.9784065524944099</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -8362,16 +8367,16 @@
         <v>22</v>
       </c>
       <c r="B8">
-        <v>1939.1083725987601</v>
+        <v>2006.6308243727599</v>
       </c>
       <c r="C8">
-        <v>8.9870810709604907</v>
+        <v>10.0566831230572</v>
       </c>
       <c r="D8">
-        <v>116.890380313199</v>
+        <v>129.477611940298</v>
       </c>
       <c r="E8">
-        <v>3.7900322152738299</v>
+        <v>4.1368935690109003</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -8379,7 +8384,7 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>276.25201938610599</v>
+        <v>293.92326051037202</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -8414,7 +8419,7 @@
       </c>
       <c r="B12" s="3">
         <f xml:space="preserve"> B2/MIN($B2:$E2)</f>
-        <v>371.89452250275474</v>
+        <v>375.11770154231999</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:E12" si="0" xml:space="preserve"> C2/MIN($B2:$E2)</f>
@@ -8422,11 +8427,11 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>63.943991040328974</v>
+        <v>59.141782963045557</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>6.7197221105754403</v>
+        <v>6.5085911252672384</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -8435,7 +8440,7 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" ref="B13:E19" si="1" xml:space="preserve"> B3/MIN($B3:$E3)</f>
-        <v>818.68043464864797</v>
+        <v>780.42680202708357</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="1"/>
@@ -8443,11 +8448,11 @@
       </c>
       <c r="D13" s="3">
         <f t="shared" si="1"/>
-        <v>42.621749795068474</v>
+        <v>44.849748747493095</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="1"/>
-        <v>1.8065534008033433</v>
+        <v>1.677367516755442</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -8456,7 +8461,7 @@
       </c>
       <c r="B14" s="3">
         <f t="shared" si="1"/>
-        <v>301.24775200180926</v>
+        <v>293.83702948784764</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="1"/>
@@ -8464,11 +8469,11 @@
       </c>
       <c r="D14" s="3">
         <f t="shared" si="1"/>
-        <v>71.746037069867171</v>
+        <v>72.624244222184501</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="1"/>
-        <v>2.0498726778459528</v>
+        <v>2.0273769885312669</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -8477,7 +8482,7 @@
       </c>
       <c r="B15" s="3">
         <f t="shared" si="1"/>
-        <v>269.65532622974769</v>
+        <v>271.9452044519382</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="1"/>
@@ -8485,11 +8490,11 @@
       </c>
       <c r="D15" s="3">
         <f t="shared" si="1"/>
-        <v>51.875396603349138</v>
+        <v>47.919221503871036</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" si="1"/>
-        <v>3.0663115909720839</v>
+        <v>2.8370154366490432</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -8498,7 +8503,7 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" si="1"/>
-        <v>451.12895232711332</v>
+        <v>434.5201546107121</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="1"/>
@@ -8506,56 +8511,56 @@
       </c>
       <c r="D16" s="3">
         <f t="shared" si="1"/>
-        <v>47.028513071895269</v>
+        <v>46.509989648033134</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="1"/>
-        <v>2.4091237407337003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.5025479494211664</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="3">
         <f t="shared" si="1"/>
-        <v>726.62424918092529</v>
+        <v>779.3709885651034</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="1"/>
-        <v>2.3611339171684032</v>
+        <v>2.7272111913357451</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="1"/>
-        <v>30.178002563163748</v>
+        <v>30.617362757614483</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="3">
         <f t="shared" si="1"/>
-        <v>511.63374411018282</v>
+        <v>485.05739654610693</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="1"/>
-        <v>2.3712413405729253</v>
+        <v>2.4309745840190122</v>
       </c>
       <c r="D18" s="3">
         <f t="shared" si="1"/>
-        <v>30.841526845637556</v>
+        <v>31.298270013568445</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -8574,6 +8579,11 @@
       <c r="E19" s="3" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -8587,9 +8597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4DC42C-376D-41DF-9AD8-63D3F4858048}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Close #254 - finalize with README
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8B9CF5-739F-42AE-837E-D59AB0EF58D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AF7CB9-C7CD-46FB-B95A-634BD7291412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
   <sheets>
     <sheet name="is" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="25">
   <si>
     <t>Components</t>
   </si>
@@ -105,16 +105,13 @@
     <t>class-validator</t>
   </si>
   <si>
-    <t>Measured by AMD 5800H</t>
+    <t>typebox</t>
   </si>
   <si>
-    <t>Measure by i5-1135g4, Surface Pro 8</t>
+    <t>Measured by AMD 5900HX</t>
   </si>
   <si>
-    <t>Measured by AMD-5900HX</t>
-  </si>
-  <si>
-    <t>typebox</t>
+    <t>Measured by Intel i5-1135g7</t>
   </si>
 </sst>
 </file>
@@ -344,28 +341,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1759.4463981229926</c:v>
+                  <c:v>1803.0919840708693</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1673.4910211592974</c:v>
+                  <c:v>2025.7246537461999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>934.56382596188257</c:v>
+                  <c:v>910.20537949563209</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>876.65118631598284</c:v>
+                  <c:v>791.60208240391262</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1867.5285171102651</c:v>
+                  <c:v>2074.7290909090952</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1330.7186555434664</c:v>
+                  <c:v>1310.4138697387521</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1027.9840809227373</c:v>
+                  <c:v>1010.3963547216247</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1548.6149035025053</c:v>
+                  <c:v>1743.3686144799733</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -439,28 +436,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2876.4254057142866</c:v>
+                  <c:v>3001.7933623315657</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2087.7839360487246</c:v>
+                  <c:v>2075.1773920680448</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>742.34457671957523</c:v>
+                  <c:v>770.62503023706108</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1874.234234234234</c:v>
+                  <c:v>1873.7547593582919</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>705.3995121035864</c:v>
+                  <c:v>644.85425531914871</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>555.19244663382449</c:v>
+                  <c:v>598.59340121059392</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>708.94180327868855</c:v>
+                  <c:v>893.12259259259224</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -534,16 +531,16 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1271.6028603263023</c:v>
+                  <c:v>1438.6576720819507</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.661674747846803</c:v>
+                  <c:v>76.050121665742722</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>251.79788732394317</c:v>
+                  <c:v>271.78743894625092</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -629,25 +626,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>145.90900887812759</c:v>
+                  <c:v>140.23872405824903</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110.24623375246759</c:v>
+                  <c:v>119.71308445353615</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>205.75697681645855</c:v>
+                  <c:v>188.4956631225522</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>133.25646271154903</c:v>
+                  <c:v>134.55581787521101</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.58826106000895</c:v>
+                  <c:v>123.97234654731463</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>111.63681610247018</c:v>
+                  <c:v>113.09405451584497</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -739,10 +736,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6506568897036433</c:v>
+                  <c:v>2.5114960282436067</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.485419440745674</c:v>
+                  <c:v>2.4691168558551451</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -819,19 +816,19 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.5034103589851542</c:v>
+                  <c:v>6.5753427852785933</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7784082634655789</c:v>
+                  <c:v>1.8048711175410641</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0436559272264332</c:v>
+                  <c:v>1.9943498968571842</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1417341366974183</c:v>
+                  <c:v>1.1165114264052871</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4774193548387089</c:v>
+                  <c:v>2.4793853073463317</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -1109,7 +1106,7 @@
                   <a:srgbClr val="7030A0"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>assert()</a:t>
+              <a:t>assertType()</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
@@ -1218,28 +1215,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>334.72656813266065</c:v>
+                  <c:v>335.85878022317149</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>647.80586160497216</c:v>
+                  <c:v>829.41938026445678</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>268.81465616659557</c:v>
+                  <c:v>291.7929140019981</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>286.77111074424812</c:v>
+                  <c:v>308.26775619945397</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>436.73251495121059</c:v>
+                  <c:v>428.22621458820959</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>784.9658720004154</c:v>
+                  <c:v>717.99775981628204</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>469.21954448644283</c:v>
+                  <c:v>504.57942313721281</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>644.54239150338776</c:v>
+                  <c:v>731.98752692031496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1313,28 +1310,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>13.797393364928913</c:v>
+                  <c:v>14.899528598490065</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6952129792418482</c:v>
+                  <c:v>10.163352438742226</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.4505659134872477</c:v>
+                  <c:v>9.7475200434841955</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0956002058186103</c:v>
+                  <c:v>4.4475642089934864</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.075572801182574</c:v>
+                  <c:v>10.498630425621558</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.4208083086364711</c:v>
+                  <c:v>7.2477949158675576</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0285638719915378</c:v>
+                  <c:v>7.3977823231779576</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.56389600878798</c:v>
+                  <c:v>13.343675417661101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1408,25 +1405,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>59.019003568124695</c:v>
+                  <c:v>62.206683941911493</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.045230675262601</c:v>
+                  <c:v>46.084315370439519</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65.729340541617759</c:v>
+                  <c:v>72.872513878932168</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.685174042540435</c:v>
+                  <c:v>19.445610151644448</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47.884973486249905</c:v>
+                  <c:v>45.726785063277759</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29.215637272402709</c:v>
+                  <c:v>29.410187143645469</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.49302169160914</c:v>
+                  <c:v>30.387296913612573</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1503,19 +1500,19 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.5024519049415286</c:v>
+                  <c:v>6.4279932380915366</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9996722628663275</c:v>
+                  <c:v>1.8049943543115226</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0407196515582138</c:v>
+                  <c:v>1.9751351170456697</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1287874473798363</c:v>
+                  <c:v>1.0751343067002523</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6001478196600178</c:v>
+                  <c:v>2.433234737655555</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -1613,10 +1610,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0121828486678308</c:v>
+                  <c:v>2.7048617708531326</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5965344313616026</c:v>
+                  <c:v>2.4714444503255182</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1996,28 +1993,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>41.464226187587265</c:v>
+                  <c:v>288.51028100126848</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>210.7538181818168</c:v>
+                  <c:v>469.54843461852619</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110.37145283492914</c:v>
+                  <c:v>248.54188336699238</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>164.23292145388771</c:v>
+                  <c:v>236.19522243086899</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>114.51504902072725</c:v>
+                  <c:v>341.8003886903623</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>554.82917714696475</c:v>
+                  <c:v>547.95564980510312</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>428.08255509899141</c:v>
+                  <c:v>390.83244743680405</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>332.895194986072</c:v>
+                  <c:v>400.43040780141746</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2037,7 +2034,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>class-validator</c:v>
+                  <c:v>typebox</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2091,28 +2088,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.8482689435676538</c:v>
+                  <c:v>13.613431186071697</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5611383600608848</c:v>
+                  <c:v>9.7333637274802669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2524009462043262</c:v>
+                  <c:v>10.163036039409622</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4225825471698279</c:v>
+                  <c:v>4.746021470947869</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.7683933139702659</c:v>
+                  <c:v>11.764202926087764</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0211081794195289</c:v>
+                  <c:v>6.9350664767331454</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0273485600794467</c:v>
+                  <c:v>6.4506618531889135</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.755646817248483</c:v>
+                  <c:v>13.288651004168278</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2186,25 +2183,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>8.1901063066831981</c:v>
+                  <c:v>61.666702623078194</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.014319238561544</c:v>
+                  <c:v>44.311688809046203</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.520472860162847</c:v>
+                  <c:v>73.238313136369683</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.383819218955724</c:v>
+                  <c:v>21.554535939768407</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.93191364619927</c:v>
+                  <c:v>53.945853043203897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.327915194346364</c:v>
+                  <c:v>28.921411358911392</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27.12707435318012</c:v>
+                  <c:v>28.023620149433629</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2281,19 +2278,19 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>6.9973507869720999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.8443031662926925</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2.1920228660517136</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.1939098074372894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2.6199974790445575</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -2310,6 +2307,101 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-83BA-4704-941C-FD22C3C356F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>validate!$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>class-validator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>validate!$A$12:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (union, explicit)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union, implicit)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ultimate union</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>validate!$F$12:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>##,##0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2402980877390335</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1478045763760063</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4BEE-4FFD-A5D1-DE729CB17E86}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6453,15 +6545,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>2069</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>185529</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6872,7 +6964,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6890,7 +6982,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
         <v>14</v>
@@ -6910,22 +7002,22 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>110300.239896659</v>
+        <v>117845.05232237899</v>
       </c>
       <c r="C2" s="2">
-        <v>180324</v>
+        <v>196188.82395909401</v>
       </c>
       <c r="D2">
-        <v>79717.177344475305</v>
+        <v>94026.644307806899</v>
       </c>
       <c r="E2">
-        <v>9147.0809792843702</v>
+        <v>9165.6110283159396</v>
       </c>
       <c r="F2">
-        <v>62.690309869245901</v>
+        <v>65.357204936554794</v>
       </c>
       <c r="G2">
-        <v>407.70081061164302</v>
+        <v>429.74602594555</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -6933,22 +7025,22 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>67586.952504158195</v>
+        <v>84088.051470588194</v>
       </c>
       <c r="C3" s="2">
-        <v>84318.918918918906</v>
+        <v>86140.840035746194</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
       <c r="E3">
-        <v>4452.4929444967001</v>
+        <v>4969.3032015065901</v>
       </c>
       <c r="F3">
-        <v>40.386803185437998</v>
+        <v>41.510109142959301</v>
       </c>
       <c r="G3">
-        <v>71.824224519940898</v>
+        <v>74.9203970781045</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -6956,22 +7048,22 @@
         <v>15</v>
       </c>
       <c r="B4" s="2">
-        <v>15127.831715210301</v>
+        <v>16115.7721194357</v>
       </c>
       <c r="C4" s="2">
-        <v>12016.369047619</v>
+        <v>13644.412191582</v>
       </c>
       <c r="D4">
-        <v>1143.804087645</v>
+        <v>1346.5163555719801</v>
       </c>
       <c r="E4">
-        <v>3330.59854559015</v>
+        <v>3337.43704532736</v>
       </c>
       <c r="F4">
-        <v>16.187050359712199</v>
+        <v>17.705643673920999</v>
       </c>
       <c r="G4">
-        <v>33.080761411938603</v>
+        <v>35.311248634874403</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -6979,22 +7071,22 @@
         <v>16</v>
       </c>
       <c r="B5" s="2">
-        <v>14312.672429648699</v>
+        <v>14110.0407558354</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D5">
-        <v>4110.98591549295</v>
+        <v>4844.5196465501003</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
       <c r="F5">
-        <v>16.326530612244898</v>
+        <v>17.824663514005</v>
       </c>
       <c r="G5">
-        <v>18.6405573338354</v>
+        <v>19.901440485216</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -7002,22 +7094,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>6669.7447039652297</v>
+        <v>7841.0018552875699</v>
       </c>
       <c r="C6" s="2">
-        <v>6693.69369369369</v>
+        <v>7081.4616755793204</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
       <c r="E6">
-        <v>475.91593825553201</v>
+        <v>508.52538879520301</v>
       </c>
       <c r="F6">
-        <v>3.5714285714285698</v>
+        <v>3.7792894935752002</v>
       </c>
       <c r="G6">
-        <v>8.8479262672810997</v>
+        <v>9.3703148425787095</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -7025,22 +7117,22 @@
         <v>17</v>
       </c>
       <c r="B7" s="2">
-        <v>3773.3043162858098</v>
+        <v>3960.4499274310501</v>
       </c>
       <c r="C7" s="2">
-        <v>2000.18765246763</v>
+        <v>1948.9361702127601</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
       <c r="E7">
-        <v>356.11038107752898</v>
+        <v>374.68030690537</v>
       </c>
       <c r="F7">
-        <v>7.5160403299725003</v>
+        <v>7.5904677846425397</v>
       </c>
       <c r="G7">
-        <v>2.8355387523629401</v>
+        <v>3.0222893842085301</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -7048,22 +7140,22 @@
         <v>18</v>
       </c>
       <c r="B8" s="2">
-        <v>3855.1812522885298</v>
+        <v>4017.1002364926298</v>
       </c>
       <c r="C8" s="2">
-        <v>2082.1018062397302</v>
+        <v>2379.8677443056499</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
       <c r="E8">
-        <v>418.66422689844399</v>
+        <v>449.63558213418003</v>
       </c>
       <c r="F8">
-        <v>9.3209054593874807</v>
+        <v>9.8166327097610608</v>
       </c>
       <c r="G8">
-        <v>3.75023438964935</v>
+        <v>3.9757667550170299</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -7071,10 +7163,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="2">
-        <v>547.891350964975</v>
+        <v>616.68504226387302</v>
       </c>
       <c r="C9" s="2">
-        <v>250.819672131147</v>
+        <v>315.92592592592501</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -7086,7 +7178,7 @@
         <v>4</v>
       </c>
       <c r="G9">
-        <v>0.35379444542720601</v>
+        <v>0.35373187124159799</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -7097,7 +7189,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
@@ -7118,19 +7210,19 @@
       </c>
       <c r="B12" s="3">
         <f xml:space="preserve"> B2 / MIN($B2:$G2)</f>
-        <v>1759.4463981229926</v>
+        <v>1803.0919840708693</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:G12" si="0" xml:space="preserve"> C2 / MIN($B2:$G2)</f>
-        <v>2876.4254057142866</v>
+        <v>3001.7933623315657</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>1271.6028603263023</v>
+        <v>1438.6576720819507</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>145.90900887812759</v>
+        <v>140.23872405824903</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
@@ -7138,7 +7230,7 @@
       </c>
       <c r="G12" s="3">
         <f t="shared" si="0"/>
-        <v>6.5034103589851542</v>
+        <v>6.5753427852785933</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -7147,11 +7239,11 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" ref="B13:G13" si="1" xml:space="preserve"> B3 / MIN($B3:$G3)</f>
-        <v>1673.4910211592974</v>
+        <v>2025.7246537461999</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="1"/>
-        <v>2087.7839360487246</v>
+        <v>2075.1773920680448</v>
       </c>
       <c r="D13" s="3" t="e">
         <f t="shared" si="1"/>
@@ -7159,7 +7251,7 @@
       </c>
       <c r="E13" s="3">
         <f t="shared" si="1"/>
-        <v>110.24623375246759</v>
+        <v>119.71308445353615</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="1"/>
@@ -7167,7 +7259,7 @@
       </c>
       <c r="G13" s="3">
         <f t="shared" si="1"/>
-        <v>1.7784082634655789</v>
+        <v>1.8048711175410641</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -7176,19 +7268,19 @@
       </c>
       <c r="B14" s="3">
         <f t="shared" ref="B14:G14" si="2" xml:space="preserve"> B4 / MIN($B4:$G4)</f>
-        <v>934.56382596188257</v>
+        <v>910.20537949563209</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="2"/>
-        <v>742.34457671957523</v>
+        <v>770.62503023706108</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="2"/>
-        <v>70.661674747846803</v>
+        <v>76.050121665742722</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="2"/>
-        <v>205.75697681645855</v>
+        <v>188.4956631225522</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="2"/>
@@ -7196,7 +7288,7 @@
       </c>
       <c r="G14" s="3">
         <f t="shared" si="2"/>
-        <v>2.0436559272264332</v>
+        <v>1.9943498968571842</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -7205,7 +7297,7 @@
       </c>
       <c r="B15" s="3">
         <f t="shared" ref="B15:G15" si="3" xml:space="preserve"> B5 / MIN($B5:$G5)</f>
-        <v>876.65118631598284</v>
+        <v>791.60208240391262</v>
       </c>
       <c r="C15" s="3" t="e">
         <f t="shared" si="3"/>
@@ -7213,7 +7305,7 @@
       </c>
       <c r="D15" s="3">
         <f t="shared" si="3"/>
-        <v>251.79788732394317</v>
+        <v>271.78743894625092</v>
       </c>
       <c r="E15" s="3" t="e">
         <f t="shared" si="3"/>
@@ -7225,7 +7317,7 @@
       </c>
       <c r="G15" s="3">
         <f t="shared" si="3"/>
-        <v>1.1417341366974183</v>
+        <v>1.1165114264052871</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -7234,11 +7326,11 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" ref="B16:G16" si="4" xml:space="preserve"> B6 / MIN($B6:$G6)</f>
-        <v>1867.5285171102651</v>
+        <v>2074.7290909090952</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="4"/>
-        <v>1874.234234234234</v>
+        <v>1873.7547593582919</v>
       </c>
       <c r="D16" s="3" t="e">
         <f t="shared" si="4"/>
@@ -7246,7 +7338,7 @@
       </c>
       <c r="E16" s="3">
         <f t="shared" si="4"/>
-        <v>133.25646271154903</v>
+        <v>134.55581787521101</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="4"/>
@@ -7254,7 +7346,7 @@
       </c>
       <c r="G16" s="3">
         <f t="shared" si="4"/>
-        <v>2.4774193548387089</v>
+        <v>2.4793853073463317</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -7263,11 +7355,11 @@
       </c>
       <c r="B17" s="3">
         <f t="shared" ref="B17:G17" si="5" xml:space="preserve"> B7 / MIN($B7:$G7)</f>
-        <v>1330.7186555434664</v>
+        <v>1310.4138697387521</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="5"/>
-        <v>705.3995121035864</v>
+        <v>644.85425531914871</v>
       </c>
       <c r="D17" s="3" t="e">
         <f t="shared" si="5"/>
@@ -7275,11 +7367,11 @@
       </c>
       <c r="E17" s="3">
         <f t="shared" si="5"/>
-        <v>125.58826106000895</v>
+        <v>123.97234654731463</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="5"/>
-        <v>2.6506568897036433</v>
+        <v>2.5114960282436067</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="5"/>
@@ -7292,11 +7384,11 @@
       </c>
       <c r="B18" s="3">
         <f t="shared" ref="B18:G18" si="6" xml:space="preserve"> B8 / MIN($B8:$G8)</f>
-        <v>1027.9840809227373</v>
+        <v>1010.3963547216247</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="6"/>
-        <v>555.19244663382449</v>
+        <v>598.59340121059392</v>
       </c>
       <c r="D18" s="3" t="e">
         <f t="shared" si="6"/>
@@ -7304,11 +7396,11 @@
       </c>
       <c r="E18" s="3">
         <f t="shared" si="6"/>
-        <v>111.63681610247018</v>
+        <v>113.09405451584497</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="6"/>
-        <v>2.485419440745674</v>
+        <v>2.4691168558551451</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="6"/>
@@ -7321,11 +7413,11 @@
       </c>
       <c r="B19" s="3">
         <f t="shared" ref="B19:G19" si="7" xml:space="preserve"> B9 / MIN($B9:$G9)</f>
-        <v>1548.6149035025053</v>
+        <v>1743.3686144799733</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="7"/>
-        <v>708.94180327868855</v>
+        <v>893.12259259259224</v>
       </c>
       <c r="D19" s="3" t="e">
         <f t="shared" si="7"/>
@@ -7346,7 +7438,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -7361,7 +7453,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7379,7 +7471,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
@@ -7396,19 +7488,19 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>21204.3979812545</v>
+        <v>22979.1521890201</v>
       </c>
       <c r="C2">
-        <v>874.04301859278098</v>
+        <v>1019.412191582</v>
       </c>
       <c r="D2">
-        <v>3738.7604070305201</v>
+        <v>4256.1247216035599</v>
       </c>
       <c r="E2">
-        <v>411.92003017729098</v>
+        <v>439.79744936233999</v>
       </c>
       <c r="F2">
-        <v>63.348416289592699</v>
+        <v>68.419090231170699</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7416,19 +7508,19 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>25530.470420527399</v>
+        <v>35552.973977695103</v>
       </c>
       <c r="C3">
-        <v>342.68426842684198</v>
+        <v>435.65102694554298</v>
       </c>
       <c r="D3">
-        <v>1617.6205091171601</v>
+        <v>1975.3993023682699</v>
       </c>
       <c r="E3">
-        <v>78.808446455505205</v>
+        <v>77.370892018779301</v>
       </c>
       <c r="F3">
-        <v>39.410681399631599</v>
+        <v>42.8648941942485</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -7436,19 +7528,19 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>4375.3665689149502</v>
+        <v>5302.4042742653601</v>
       </c>
       <c r="C4">
-        <v>137.54578754578699</v>
+        <v>177.13004484304901</v>
       </c>
       <c r="D4">
-        <v>1069.8447893569801</v>
+        <v>1324.22519713918</v>
       </c>
       <c r="E4">
-        <v>33.215809983299302</v>
+        <v>35.891772501380402</v>
       </c>
       <c r="F4">
-        <v>16.276517922457899</v>
+        <v>18.171806167400799</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -7456,19 +7548,19 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>4546.0489445170897</v>
+        <v>5325.8222787570403</v>
       </c>
       <c r="C5">
-        <v>64.925643815741694</v>
+        <v>76.838839204234304</v>
       </c>
       <c r="D5">
-        <v>280.35483274810503</v>
+        <v>335.95425303788397</v>
       </c>
       <c r="E5">
-        <v>17.8941420229798</v>
+        <v>18.574677786201601</v>
       </c>
       <c r="F5">
-        <v>15.8525345622119</v>
+        <v>17.276611554894998</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -7476,19 +7568,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1489.7072710103801</v>
+        <v>1707.0521082673499</v>
       </c>
       <c r="C6">
-        <v>34.368070953436799</v>
+        <v>41.851032448377502</v>
       </c>
       <c r="D6">
-        <v>163.33703292637799</v>
+        <v>182.28217280349901</v>
       </c>
       <c r="E6">
-        <v>8.8691796008869108</v>
+        <v>9.6996828949822795</v>
       </c>
       <c r="F6">
-        <v>3.4110289937464402</v>
+        <v>3.98633257403189</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -7496,19 +7588,19 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>1980.8078961798501</v>
+        <v>2168.7680115273702</v>
       </c>
       <c r="C7">
-        <v>18.725904167431601</v>
+        <v>21.892527591821899</v>
       </c>
       <c r="D7">
-        <v>73.723670117815004</v>
+        <v>88.835755011955101</v>
       </c>
       <c r="E7">
-        <v>2.5234318673395801</v>
+        <v>3.0205776854823401</v>
       </c>
       <c r="F7">
-        <v>7.6010381905821198</v>
+        <v>8.1702451073532192</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -7516,19 +7608,19 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>1677.3605541377999</v>
+        <v>2004.57205559619</v>
       </c>
       <c r="C8">
-        <v>25.125628140703501</v>
+        <v>29.389600602863599</v>
       </c>
       <c r="D8">
-        <v>105.431309904153</v>
+        <v>120.72138387927799</v>
       </c>
       <c r="E8">
-        <v>3.5747883349012199</v>
+        <v>3.9727582292849002</v>
       </c>
       <c r="F8">
-        <v>9.2820609964008298</v>
+        <v>9.8184512782511995</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -7536,16 +7628,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>224.501007141549</v>
+        <v>261.84493898061697</v>
       </c>
       <c r="C9">
-        <v>4.0278286341999197</v>
+        <v>4.7732696897374698</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
       </c>
       <c r="E9">
-        <v>0.348310693138279</v>
+        <v>0.35771776068681799</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
@@ -7559,7 +7651,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
@@ -7577,19 +7669,19 @@
       </c>
       <c r="B12" s="3">
         <f xml:space="preserve"> B2/MIN($B2:$F2)</f>
-        <v>334.72656813266065</v>
+        <v>335.85878022317149</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:F12" si="0" xml:space="preserve"> C2/MIN($B2:$F2)</f>
-        <v>13.797393364928913</v>
+        <v>14.899528598490065</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>59.019003568124695</v>
+        <v>62.206683941911493</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>6.5024519049415286</v>
+        <v>6.4279932380915366</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
@@ -7602,19 +7694,19 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" ref="B13:F13" si="1" xml:space="preserve"> B3/MIN($B3:$F3)</f>
-        <v>647.80586160497216</v>
+        <v>829.41938026445678</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="1"/>
-        <v>8.6952129792418482</v>
+        <v>10.163352438742226</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="1"/>
-        <v>41.045230675262601</v>
+        <v>46.084315370439519</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="1"/>
-        <v>1.9996722628663275</v>
+        <v>1.8049943543115226</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="1"/>
@@ -7627,19 +7719,19 @@
       </c>
       <c r="B14" s="3">
         <f t="shared" ref="B14:F14" si="2" xml:space="preserve"> B4/MIN($B4:$F4)</f>
-        <v>268.81465616659557</v>
+        <v>291.7929140019981</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="2"/>
-        <v>8.4505659134872477</v>
+        <v>9.7475200434841955</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="2"/>
-        <v>65.729340541617759</v>
+        <v>72.872513878932168</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="2"/>
-        <v>2.0407196515582138</v>
+        <v>1.9751351170456697</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="2"/>
@@ -7652,19 +7744,19 @@
       </c>
       <c r="B15" s="3">
         <f t="shared" ref="B15:F15" si="3" xml:space="preserve"> B5/MIN($B5:$F5)</f>
-        <v>286.77111074424812</v>
+        <v>308.26775619945397</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="3"/>
-        <v>4.0956002058186103</v>
+        <v>4.4475642089934864</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" si="3"/>
-        <v>17.685174042540435</v>
+        <v>19.445610151644448</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" si="3"/>
-        <v>1.1287874473798363</v>
+        <v>1.0751343067002523</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="3"/>
@@ -7677,19 +7769,19 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" ref="B16:F16" si="4" xml:space="preserve"> B6/MIN($B6:$F6)</f>
-        <v>436.73251495121059</v>
+        <v>428.22621458820959</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="4"/>
-        <v>10.075572801182574</v>
+        <v>10.498630425621558</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="4"/>
-        <v>47.884973486249905</v>
+        <v>45.726785063277759</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="4"/>
-        <v>2.6001478196600178</v>
+        <v>2.433234737655555</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="4"/>
@@ -7702,15 +7794,15 @@
       </c>
       <c r="B17" s="3">
         <f t="shared" ref="B17:F17" si="5" xml:space="preserve"> B7/MIN($B7:$F7)</f>
-        <v>784.9658720004154</v>
+        <v>717.99775981628204</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="5"/>
-        <v>7.4208083086364711</v>
+        <v>7.2477949158675576</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="5"/>
-        <v>29.215637272402709</v>
+        <v>29.410187143645469</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="5"/>
@@ -7718,7 +7810,7 @@
       </c>
       <c r="F17" s="3">
         <f t="shared" si="5"/>
-        <v>3.0121828486678308</v>
+        <v>2.7048617708531326</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -7727,15 +7819,15 @@
       </c>
       <c r="B18" s="3">
         <f t="shared" ref="B18:F18" si="6" xml:space="preserve"> B8/MIN($B8:$F8)</f>
-        <v>469.21954448644283</v>
+        <v>504.57942313721281</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="6"/>
-        <v>7.0285638719915378</v>
+        <v>7.3977823231779576</v>
       </c>
       <c r="D18" s="3">
         <f t="shared" si="6"/>
-        <v>29.49302169160914</v>
+        <v>30.387296913612573</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" si="6"/>
@@ -7743,7 +7835,7 @@
       </c>
       <c r="F18" s="3">
         <f t="shared" si="6"/>
-        <v>2.5965344313616026</v>
+        <v>2.4714444503255182</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -7752,11 +7844,11 @@
       </c>
       <c r="B19" s="3">
         <f t="shared" ref="B19:F19" si="7" xml:space="preserve"> B9/MIN($B9:$F9)</f>
-        <v>644.54239150338776</v>
+        <v>731.98752692031496</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="7"/>
-        <v>11.56389600878798</v>
+        <v>13.343675417661101</v>
       </c>
       <c r="D19" s="3" t="e">
         <f t="shared" si="7"/>
@@ -7785,11 +7877,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4DC42C-376D-41DF-9AD8-63D3F4858048}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7806,7 +7896,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
@@ -7823,19 +7913,19 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>15912.3591486317</v>
+        <v>17096.1189698948</v>
       </c>
       <c r="C2">
-        <v>709.29381631906301</v>
+        <v>806.68473351400098</v>
       </c>
       <c r="D2">
-        <v>3143.0446194225701</v>
+        <v>3654.1549953314602</v>
       </c>
       <c r="E2">
-        <v>383.76115055525202</v>
+        <v>414.63874740614898</v>
       </c>
       <c r="F2">
-        <v>61.909949164851099</v>
+        <v>59.256532940743398</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7843,19 +7933,19 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>14909.9999999999</v>
+        <v>17804.438784791699</v>
       </c>
       <c r="C3">
-        <v>322.68251904142602</v>
+        <v>369.07178446207701</v>
       </c>
       <c r="D3">
-        <v>1557.42611298166</v>
+        <v>1680.22017045454</v>
       </c>
       <c r="E3">
-        <v>70.746049246600506</v>
+        <v>69.932685115931093</v>
       </c>
       <c r="F3">
-        <v>41.165413533834503</v>
+        <v>37.918215613382898</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -7863,19 +7953,19 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>3559.7206909224501</v>
+        <v>3906.17726051924</v>
       </c>
       <c r="C4">
-        <v>137.149228767887</v>
+        <v>159.726078104756</v>
       </c>
       <c r="D4">
-        <v>1048.85635864592</v>
+        <v>1151.0407400818301</v>
       </c>
       <c r="E4">
-        <v>32.252186588921198</v>
+        <v>34.4506517690875</v>
       </c>
       <c r="F4">
-        <v>16.676035225782201</v>
+        <v>15.716374269005801</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -7883,19 +7973,19 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>3298.97473452947</v>
+        <v>3554.1172240201299</v>
       </c>
       <c r="C5">
-        <v>68.75</v>
+        <v>71.41514752866</v>
       </c>
       <c r="D5">
-        <v>288.93023255813898</v>
+        <v>324.33910665451202</v>
       </c>
       <c r="E5">
-        <v>20.087170740951201</v>
+        <v>17.965204236005999</v>
       </c>
       <c r="F5">
-        <v>15.565610859728499</v>
+        <v>15.047371354263399</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -7903,19 +7993,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1059.72377752892</v>
+        <v>1159.30035734436</v>
       </c>
       <c r="C6">
-        <v>34.872761545711597</v>
+        <v>39.901197035910997</v>
       </c>
       <c r="D6">
-        <v>165.94216594216499</v>
+        <v>182.970671712393</v>
       </c>
       <c r="E6">
-        <v>9.25401322001888</v>
+        <v>8.8863679334467705</v>
       </c>
       <c r="F6">
-        <v>3.5930408472012099</v>
+        <v>3.3917467495760301</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -7923,19 +8013,19 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>1563.7800934243601</v>
+        <v>1650.7795889440099</v>
       </c>
       <c r="C7">
-        <v>19.788918205804698</v>
+        <v>20.892687559354201</v>
       </c>
       <c r="D7">
-        <v>74.204946996466404</v>
+        <v>87.129087129087097</v>
       </c>
       <c r="E7">
-        <v>2.8184892897406901</v>
+        <v>3.0126153266804701</v>
       </c>
       <c r="F7">
-        <v>7.4836295603367597</v>
+        <v>6.7491563554555603</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -7943,19 +8033,19 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>1540.1568920433299</v>
+        <v>1552.9766123316699</v>
       </c>
       <c r="C8">
-        <v>25.2830188679245</v>
+        <v>25.631768953068502</v>
       </c>
       <c r="D8">
-        <v>97.597881596368396</v>
+        <v>111.35213304410701</v>
       </c>
       <c r="E8">
-        <v>3.5978034463169801</v>
+        <v>3.9735099337748299</v>
       </c>
       <c r="F8">
-        <v>8.9502144322207702</v>
+        <v>8.5343228200371009</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -7963,16 +8053,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>116.29526462395501</v>
+        <v>142.7304964539</v>
       </c>
       <c r="C9">
-        <v>4.1067761806981498</v>
+        <v>4.7366426676771498</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
       </c>
       <c r="E9">
-        <v>0.34934497816593801</v>
+        <v>0.356442701835679</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
@@ -7986,13 +8076,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
       </c>
       <c r="E11" t="s">
         <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -8000,18 +8093,22 @@
         <v>2</v>
       </c>
       <c r="B12" s="3">
-        <f xml:space="preserve"> B2/MIN($B2:$E2)</f>
-        <v>41.464226187587265</v>
+        <f xml:space="preserve"> B2/MIN($B2:$F2)</f>
+        <v>288.51028100126848</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" ref="C12:E12" si="0" xml:space="preserve"> C2/MIN($B2:$E2)</f>
-        <v>1.8482689435676538</v>
+        <f t="shared" ref="C12:F12" si="0" xml:space="preserve"> C2/MIN($B2:$F2)</f>
+        <v>13.613431186071697</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>8.1901063066831981</v>
+        <v>61.666702623078194</v>
       </c>
       <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>6.9973507869720999</v>
+      </c>
+      <c r="F12" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -8021,18 +8118,22 @@
         <v>3</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" ref="B13:E13" si="1" xml:space="preserve"> B3/MIN($B3:$E3)</f>
-        <v>210.7538181818168</v>
+        <f t="shared" ref="B13:F13" si="1" xml:space="preserve"> B3/MIN($B3:$F3)</f>
+        <v>469.54843461852619</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="1"/>
-        <v>4.5611383600608848</v>
+        <v>9.7333637274802669</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="1"/>
-        <v>22.014319238561544</v>
+        <v>44.311688809046203</v>
       </c>
       <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>1.8443031662926925</v>
+      </c>
+      <c r="F13" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -8042,18 +8143,22 @@
         <v>15</v>
       </c>
       <c r="B14" s="3">
-        <f t="shared" ref="B14:E14" si="2" xml:space="preserve"> B4/MIN($B4:$E4)</f>
-        <v>110.37145283492914</v>
+        <f t="shared" ref="B14:F14" si="2" xml:space="preserve"> B4/MIN($B4:$F4)</f>
+        <v>248.54188336699238</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="2"/>
-        <v>4.2524009462043262</v>
+        <v>10.163036039409622</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="2"/>
-        <v>32.520472860162847</v>
+        <v>73.238313136369683</v>
       </c>
       <c r="E14" s="3">
+        <f t="shared" si="2"/>
+        <v>2.1920228660517136</v>
+      </c>
+      <c r="F14" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -8063,18 +8168,22 @@
         <v>16</v>
       </c>
       <c r="B15" s="3">
-        <f t="shared" ref="B15:E15" si="3" xml:space="preserve"> B5/MIN($B5:$E5)</f>
-        <v>164.23292145388771</v>
+        <f t="shared" ref="B15:F15" si="3" xml:space="preserve"> B5/MIN($B5:$F5)</f>
+        <v>236.19522243086899</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="3"/>
-        <v>3.4225825471698279</v>
+        <v>4.746021470947869</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" si="3"/>
-        <v>14.383819218955724</v>
+        <v>21.554535939768407</v>
       </c>
       <c r="E15" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1939098074372894</v>
+      </c>
+      <c r="F15" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -8084,75 +8193,87 @@
         <v>5</v>
       </c>
       <c r="B16" s="3">
-        <f t="shared" ref="B16:E16" si="4" xml:space="preserve"> B6/MIN($B6:$E6)</f>
-        <v>114.51504902072725</v>
+        <f t="shared" ref="B16:F16" si="4" xml:space="preserve"> B6/MIN($B6:$F6)</f>
+        <v>341.8003886903623</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="4"/>
-        <v>3.7683933139702659</v>
+        <v>11.764202926087764</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="4"/>
-        <v>17.93191364619927</v>
+        <v>53.945853043203897</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="4"/>
+        <v>2.6199974790445575</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" ref="B17:E17" si="5" xml:space="preserve"> B7/MIN($B7:$E7)</f>
-        <v>554.82917714696475</v>
+        <f t="shared" ref="B17:F17" si="5" xml:space="preserve"> B7/MIN($B7:$F7)</f>
+        <v>547.95564980510312</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="5"/>
-        <v>7.0211081794195289</v>
+        <v>6.9350664767331454</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="5"/>
-        <v>26.327915194346364</v>
+        <v>28.921411358911392</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="3">
+        <f t="shared" si="5"/>
+        <v>2.2402980877390335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" ref="B18:E18" si="6" xml:space="preserve"> B8/MIN($B8:$E8)</f>
-        <v>428.08255509899141</v>
+        <f t="shared" ref="B18:F18" si="6" xml:space="preserve"> B8/MIN($B8:$F8)</f>
+        <v>390.83244743680405</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="6"/>
-        <v>7.0273485600794467</v>
+        <v>6.4506618531889135</v>
       </c>
       <c r="D18" s="3">
         <f t="shared" si="6"/>
-        <v>27.12707435318012</v>
+        <v>28.023620149433629</v>
       </c>
       <c r="E18" s="3">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F18" s="3">
+        <f t="shared" si="6"/>
+        <v>2.1478045763760063</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" ref="B19:E19" si="7" xml:space="preserve"> B9/MIN($B9:$E9)</f>
-        <v>332.895194986072</v>
+        <f t="shared" ref="B19:F19" si="7" xml:space="preserve"> B9/MIN($B9:$F9)</f>
+        <v>400.43040780141746</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="7"/>
-        <v>11.755646817248483</v>
+        <v>13.288651004168278</v>
       </c>
       <c r="D19" s="3" t="e">
         <f t="shared" si="7"/>
@@ -8162,10 +8283,9 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G23" t="s">
-        <v>23</v>
+      <c r="F19" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -8203,7 +8323,7 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -8315,7 +8435,7 @@
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -8341,7 +8461,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" ref="B13:D19" si="1" xml:space="preserve"> B3 / MIN($B3:$E3)</f>
+        <f t="shared" ref="B13:D18" si="1" xml:space="preserve"> B3 / MIN($B3:$E3)</f>
         <v>7940.3939676037953</v>
       </c>
       <c r="C13" s="1">
@@ -8460,7 +8580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EFA07C-E270-4B85-8B26-6FA6BD53AA2B}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Developing #257 - spoiler functions are reusable
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AF7CB9-C7CD-46FB-B95A-634BD7291412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B21714-3332-4BB0-BA06-682659F8105B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
   <sheets>
     <sheet name="is" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="25">
   <si>
     <t>Components</t>
   </si>
@@ -341,28 +341,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1803.0919840708693</c:v>
+                  <c:v>1716.3710909901233</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2025.7246537461999</c:v>
+                  <c:v>1712.0344564644208</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>910.20537949563209</c:v>
+                  <c:v>218.11394055275514</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>791.60208240391262</c:v>
+                  <c:v>9999.99</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2074.7290909090952</c:v>
+                  <c:v>752.48554641332726</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1310.4138697387521</c:v>
+                  <c:v>910.91728527242594</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1010.3963547216247</c:v>
+                  <c:v>9999.99</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1743.3686144799733</c:v>
+                  <c:v>9999.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -436,28 +436,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3001.7933623315657</c:v>
+                  <c:v>2958.275825332566</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2075.1773920680448</c:v>
+                  <c:v>2175.6998457331215</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>770.62503023706108</c:v>
+                  <c:v>370.88554491563849</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1873.7547593582919</c:v>
+                  <c:v>708.73286132302189</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>644.85425531914871</c:v>
+                  <c:v>703.83583149644937</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>598.59340121059392</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>893.12259259259224</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -531,22 +531,22 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1438.6576720819507</c:v>
+                  <c:v>634.98618008104415</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>855.002938990144</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>202.64369855207511</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>76.050121665742722</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>271.78743894625092</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>232.47100123663625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>281.49277258567065</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -626,25 +626,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>140.23872405824903</c:v>
+                  <c:v>134.4488632058609</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>119.71308445353615</c:v>
+                  <c:v>112.24391976238661</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>188.4956631225522</c:v>
+                  <c:v>98.513577794225156</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>134.55581787521101</c:v>
+                  <c:v>51.827842724448971</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>123.97234654731463</c:v>
+                  <c:v>130.41386815920433</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>113.09405451584497</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -721,25 +721,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5.8542376143570616</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.8502706552706571</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5114960282436067</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4691168558551451</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -816,28 +816,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.5753427852785933</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8048711175410641</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9943498968571842</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1165114264052871</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4793853073463317</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -915,7 +915,8 @@
         <c:axId val="480554528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="3000"/>
+          <c:max val="3200"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1215,28 +1216,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>335.85878022317149</c:v>
+                  <c:v>332.746842533684</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>829.41938026445678</c:v>
+                  <c:v>666.89171571387453</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>291.7929140019981</c:v>
+                  <c:v>259.84801423535163</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>308.26775619945397</c:v>
+                  <c:v>9999.99</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>428.22621458820959</c:v>
+                  <c:v>417.23237169935095</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>717.99775981628204</c:v>
+                  <c:v>736.17855836077445</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>504.57942313721281</c:v>
+                  <c:v>9999.99</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>731.98752692031496</c:v>
+                  <c:v>9999.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1310,28 +1311,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>14.899528598490065</c:v>
+                  <c:v>14.325122893734195</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.163352438742226</c:v>
+                  <c:v>8.4259909444211445</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.7475200434841955</c:v>
+                  <c:v>8.660050441670224</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.4475642089934864</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.498630425621558</c:v>
+                  <c:v>9.5644662503716908</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.2477949158675576</c:v>
+                  <c:v>7.5110705016155661</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.3977823231779576</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.343675417661101</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1405,25 +1406,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>62.206683941911493</c:v>
+                  <c:v>58.556035850635247</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46.084315370439519</c:v>
+                  <c:v>37.959376386982719</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72.872513878932168</c:v>
+                  <c:v>65.91523224830145</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.445610151644448</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.726785063277759</c:v>
+                  <c:v>44.019297598477905</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29.410187143645469</c:v>
+                  <c:v>29.314369995785984</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.387296913612573</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1500,28 +1501,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.4279932380915366</c:v>
+                  <c:v>6.3728307942069069</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8049943543115226</c:v>
+                  <c:v>1.8198606371180286</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9751351170456697</c:v>
+                  <c:v>1.9347346840741886</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0751343067002523</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.433234737655555</c:v>
+                  <c:v>2.5721183040825109</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1604,16 +1605,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.7048617708531326</c:v>
+                  <c:v>2.768639885374657</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4714444503255182</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1694,6 +1695,7 @@
         <c:axId val="381772640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="800"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1993,28 +1995,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>288.51028100126848</c:v>
+                  <c:v>268.23526420622443</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>469.54843461852619</c:v>
+                  <c:v>371.20787873711248</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>248.54188336699238</c:v>
+                  <c:v>212.96363282186502</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>236.19522243086899</c:v>
+                  <c:v>9999.99</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>341.8003886903623</c:v>
+                  <c:v>244.90415776912485</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>547.95564980510312</c:v>
+                  <c:v>604.30986250033095</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>390.83244743680405</c:v>
+                  <c:v>9999.99</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>400.43040780141746</c:v>
+                  <c:v>9999.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2088,28 +2090,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>13.613431186071697</c:v>
+                  <c:v>12.487759940792849</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.7333637274802669</c:v>
+                  <c:v>8.4286770773598985</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.163036039409622</c:v>
+                  <c:v>8.8534415338868087</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.746021470947869</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.764202926087764</c:v>
+                  <c:v>9.7137126185266283</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.9350664767331454</c:v>
+                  <c:v>8.1263985730500981</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.4506618531889135</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.288651004168278</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2183,25 +2185,25 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>61.666702623078194</c:v>
+                  <c:v>53.408595188812598</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44.311688809046203</c:v>
+                  <c:v>40.745393000293141</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>73.238313136369683</c:v>
+                  <c:v>64.381765852157386</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.554535939768407</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53.945853043203897</c:v>
+                  <c:v>43.656701000789333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28.921411358911392</c:v>
+                  <c:v>27.527834049104669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.023620149433629</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2278,28 +2280,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.9973507869720999</c:v>
+                  <c:v>6.4245749700543353</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8443031662926925</c:v>
+                  <c:v>1.8514451249447279</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1920228660517136</c:v>
+                  <c:v>1.9474428084508635</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1939098074372894</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6199974790445575</c:v>
+                  <c:v>2.5896423433702087</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2382,16 +2384,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2402980877390335</c:v>
+                  <c:v>2.7214447195607736</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.1478045763760063</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2472,6 +2474,7 @@
         <c:axId val="381772640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="700"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6964,13 +6967,13 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6991,10 +6994,10 @@
         <v>19</v>
       </c>
       <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -7002,22 +7005,22 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>117845.05232237899</v>
+        <v>109269.155555555</v>
       </c>
       <c r="C2" s="2">
-        <v>196188.82395909401</v>
+        <v>188332.40843507199</v>
       </c>
       <c r="D2">
-        <v>94026.644307806899</v>
+        <v>40425.059622087603</v>
       </c>
       <c r="E2">
-        <v>9165.6110283159396</v>
+        <v>8559.4040968342597</v>
       </c>
       <c r="F2">
-        <v>65.357204936554794</v>
+        <v>372.69772481040002</v>
       </c>
       <c r="G2">
-        <v>429.74602594555</v>
+        <v>63.662896753009797</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -7025,22 +7028,22 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>84088.051470588194</v>
+        <v>66141.004261626804</v>
       </c>
       <c r="C3" s="2">
-        <v>86140.840035746194</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
+        <v>84053.783044667201</v>
+      </c>
+      <c r="D3">
+        <v>33031.317108088697</v>
       </c>
       <c r="E3">
-        <v>4969.3032015065901</v>
+        <v>4336.3178511471697</v>
       </c>
       <c r="F3">
-        <v>41.510109142959301</v>
+        <v>71.481481481481396</v>
       </c>
       <c r="G3">
-        <v>74.9203970781045</v>
+        <v>38.632986627043003</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -7048,22 +7051,22 @@
         <v>15</v>
       </c>
       <c r="B4" s="2">
-        <v>16115.7721194357</v>
+        <v>7010.9508082739403</v>
       </c>
       <c r="C4" s="2">
-        <v>13644.412191582</v>
+        <v>11921.568627450901</v>
       </c>
       <c r="D4">
-        <v>1346.5163555719801</v>
+        <v>6513.6827043462699</v>
       </c>
       <c r="E4">
-        <v>3337.43704532736</v>
+        <v>3166.5736087846599</v>
       </c>
       <c r="F4">
-        <v>17.705643673920999</v>
-      </c>
-      <c r="G4">
-        <v>35.311248634874403</v>
+        <v>32.143524574845799</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -7071,22 +7074,22 @@
         <v>16</v>
       </c>
       <c r="B5" s="2">
-        <v>14110.0407558354</v>
+        <v>14108.723135271801</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>4844.5196465501003</v>
+      <c r="D5" t="s">
+        <v>4</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="F5">
-        <v>17.824663514005</v>
-      </c>
-      <c r="G5">
-        <v>19.901440485216</v>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -7094,22 +7097,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>7841.0018552875699</v>
+        <v>6906.1232017705597</v>
       </c>
       <c r="C6" s="2">
-        <v>7081.4616755793204</v>
-      </c>
-      <c r="D6" t="s">
+        <v>6504.5720555961898</v>
+      </c>
+      <c r="D6">
+        <v>2133.5604159196801</v>
+      </c>
+      <c r="E6">
+        <v>475.66291318561503</v>
+      </c>
+      <c r="F6">
+        <v>9.1777486420677992</v>
+      </c>
+      <c r="G6" t="s">
         <v>4</v>
-      </c>
-      <c r="E6">
-        <v>508.52538879520301</v>
-      </c>
-      <c r="F6">
-        <v>3.7792894935752002</v>
-      </c>
-      <c r="G6">
-        <v>9.3703148425787095</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -7117,22 +7120,22 @@
         <v>17</v>
       </c>
       <c r="B7" s="2">
-        <v>3960.4499274310501</v>
+        <v>2573.69735902926</v>
       </c>
       <c r="C7" s="2">
-        <v>1948.9361702127601</v>
-      </c>
-      <c r="D7" t="s">
+        <v>1988.6113152093999</v>
+      </c>
+      <c r="D7">
+        <v>795.32710280373794</v>
+      </c>
+      <c r="E7">
+        <v>368.47014925373099</v>
+      </c>
+      <c r="F7">
+        <v>2.8253908457336498</v>
+      </c>
+      <c r="G7" t="s">
         <v>4</v>
-      </c>
-      <c r="E7">
-        <v>374.68030690537</v>
-      </c>
-      <c r="F7">
-        <v>7.5904677846425397</v>
-      </c>
-      <c r="G7">
-        <v>3.0222893842085301</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -7140,22 +7143,22 @@
         <v>18</v>
       </c>
       <c r="B8" s="2">
-        <v>4017.1002364926298</v>
-      </c>
-      <c r="C8" s="2">
-        <v>2379.8677443056499</v>
+        <v>1641.1124977714301</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="E8">
-        <v>449.63558213418003</v>
-      </c>
-      <c r="F8">
-        <v>9.8166327097610608</v>
-      </c>
-      <c r="G8">
-        <v>3.9757667550170299</v>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -7163,10 +7166,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="2">
-        <v>616.68504226387302</v>
-      </c>
-      <c r="C9" s="2">
-        <v>315.92592592592501</v>
+        <v>443.81223328591699</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -7177,8 +7180,8 @@
       <c r="F9" t="s">
         <v>4</v>
       </c>
-      <c r="G9">
-        <v>0.35373187124159799</v>
+      <c r="G9" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -7209,28 +7212,28 @@
         <v>2</v>
       </c>
       <c r="B12" s="3">
-        <f xml:space="preserve"> B2 / MIN($B2:$G2)</f>
-        <v>1803.0919840708693</v>
+        <f xml:space="preserve"> IF(B2 = MIN($B2:$G2), 9999.99, B2 / MIN($B2:$G2))</f>
+        <v>1716.3710909901233</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:G12" si="0" xml:space="preserve"> C2 / MIN($B2:$G2)</f>
-        <v>3001.7933623315657</v>
+        <v>2958.275825332566</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>1438.6576720819507</v>
+        <v>634.98618008104415</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>140.23872405824903</v>
+        <v>134.4488632058609</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5.8542376143570616</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="0"/>
-        <v>6.5753427852785933</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -7238,28 +7241,28 @@
         <v>3</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" ref="B13:G13" si="1" xml:space="preserve"> B3 / MIN($B3:$G3)</f>
-        <v>2025.7246537461999</v>
+        <f t="shared" ref="B13:B19" si="1" xml:space="preserve"> IF(B3 = MIN($B3:$G3), 9999.99, B3 / MIN($B3:$G3))</f>
+        <v>1712.0344564644208</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="1"/>
-        <v>2075.1773920680448</v>
-      </c>
-      <c r="D13" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <f t="shared" ref="B13:G13" si="2" xml:space="preserve"> C3 / MIN($B3:$G3)</f>
+        <v>2175.6998457331215</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="2"/>
+        <v>855.002938990144</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="1"/>
-        <v>119.71308445353615</v>
+        <f t="shared" si="2"/>
+        <v>112.24391976238661</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>1.8502706552706571</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="2"/>
         <v>1</v>
-      </c>
-      <c r="G13" s="3">
-        <f t="shared" si="1"/>
-        <v>1.8048711175410641</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -7267,28 +7270,28 @@
         <v>15</v>
       </c>
       <c r="B14" s="3">
-        <f t="shared" ref="B14:G14" si="2" xml:space="preserve"> B4 / MIN($B4:$G4)</f>
-        <v>910.20537949563209</v>
+        <f t="shared" si="1"/>
+        <v>218.11394055275514</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="2"/>
-        <v>770.62503023706108</v>
+        <f t="shared" ref="B14:G14" si="3" xml:space="preserve"> C4 / MIN($B4:$G4)</f>
+        <v>370.88554491563849</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="2"/>
-        <v>76.050121665742722</v>
+        <f t="shared" si="3"/>
+        <v>202.64369855207511</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="2"/>
-        <v>188.4956631225522</v>
+        <f t="shared" si="3"/>
+        <v>98.513577794225156</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G14" s="3">
-        <f t="shared" si="2"/>
-        <v>1.9943498968571842</v>
+      <c r="G14" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -7296,28 +7299,28 @@
         <v>16</v>
       </c>
       <c r="B15" s="3">
-        <f t="shared" ref="B15:G15" si="3" xml:space="preserve"> B5 / MIN($B5:$G5)</f>
-        <v>791.60208240391262</v>
+        <f t="shared" si="1"/>
+        <v>9999.99</v>
       </c>
       <c r="C15" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="B15:G15" si="4" xml:space="preserve"> C5 / MIN($B5:$G5)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D15" s="3">
-        <f t="shared" si="3"/>
-        <v>271.78743894625092</v>
+      <c r="D15" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
       </c>
       <c r="E15" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F15" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G15" s="3">
-        <f t="shared" si="3"/>
-        <v>1.1165114264052871</v>
+      <c r="F15" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G15" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -7325,28 +7328,28 @@
         <v>5</v>
       </c>
       <c r="B16" s="3">
-        <f t="shared" ref="B16:G16" si="4" xml:space="preserve"> B6 / MIN($B6:$G6)</f>
-        <v>2074.7290909090952</v>
+        <f t="shared" si="1"/>
+        <v>752.48554641332726</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" si="4"/>
-        <v>1873.7547593582919</v>
-      </c>
-      <c r="D16" s="3" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="B16:G16" si="5" xml:space="preserve"> C6 / MIN($B6:$G6)</f>
+        <v>708.73286132302189</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="5"/>
+        <v>232.47100123663625</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="5"/>
+        <v>51.827842724448971</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G16" s="3" t="e">
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="shared" si="4"/>
-        <v>134.55581787521101</v>
-      </c>
-      <c r="F16" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="G16" s="3">
-        <f t="shared" si="4"/>
-        <v>2.4793853073463317</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -7354,28 +7357,28 @@
         <v>17</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" ref="B17:G17" si="5" xml:space="preserve"> B7 / MIN($B7:$G7)</f>
-        <v>1310.4138697387521</v>
+        <f t="shared" si="1"/>
+        <v>910.91728527242594</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="5"/>
-        <v>644.85425531914871</v>
-      </c>
-      <c r="D17" s="3" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="B17:G17" si="6" xml:space="preserve"> C7 / MIN($B7:$G7)</f>
+        <v>703.83583149644937</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="6"/>
+        <v>281.49277258567065</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="6"/>
+        <v>130.41386815920433</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G17" s="3" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
-      </c>
-      <c r="E17" s="3">
-        <f t="shared" si="5"/>
-        <v>123.97234654731463</v>
-      </c>
-      <c r="F17" s="3">
-        <f t="shared" si="5"/>
-        <v>2.5114960282436067</v>
-      </c>
-      <c r="G17" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -7383,28 +7386,28 @@
         <v>18</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" ref="B18:G18" si="6" xml:space="preserve"> B8 / MIN($B8:$G8)</f>
-        <v>1010.3963547216247</v>
-      </c>
-      <c r="C18" s="3">
-        <f t="shared" si="6"/>
-        <v>598.59340121059392</v>
+        <f t="shared" si="1"/>
+        <v>9999.99</v>
+      </c>
+      <c r="C18" s="3" t="e">
+        <f t="shared" ref="B18:G18" si="7" xml:space="preserve"> C8 / MIN($B8:$G8)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D18" s="3" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E18" s="3">
-        <f t="shared" si="6"/>
-        <v>113.09405451584497</v>
-      </c>
-      <c r="F18" s="3">
-        <f t="shared" si="6"/>
-        <v>2.4691168558551451</v>
-      </c>
-      <c r="G18" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
+      <c r="E18" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F18" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G18" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -7412,28 +7415,28 @@
         <v>11</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" ref="B19:G19" si="7" xml:space="preserve"> B9 / MIN($B9:$G9)</f>
-        <v>1743.3686144799733</v>
-      </c>
-      <c r="C19" s="3">
-        <f t="shared" si="7"/>
-        <v>893.12259259259224</v>
+        <f t="shared" si="1"/>
+        <v>9999.99</v>
+      </c>
+      <c r="C19" s="3" t="e">
+        <f t="shared" ref="B19:G19" si="8" xml:space="preserve"> C9 / MIN($B9:$G9)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D19" s="3" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="E19" s="3" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="F19" s="3" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G19" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="G19" s="3" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -7452,8 +7455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050C2C99-5EE7-403C-9AB2-DBCB91E8248D}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7488,19 +7491,19 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>22979.1521890201</v>
+        <v>20567.3992673992</v>
       </c>
       <c r="C2">
-        <v>1019.412191582</v>
+        <v>885.44949026876702</v>
       </c>
       <c r="D2">
-        <v>4256.1247216035599</v>
+        <v>3619.4043486205001</v>
       </c>
       <c r="E2">
-        <v>439.79744936233999</v>
+        <v>393.91074130105898</v>
       </c>
       <c r="F2">
-        <v>68.419090231170699</v>
+        <v>61.810952467016001</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7508,19 +7511,19 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>35552.973977695103</v>
+        <v>26125.910140294702</v>
       </c>
       <c r="C3">
-        <v>435.65102694554298</v>
+        <v>330.093592512599</v>
       </c>
       <c r="D3">
-        <v>1975.3993023682699</v>
+        <v>1487.08288482238</v>
       </c>
       <c r="E3">
-        <v>77.370892018779301</v>
+        <v>71.294206170052604</v>
       </c>
       <c r="F3">
-        <v>42.8648941942485</v>
+        <v>39.175640549572897</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -7528,19 +7531,19 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>5302.4042742653601</v>
+        <v>4308.7667708141798</v>
       </c>
       <c r="C4">
-        <v>177.13004484304901</v>
+        <v>143.599856579419</v>
       </c>
       <c r="D4">
-        <v>1324.22519713918</v>
+        <v>1092.99800977021</v>
       </c>
       <c r="E4">
-        <v>35.891772501380402</v>
+        <v>32.081524816002997</v>
       </c>
       <c r="F4">
-        <v>18.171806167400799</v>
+        <v>16.581872997927199</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -7548,19 +7551,19 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>5325.8222787570403</v>
-      </c>
-      <c r="C5">
-        <v>76.838839204234304</v>
-      </c>
-      <c r="D5">
-        <v>335.95425303788397</v>
-      </c>
-      <c r="E5">
-        <v>18.574677786201601</v>
-      </c>
-      <c r="F5">
-        <v>17.276611554894998</v>
+        <v>4320.1544685546096</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -7568,19 +7571,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1707.0521082673499</v>
+        <v>1503.3975084937699</v>
       </c>
       <c r="C6">
-        <v>41.851032448377502</v>
+        <v>34.463276836158101</v>
       </c>
       <c r="D6">
-        <v>182.28217280349901</v>
+        <v>158.613057912209</v>
       </c>
       <c r="E6">
-        <v>9.6996828949822795</v>
+        <v>9.2680158880272305</v>
       </c>
       <c r="F6">
-        <v>3.98633257403189</v>
+        <v>3.60326190024653</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -7588,19 +7591,19 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>2168.7680115273702</v>
+        <v>1926.08854738382</v>
       </c>
       <c r="C7">
-        <v>21.892527591821899</v>
+        <v>19.651464590285499</v>
       </c>
       <c r="D7">
-        <v>88.835755011955101</v>
+        <v>76.696165191740405</v>
       </c>
       <c r="E7">
-        <v>3.0205776854823401</v>
+        <v>2.6163333956269801</v>
       </c>
       <c r="F7">
-        <v>8.1702451073532192</v>
+        <v>7.2436849925705697</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -7608,19 +7611,19 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>2004.57205559619</v>
-      </c>
-      <c r="C8">
-        <v>29.389600602863599</v>
-      </c>
-      <c r="D8">
-        <v>120.72138387927799</v>
-      </c>
-      <c r="E8">
-        <v>3.9727582292849002</v>
-      </c>
-      <c r="F8">
-        <v>9.8184512782511995</v>
+        <v>1079.67183226982</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -7628,16 +7631,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>261.84493898061697</v>
-      </c>
-      <c r="C9">
-        <v>4.7732696897374698</v>
+        <v>210.21184139054799</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="E9">
-        <v>0.35771776068681799</v>
+      <c r="E9" t="s">
+        <v>4</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
@@ -7668,20 +7671,20 @@
         <v>2</v>
       </c>
       <c r="B12" s="3">
-        <f xml:space="preserve"> B2/MIN($B2:$F2)</f>
-        <v>335.85878022317149</v>
+        <f xml:space="preserve"> IF(B2 = MIN($B2:$F2), 9999.99, B2 / MIN($B2:$F2))</f>
+        <v>332.746842533684</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:F12" si="0" xml:space="preserve"> C2/MIN($B2:$F2)</f>
-        <v>14.899528598490065</v>
+        <v>14.325122893734195</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>62.206683941911493</v>
+        <v>58.556035850635247</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>6.4279932380915366</v>
+        <v>6.3728307942069069</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
@@ -7693,23 +7696,23 @@
         <v>3</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" ref="B13:F13" si="1" xml:space="preserve"> B3/MIN($B3:$F3)</f>
-        <v>829.41938026445678</v>
+        <f t="shared" ref="B13:B19" si="1" xml:space="preserve"> IF(B3 = MIN($B3:$F3), 9999.99, B3 / MIN($B3:$F3))</f>
+        <v>666.89171571387453</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="1"/>
-        <v>10.163352438742226</v>
+        <f t="shared" ref="B13:F13" si="2" xml:space="preserve"> C3/MIN($B3:$F3)</f>
+        <v>8.4259909444211445</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="1"/>
-        <v>46.084315370439519</v>
+        <f t="shared" si="2"/>
+        <v>37.959376386982719</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="1"/>
-        <v>1.8049943543115226</v>
+        <f t="shared" si="2"/>
+        <v>1.8198606371180286</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -7718,23 +7721,23 @@
         <v>15</v>
       </c>
       <c r="B14" s="3">
-        <f t="shared" ref="B14:F14" si="2" xml:space="preserve"> B4/MIN($B4:$F4)</f>
-        <v>291.7929140019981</v>
+        <f t="shared" si="1"/>
+        <v>259.84801423535163</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="2"/>
-        <v>9.7475200434841955</v>
+        <f t="shared" ref="B14:F14" si="3" xml:space="preserve"> C4/MIN($B4:$F4)</f>
+        <v>8.660050441670224</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="2"/>
-        <v>72.872513878932168</v>
+        <f t="shared" si="3"/>
+        <v>65.91523224830145</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="2"/>
-        <v>1.9751351170456697</v>
+        <f t="shared" si="3"/>
+        <v>1.9347346840741886</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7743,24 +7746,24 @@
         <v>16</v>
       </c>
       <c r="B15" s="3">
-        <f t="shared" ref="B15:F15" si="3" xml:space="preserve"> B5/MIN($B5:$F5)</f>
-        <v>308.26775619945397</v>
-      </c>
-      <c r="C15" s="3">
-        <f t="shared" si="3"/>
-        <v>4.4475642089934864</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" si="3"/>
-        <v>19.445610151644448</v>
-      </c>
-      <c r="E15" s="3">
-        <f t="shared" si="3"/>
-        <v>1.0751343067002523</v>
-      </c>
-      <c r="F15" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>9999.99</v>
+      </c>
+      <c r="C15" s="3" t="e">
+        <f t="shared" ref="B15:F15" si="4" xml:space="preserve"> C5/MIN($B5:$F5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D15" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E15" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F15" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -7768,23 +7771,23 @@
         <v>5</v>
       </c>
       <c r="B16" s="3">
-        <f t="shared" ref="B16:F16" si="4" xml:space="preserve"> B6/MIN($B6:$F6)</f>
-        <v>428.22621458820959</v>
+        <f t="shared" si="1"/>
+        <v>417.23237169935095</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" si="4"/>
-        <v>10.498630425621558</v>
+        <f t="shared" ref="B16:F16" si="5" xml:space="preserve"> C6/MIN($B6:$F6)</f>
+        <v>9.5644662503716908</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="4"/>
-        <v>45.726785063277759</v>
+        <f t="shared" si="5"/>
+        <v>44.019297598477905</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="4"/>
-        <v>2.433234737655555</v>
+        <f t="shared" si="5"/>
+        <v>2.5721183040825109</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -7793,24 +7796,24 @@
         <v>17</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" ref="B17:F17" si="5" xml:space="preserve"> B7/MIN($B7:$F7)</f>
-        <v>717.99775981628204</v>
+        <f t="shared" si="1"/>
+        <v>736.17855836077445</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="5"/>
-        <v>7.2477949158675576</v>
+        <f t="shared" ref="B17:F17" si="6" xml:space="preserve"> C7/MIN($B7:$F7)</f>
+        <v>7.5110705016155661</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="5"/>
-        <v>29.410187143645469</v>
+        <f t="shared" si="6"/>
+        <v>29.314369995785984</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="5"/>
-        <v>2.7048617708531326</v>
+        <f t="shared" si="6"/>
+        <v>2.768639885374657</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -7818,24 +7821,24 @@
         <v>18</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" ref="B18:F18" si="6" xml:space="preserve"> B8/MIN($B8:$F8)</f>
-        <v>504.57942313721281</v>
-      </c>
-      <c r="C18" s="3">
-        <f t="shared" si="6"/>
-        <v>7.3977823231779576</v>
-      </c>
-      <c r="D18" s="3">
-        <f t="shared" si="6"/>
-        <v>30.387296913612573</v>
-      </c>
-      <c r="E18" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="F18" s="3">
-        <f t="shared" si="6"/>
-        <v>2.4714444503255182</v>
+        <f t="shared" si="1"/>
+        <v>9999.99</v>
+      </c>
+      <c r="C18" s="3" t="e">
+        <f t="shared" ref="B18:F18" si="7" xml:space="preserve"> C8/MIN($B8:$F8)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D18" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E18" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F18" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -7843,23 +7846,23 @@
         <v>11</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" ref="B19:F19" si="7" xml:space="preserve"> B9/MIN($B9:$F9)</f>
-        <v>731.98752692031496</v>
-      </c>
-      <c r="C19" s="3">
-        <f t="shared" si="7"/>
-        <v>13.343675417661101</v>
+        <f t="shared" si="1"/>
+        <v>9999.99</v>
+      </c>
+      <c r="C19" s="3" t="e">
+        <f t="shared" ref="B19:F19" si="8" xml:space="preserve"> C9/MIN($B9:$F9)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D19" s="3" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E19" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="E19" s="3" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
       </c>
       <c r="F19" s="3" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7879,7 +7882,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4DC42C-376D-41DF-9AD8-63D3F4858048}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7913,19 +7918,19 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>17096.1189698948</v>
+        <v>16749.399371650299</v>
       </c>
       <c r="C2">
-        <v>806.68473351400098</v>
+        <v>779.77248489157398</v>
       </c>
       <c r="D2">
-        <v>3654.1549953314602</v>
+        <v>3334.98987667955</v>
       </c>
       <c r="E2">
-        <v>414.63874740614898</v>
+        <v>401.16937004903798</v>
       </c>
       <c r="F2">
-        <v>59.256532940743398</v>
+        <v>62.442943217089599</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7933,19 +7938,19 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>17804.438784791699</v>
+        <v>14503.514613392501</v>
       </c>
       <c r="C3">
-        <v>369.07178446207701</v>
+        <v>329.31801334321699</v>
       </c>
       <c r="D3">
-        <v>1680.22017045454</v>
+        <v>1591.9689119170901</v>
       </c>
       <c r="E3">
-        <v>69.932685115931093</v>
+        <v>72.338069754567201</v>
       </c>
       <c r="F3">
-        <v>37.918215613382898</v>
+        <v>39.071138960560198</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -7953,19 +7958,19 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>3906.17726051924</v>
+        <v>3444.5876288659701</v>
       </c>
       <c r="C4">
-        <v>159.726078104756</v>
+        <v>143.20029563931999</v>
       </c>
       <c r="D4">
-        <v>1151.0407400818301</v>
+        <v>1041.3450937155401</v>
       </c>
       <c r="E4">
-        <v>34.4506517690875</v>
+        <v>31.498980915323301</v>
       </c>
       <c r="F4">
-        <v>15.716374269005801</v>
+        <v>16.174534511942799</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -7973,19 +7978,19 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>3554.1172240201299</v>
-      </c>
-      <c r="C5">
-        <v>71.41514752866</v>
-      </c>
-      <c r="D5">
-        <v>324.33910665451202</v>
-      </c>
-      <c r="E5">
-        <v>17.965204236005999</v>
-      </c>
-      <c r="F5">
-        <v>15.047371354263399</v>
+        <v>3097.37221022318</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -7993,19 +7998,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1159.30035734436</v>
+        <v>873.50835322195701</v>
       </c>
       <c r="C6">
-        <v>39.901197035910997</v>
+        <v>34.646243617797197</v>
       </c>
       <c r="D6">
-        <v>182.970671712393</v>
+        <v>155.71190520274001</v>
       </c>
       <c r="E6">
-        <v>8.8863679334467705</v>
+        <v>9.2365692742695504</v>
       </c>
       <c r="F6">
-        <v>3.3917467495760301</v>
+        <v>3.5667354984043498</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -8013,19 +8018,19 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>1650.7795889440099</v>
+        <v>1589.69148346573</v>
       </c>
       <c r="C7">
-        <v>20.892687559354201</v>
+        <v>21.377222852818701</v>
       </c>
       <c r="D7">
-        <v>87.129087129087097</v>
+        <v>72.4144450746833</v>
       </c>
       <c r="E7">
-        <v>3.0126153266804701</v>
+        <v>2.6305900037579799</v>
       </c>
       <c r="F7">
-        <v>6.7491563554555603</v>
+        <v>7.1590052750565096</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -8033,19 +8038,19 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>1552.9766123316699</v>
-      </c>
-      <c r="C8">
-        <v>25.631768953068502</v>
-      </c>
-      <c r="D8">
-        <v>111.35213304410701</v>
-      </c>
-      <c r="E8">
-        <v>3.9735099337748299</v>
-      </c>
-      <c r="F8">
-        <v>8.5343228200371009</v>
+        <v>811.22819767441797</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -8053,16 +8058,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>142.7304964539</v>
-      </c>
-      <c r="C9">
-        <v>4.7366426676771498</v>
+        <v>112.361526288025</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="E9">
-        <v>0.356442701835679</v>
+      <c r="E9" t="s">
+        <v>4</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
@@ -8093,20 +8098,20 @@
         <v>2</v>
       </c>
       <c r="B12" s="3">
-        <f xml:space="preserve"> B2/MIN($B2:$F2)</f>
-        <v>288.51028100126848</v>
+        <f xml:space="preserve"> IF(B2 = MIN($B2:$F2), 9999.99, B2 / MIN($B2:$F2))</f>
+        <v>268.23526420622443</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:F12" si="0" xml:space="preserve"> C2/MIN($B2:$F2)</f>
-        <v>13.613431186071697</v>
+        <v>12.487759940792849</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>61.666702623078194</v>
+        <v>53.408595188812598</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>6.9973507869720999</v>
+        <v>6.4245749700543353</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
@@ -8118,23 +8123,23 @@
         <v>3</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" ref="B13:F13" si="1" xml:space="preserve"> B3/MIN($B3:$F3)</f>
-        <v>469.54843461852619</v>
+        <f t="shared" ref="B13:B19" si="1" xml:space="preserve"> IF(B3 = MIN($B3:$F3), 9999.99, B3 / MIN($B3:$F3))</f>
+        <v>371.20787873711248</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="1"/>
-        <v>9.7333637274802669</v>
+        <f t="shared" ref="B13:F13" si="2" xml:space="preserve"> C3/MIN($B3:$F3)</f>
+        <v>8.4286770773598985</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="1"/>
-        <v>44.311688809046203</v>
+        <f t="shared" si="2"/>
+        <v>40.745393000293141</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="1"/>
-        <v>1.8443031662926925</v>
+        <f t="shared" si="2"/>
+        <v>1.8514451249447279</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -8143,23 +8148,23 @@
         <v>15</v>
       </c>
       <c r="B14" s="3">
-        <f t="shared" ref="B14:F14" si="2" xml:space="preserve"> B4/MIN($B4:$F4)</f>
-        <v>248.54188336699238</v>
+        <f t="shared" si="1"/>
+        <v>212.96363282186502</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="2"/>
-        <v>10.163036039409622</v>
+        <f t="shared" ref="B14:F14" si="3" xml:space="preserve"> C4/MIN($B4:$F4)</f>
+        <v>8.8534415338868087</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="2"/>
-        <v>73.238313136369683</v>
+        <f t="shared" si="3"/>
+        <v>64.381765852157386</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="2"/>
-        <v>2.1920228660517136</v>
+        <f t="shared" si="3"/>
+        <v>1.9474428084508635</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -8168,24 +8173,24 @@
         <v>16</v>
       </c>
       <c r="B15" s="3">
-        <f t="shared" ref="B15:F15" si="3" xml:space="preserve"> B5/MIN($B5:$F5)</f>
-        <v>236.19522243086899</v>
-      </c>
-      <c r="C15" s="3">
-        <f t="shared" si="3"/>
-        <v>4.746021470947869</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" si="3"/>
-        <v>21.554535939768407</v>
-      </c>
-      <c r="E15" s="3">
-        <f t="shared" si="3"/>
-        <v>1.1939098074372894</v>
-      </c>
-      <c r="F15" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>9999.99</v>
+      </c>
+      <c r="C15" s="3" t="e">
+        <f t="shared" ref="B15:F15" si="4" xml:space="preserve"> C5/MIN($B5:$F5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D15" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E15" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F15" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -8193,23 +8198,23 @@
         <v>5</v>
       </c>
       <c r="B16" s="3">
-        <f t="shared" ref="B16:F16" si="4" xml:space="preserve"> B6/MIN($B6:$F6)</f>
-        <v>341.8003886903623</v>
+        <f t="shared" si="1"/>
+        <v>244.90415776912485</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" si="4"/>
-        <v>11.764202926087764</v>
+        <f t="shared" ref="B16:F16" si="5" xml:space="preserve"> C6/MIN($B6:$F6)</f>
+        <v>9.7137126185266283</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="4"/>
-        <v>53.945853043203897</v>
+        <f t="shared" si="5"/>
+        <v>43.656701000789333</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="4"/>
-        <v>2.6199974790445575</v>
+        <f t="shared" si="5"/>
+        <v>2.5896423433702087</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -8218,24 +8223,24 @@
         <v>17</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" ref="B17:F17" si="5" xml:space="preserve"> B7/MIN($B7:$F7)</f>
-        <v>547.95564980510312</v>
+        <f t="shared" si="1"/>
+        <v>604.30986250033095</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="5"/>
-        <v>6.9350664767331454</v>
+        <f t="shared" ref="B17:F17" si="6" xml:space="preserve"> C7/MIN($B7:$F7)</f>
+        <v>8.1263985730500981</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="5"/>
-        <v>28.921411358911392</v>
+        <f t="shared" si="6"/>
+        <v>27.527834049104669</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="5"/>
-        <v>2.2402980877390335</v>
+        <f t="shared" si="6"/>
+        <v>2.7214447195607736</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -8243,24 +8248,24 @@
         <v>18</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" ref="B18:F18" si="6" xml:space="preserve"> B8/MIN($B8:$F8)</f>
-        <v>390.83244743680405</v>
-      </c>
-      <c r="C18" s="3">
-        <f t="shared" si="6"/>
-        <v>6.4506618531889135</v>
-      </c>
-      <c r="D18" s="3">
-        <f t="shared" si="6"/>
-        <v>28.023620149433629</v>
-      </c>
-      <c r="E18" s="3">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="F18" s="3">
-        <f t="shared" si="6"/>
-        <v>2.1478045763760063</v>
+        <f t="shared" si="1"/>
+        <v>9999.99</v>
+      </c>
+      <c r="C18" s="3" t="e">
+        <f t="shared" ref="B18:F18" si="7" xml:space="preserve"> C8/MIN($B8:$F8)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D18" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E18" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F18" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -8268,23 +8273,23 @@
         <v>11</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" ref="B19:F19" si="7" xml:space="preserve"> B9/MIN($B9:$F9)</f>
-        <v>400.43040780141746</v>
-      </c>
-      <c r="C19" s="3">
-        <f t="shared" si="7"/>
-        <v>13.288651004168278</v>
+        <f t="shared" si="1"/>
+        <v>9999.99</v>
+      </c>
+      <c r="C19" s="3" t="e">
+        <f t="shared" ref="B19:F19" si="8" xml:space="preserve"> C9/MIN($B9:$F9)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D19" s="3" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E19" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
+      <c r="E19" s="3" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
       </c>
       <c r="F19" s="3" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Complement #257 - prepare next benchmrk
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B21714-3332-4BB0-BA06-682659F8105B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB59B0F-A062-4BC3-BD47-ABB26641B1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
   <sheets>
     <sheet name="is" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="25">
   <si>
     <t>Components</t>
   </si>
@@ -341,28 +341,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1716.3710909901233</c:v>
+                  <c:v>1783.0047956673916</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1712.0344564644208</c:v>
+                  <c:v>1731.489894307435</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>218.11394055275514</c:v>
+                  <c:v>1001.5800577932603</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9999.99</c:v>
+                  <c:v>947.77617797030143</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>752.48554641332726</c:v>
+                  <c:v>1967.8209887888288</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>910.91728527242594</c:v>
+                  <c:v>927.17780214425011</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9999.99</c:v>
+                  <c:v>843.15395306858841</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9999.99</c:v>
+                  <c:v>1541.7506384531175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -436,22 +436,22 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2958.275825332566</c:v>
+                  <c:v>2754.0771315573656</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2175.6998457331215</c:v>
+                  <c:v>2099.18831168831</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>370.88554491563849</c:v>
+                  <c:v>759.01963109269548</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>708.73286132302189</c:v>
+                  <c:v>1894.3512730447903</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>703.83583149644937</c:v>
+                  <c:v>677.86179279941291</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -531,22 +531,22 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>634.98618008104415</c:v>
+                  <c:v>662.67459316639543</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>855.002938990144</c:v>
+                  <c:v>922.90893916913751</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>202.64369855207511</c:v>
+                  <c:v>417.88113110080889</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>232.47100123663625</c:v>
+                  <c:v>636.38403767304044</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>281.49277258567065</c:v>
+                  <c:v>250.18360128617391</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -626,22 +626,22 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>134.4488632058609</c:v>
+                  <c:v>129.62210518857898</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>112.24391976238661</c:v>
+                  <c:v>104.52103441995976</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.513577794225156</c:v>
+                  <c:v>206.40249309584775</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51.827842724448971</c:v>
+                  <c:v>142.1766887336033</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>130.41386815920433</c:v>
+                  <c:v>126.55968447648989</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -667,7 +667,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>class-validator</c:v>
+                  <c:v>zod</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -721,28 +721,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5.8542376143570616</c:v>
+                  <c:v>5.9989255461205744</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8502706552706571</c:v>
+                  <c:v>1.7877147124719925</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2.04975118048797</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.2028466545053254</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2.6652733253713872</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -762,7 +762,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>zod</c:v>
+                  <c:v>class-validator</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -822,19 +822,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2.8058311245740275</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.6844251463092288</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1216,28 +1216,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>332.746842533684</c:v>
+                  <c:v>343.57413114224778</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>666.89171571387453</c:v>
+                  <c:v>657.84713118886725</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>259.84801423535163</c:v>
+                  <c:v>268.21677787688088</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9999.99</c:v>
+                  <c:v>298.8662001479222</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>417.23237169935095</c:v>
+                  <c:v>447.0000000000008</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>736.17855836077445</c:v>
+                  <c:v>684.19366305080507</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9999.99</c:v>
+                  <c:v>669.92341678939908</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9999.99</c:v>
+                  <c:v>638.94917106941091</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1311,22 +1311,22 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>14.325122893734195</c:v>
+                  <c:v>12.026843582007581</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.4259909444211445</c:v>
+                  <c:v>8.5389014062621271</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.660050441670224</c:v>
+                  <c:v>9.098433350592078</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.5644662503716908</c:v>
+                  <c:v>10.57552822453485</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.5110705016155661</c:v>
+                  <c:v>7.0719471947194732</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1406,22 +1406,22 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>58.556035850635247</c:v>
+                  <c:v>53.374574410888954</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37.959376386982719</c:v>
+                  <c:v>41.670140785915777</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65.91523224830145</c:v>
+                  <c:v>63.734675183204246</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.019297598477905</c:v>
+                  <c:v>49.630353817504599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29.314369995785984</c:v>
+                  <c:v>27.927183183183192</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1501,28 +1501,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.3728307942069069</c:v>
+                  <c:v>6.1890675160989321</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8198606371180286</c:v>
+                  <c:v>1.8028449930053263</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9347346840741886</c:v>
+                  <c:v>2.0020655343530995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.3455473066178698</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5721183040825109</c:v>
+                  <c:v>2.6641509433962325</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1605,16 +1605,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.768639885374657</c:v>
+                  <c:v>2.6319349962207097</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.7914399709829634</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1695,7 +1695,7 @@
         <c:axId val="381772640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="800"/>
+          <c:max val="700"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1995,28 +1995,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>268.23526420622443</c:v>
+                  <c:v>272.96321534783755</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>371.20787873711248</c:v>
+                  <c:v>390.4314891964388</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>212.96363282186502</c:v>
+                  <c:v>212.18205509742634</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9999.99</c:v>
+                  <c:v>214.98398307645883</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>244.90415776912485</c:v>
+                  <c:v>249.23540583098767</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>604.30986250033095</c:v>
+                  <c:v>559.94532835024029</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9999.99</c:v>
+                  <c:v>421.32277138749134</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9999.99</c:v>
+                  <c:v>378.35975609756002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2090,22 +2090,22 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>12.487759940792849</c:v>
+                  <c:v>13.727728403401954</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.4286770773598985</c:v>
+                  <c:v>8.2699601834688128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.8534415338868087</c:v>
+                  <c:v>9.814733787767091</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.7137126185266283</c:v>
+                  <c:v>9.7860568056068082</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.1263985730500981</c:v>
+                  <c:v>7.288653555219371</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2185,22 +2185,22 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>53.408595188812598</c:v>
+                  <c:v>54.659801911956919</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.745393000293141</c:v>
+                  <c:v>39.744893986053413</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.381765852157386</c:v>
+                  <c:v>71.94784355374928</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.656701000789333</c:v>
+                  <c:v>44.930065946373965</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27.527834049104669</c:v>
+                  <c:v>26.906493023255834</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2280,28 +2280,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.4245749700543353</c:v>
+                  <c:v>6.6433212988161552</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8514451249447279</c:v>
+                  <c:v>1.8340897682048936</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9474428084508635</c:v>
+                  <c:v>2.0981537796903047</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.085172350902794</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5896423433702087</c:v>
+                  <c:v>2.3815545537927161</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2384,16 +2384,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.7214447195607736</c:v>
+                  <c:v>2.5866861741038769</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.6303520994163088</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2759,25 +2759,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>84474.4925946242</c:v>
+                  <c:v>95835.242771412901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65514.801712902598</c:v>
+                  <c:v>66020.511889635105</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11692.474674384899</c:v>
+                  <c:v>12671.068850149601</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11202.996528412201</c:v>
+                  <c:v>3498.8162447641598</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5208.7633532500404</c:v>
+                  <c:v>5398.1735159817299</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3656.17128463476</c:v>
+                  <c:v>3563.6396790663698</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>530.54196121080201</c:v>
+                  <c:v>532.55813953488303</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2797,7 +2797,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ajv</c:v>
+                  <c:v>typebox</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2848,25 +2848,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.3939948736726402</c:v>
+                  <c:v>183.42981186685901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.2508250825082499</c:v>
+                  <c:v>758.99612474626304</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0389205067009302</c:v>
+                  <c:v>79.673321234119697</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8426145700200802</c:v>
+                  <c:v>959.05213270142099</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.3348768290424093</c:v>
+                  <c:v>735.16988062442601</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.4246165357276404</c:v>
+                  <c:v>234.01510963699999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.73139513622234398</c:v>
+                  <c:v>11.198825041307099</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2886,7 +2886,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>typebox</c:v>
+                  <c:v>ajv</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2937,25 +2937,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>177.410666187825</c:v>
+                  <c:v>4.7050307636626796</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>760.90942427575999</c:v>
+                  <c:v>8.5232536594404298</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79.009648643728298</c:v>
+                  <c:v>4.11445670469422</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>914.52830188679195</c:v>
+                  <c:v>6.0998151571164501</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>740.86502609992499</c:v>
+                  <c:v>8.8695980373655399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>226.08854071779899</c:v>
+                  <c:v>5.8964437073889799</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.193133047210299</c:v>
+                  <c:v>0.90334236675699997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6967,14 +6967,16 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -7005,22 +7007,22 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>109269.155555555</v>
+        <v>111761.746821448</v>
       </c>
       <c r="C2" s="2">
-        <v>188332.40843507199</v>
+        <v>172630.19810815601</v>
       </c>
       <c r="D2">
-        <v>40425.059622087603</v>
+        <v>41537.560799855797</v>
       </c>
       <c r="E2">
-        <v>8559.4040968342597</v>
+        <v>8124.9321021184096</v>
       </c>
       <c r="F2">
-        <v>372.69772481040002</v>
+        <v>376.02276769832798</v>
       </c>
       <c r="G2">
-        <v>63.662896753009797</v>
+        <v>62.681686046511601</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -7028,22 +7030,22 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>66141.004261626804</v>
+        <v>69259.595772297398</v>
       </c>
       <c r="C3" s="2">
-        <v>84053.783044667201</v>
+        <v>83967.532467532394</v>
       </c>
       <c r="D3">
-        <v>33031.317108088697</v>
+        <v>36916.357566765502</v>
       </c>
       <c r="E3">
-        <v>4336.3178511471697</v>
+        <v>4180.8413767983902</v>
       </c>
       <c r="F3">
-        <v>71.481481481481396</v>
+        <v>71.508588498879703</v>
       </c>
       <c r="G3">
-        <v>38.632986627043003</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -7051,22 +7053,22 @@
         <v>15</v>
       </c>
       <c r="B4" s="2">
-        <v>7010.9508082739403</v>
+        <v>16044.460509669199</v>
       </c>
       <c r="C4" s="2">
-        <v>11921.568627450901</v>
+        <v>12158.8488133059</v>
       </c>
       <c r="D4">
-        <v>6513.6827043462699</v>
+        <v>6694.1002404290703</v>
       </c>
       <c r="E4">
-        <v>3166.5736087846599</v>
+        <v>3306.39235855988</v>
       </c>
       <c r="F4">
-        <v>32.143524574845799</v>
-      </c>
-      <c r="G4" t="s">
-        <v>4</v>
+        <v>32.835270245342102</v>
+      </c>
+      <c r="G4">
+        <v>16.019149327932201</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -7074,7 +7076,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="2">
-        <v>14108.723135271801</v>
+        <v>14551.1414704296</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
@@ -7085,11 +7087,11 @@
       <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>4</v>
+      <c r="F5">
+        <v>18.467220683287099</v>
+      </c>
+      <c r="G5">
+        <v>15.3529301628908</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -7097,22 +7099,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>6906.1232017705597</v>
+        <v>6543.6500643264098</v>
       </c>
       <c r="C6" s="2">
-        <v>6504.5720555961898</v>
+        <v>6299.3391677085101</v>
       </c>
       <c r="D6">
-        <v>2133.5604159196801</v>
+        <v>2116.1856046766502</v>
       </c>
       <c r="E6">
-        <v>475.66291318561503</v>
+        <v>472.78411180581099</v>
       </c>
       <c r="F6">
-        <v>9.1777486420677992</v>
-      </c>
-      <c r="G6" t="s">
-        <v>4</v>
+        <v>8.8629077880445006</v>
+      </c>
+      <c r="G6">
+        <v>3.3253279142804302</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -7120,22 +7122,22 @@
         <v>17</v>
       </c>
       <c r="B7" s="2">
-        <v>2573.69735902926</v>
+        <v>2627.5584795321602</v>
       </c>
       <c r="C7" s="2">
-        <v>1988.6113152093999</v>
+        <v>1921.0139603232899</v>
       </c>
       <c r="D7">
-        <v>795.32710280373794</v>
+        <v>709.00321543408302</v>
       </c>
       <c r="E7">
-        <v>368.47014925373099</v>
+        <v>358.66149010907702</v>
       </c>
       <c r="F7">
-        <v>2.8253908457336498</v>
-      </c>
-      <c r="G7" t="s">
-        <v>4</v>
+        <v>2.8339316077838599</v>
+      </c>
+      <c r="G7">
+        <v>7.9515335100340696</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -7143,7 +7145,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="2">
-        <v>1641.1124977714301</v>
+        <v>1541.6967509025201</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
@@ -7154,11 +7156,11 @@
       <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" t="s">
-        <v>4</v>
+      <c r="F8">
+        <v>1.82848784055586</v>
+      </c>
+      <c r="G8">
+        <v>4.90843873890881</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -7166,7 +7168,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="2">
-        <v>443.81223328591699</v>
+        <v>549.25209777453404</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
@@ -7177,8 +7179,8 @@
       <c r="E9" t="s">
         <v>4</v>
       </c>
-      <c r="F9" t="s">
-        <v>4</v>
+      <c r="F9">
+        <v>0.35625222657641598</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
@@ -7201,10 +7203,10 @@
         <v>19</v>
       </c>
       <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
         <v>21</v>
-      </c>
-      <c r="G11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -7213,23 +7215,23 @@
       </c>
       <c r="B12" s="3">
         <f xml:space="preserve"> IF(B2 = MIN($B2:$G2), 9999.99, B2 / MIN($B2:$G2))</f>
-        <v>1716.3710909901233</v>
+        <v>1783.0047956673916</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:G12" si="0" xml:space="preserve"> C2 / MIN($B2:$G2)</f>
-        <v>2958.275825332566</v>
+        <v>2754.0771315573656</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>634.98618008104415</v>
+        <v>662.67459316639543</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>134.4488632058609</v>
+        <v>129.62210518857898</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
-        <v>5.8542376143570616</v>
+        <v>5.9989255461205744</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="0"/>
@@ -7242,23 +7244,23 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" ref="B13:B19" si="1" xml:space="preserve"> IF(B3 = MIN($B3:$G3), 9999.99, B3 / MIN($B3:$G3))</f>
-        <v>1712.0344564644208</v>
+        <v>1731.489894307435</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" ref="B13:G13" si="2" xml:space="preserve"> C3 / MIN($B3:$G3)</f>
-        <v>2175.6998457331215</v>
+        <f t="shared" ref="C13:G13" si="2" xml:space="preserve"> C3 / MIN($B3:$G3)</f>
+        <v>2099.18831168831</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="2"/>
-        <v>855.002938990144</v>
+        <v>922.90893916913751</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="2"/>
-        <v>112.24391976238661</v>
+        <v>104.52103441995976</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="2"/>
-        <v>1.8502706552706571</v>
+        <v>1.7877147124719925</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="2"/>
@@ -7271,27 +7273,27 @@
       </c>
       <c r="B14" s="3">
         <f t="shared" si="1"/>
-        <v>218.11394055275514</v>
+        <v>1001.5800577932603</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" ref="B14:G14" si="3" xml:space="preserve"> C4 / MIN($B4:$G4)</f>
-        <v>370.88554491563849</v>
+        <f t="shared" ref="C14:G14" si="3" xml:space="preserve"> C4 / MIN($B4:$G4)</f>
+        <v>759.01963109269548</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="3"/>
-        <v>202.64369855207511</v>
+        <v>417.88113110080889</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="3"/>
-        <v>98.513577794225156</v>
+        <v>206.40249309584775</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="3"/>
+        <v>2.04975118048797</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="3"/>
         <v>1</v>
-      </c>
-      <c r="G14" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -7300,10 +7302,10 @@
       </c>
       <c r="B15" s="3">
         <f t="shared" si="1"/>
-        <v>9999.99</v>
+        <v>947.77617797030143</v>
       </c>
       <c r="C15" s="3" t="e">
-        <f t="shared" ref="B15:G15" si="4" xml:space="preserve"> C5 / MIN($B5:$G5)</f>
+        <f t="shared" ref="C15:G15" si="4" xml:space="preserve"> C5 / MIN($B5:$G5)</f>
         <v>#VALUE!</v>
       </c>
       <c r="D15" s="3" t="e">
@@ -7314,13 +7316,13 @@
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F15" s="3" t="e">
+      <c r="F15" s="3">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G15" s="3" t="e">
+        <v>1.2028466545053254</v>
+      </c>
+      <c r="G15" s="3">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -7329,27 +7331,27 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" si="1"/>
-        <v>752.48554641332726</v>
+        <v>1967.8209887888288</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" ref="B16:G16" si="5" xml:space="preserve"> C6 / MIN($B6:$G6)</f>
-        <v>708.73286132302189</v>
+        <f t="shared" ref="C16:G16" si="5" xml:space="preserve"> C6 / MIN($B6:$G6)</f>
+        <v>1894.3512730447903</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="5"/>
-        <v>232.47100123663625</v>
+        <v>636.38403767304044</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="5"/>
-        <v>51.827842724448971</v>
+        <v>142.1766887336033</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="5"/>
+        <v>2.6652733253713872</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="5"/>
         <v>1</v>
-      </c>
-      <c r="G16" s="3" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -7358,27 +7360,27 @@
       </c>
       <c r="B17" s="3">
         <f t="shared" si="1"/>
-        <v>910.91728527242594</v>
+        <v>927.17780214425011</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" ref="B17:G17" si="6" xml:space="preserve"> C7 / MIN($B7:$G7)</f>
-        <v>703.83583149644937</v>
+        <f t="shared" ref="C17:G17" si="6" xml:space="preserve"> C7 / MIN($B7:$G7)</f>
+        <v>677.86179279941291</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="6"/>
-        <v>281.49277258567065</v>
+        <v>250.18360128617391</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="6"/>
-        <v>130.41386815920433</v>
+        <v>126.55968447648989</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="G17" s="3" t="e">
+      <c r="G17" s="3">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>2.8058311245740275</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -7387,10 +7389,10 @@
       </c>
       <c r="B18" s="3">
         <f t="shared" si="1"/>
-        <v>9999.99</v>
+        <v>843.15395306858841</v>
       </c>
       <c r="C18" s="3" t="e">
-        <f t="shared" ref="B18:G18" si="7" xml:space="preserve"> C8 / MIN($B8:$G8)</f>
+        <f t="shared" ref="C18:G18" si="7" xml:space="preserve"> C8 / MIN($B8:$G8)</f>
         <v>#VALUE!</v>
       </c>
       <c r="D18" s="3" t="e">
@@ -7401,13 +7403,13 @@
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F18" s="3" t="e">
+      <c r="F18" s="3">
         <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G18" s="3" t="e">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
         <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+        <v>2.6844251463092288</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -7416,10 +7418,10 @@
       </c>
       <c r="B19" s="3">
         <f t="shared" si="1"/>
-        <v>9999.99</v>
+        <v>1541.7506384531175</v>
       </c>
       <c r="C19" s="3" t="e">
-        <f t="shared" ref="B19:G19" si="8" xml:space="preserve"> C9 / MIN($B9:$G9)</f>
+        <f t="shared" ref="C19:G19" si="8" xml:space="preserve"> C9 / MIN($B9:$G9)</f>
         <v>#VALUE!</v>
       </c>
       <c r="D19" s="3" t="e">
@@ -7430,9 +7432,9 @@
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F19" s="3" t="e">
+      <c r="F19" s="3">
         <f t="shared" si="8"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="G19" s="3" t="e">
         <f t="shared" si="8"/>
@@ -7455,8 +7457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050C2C99-5EE7-403C-9AB2-DBCB91E8248D}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7491,19 +7493,19 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>20567.3992673992</v>
+        <v>21352.768070627098</v>
       </c>
       <c r="C2">
-        <v>885.44949026876702</v>
+        <v>747.45558047265797</v>
       </c>
       <c r="D2">
-        <v>3619.4043486205001</v>
+        <v>3317.1732239418202</v>
       </c>
       <c r="E2">
-        <v>393.91074130105898</v>
+        <v>384.64398587097901</v>
       </c>
       <c r="F2">
-        <v>61.810952467016001</v>
+        <v>62.148940025366898</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7511,19 +7513,19 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>26125.910140294702</v>
+        <v>25638.297872340401</v>
       </c>
       <c r="C3">
-        <v>330.093592512599</v>
+        <v>332.78688524590098</v>
       </c>
       <c r="D3">
-        <v>1487.08288482238</v>
+        <v>1624.0117668688999</v>
       </c>
       <c r="E3">
-        <v>71.294206170052604</v>
+        <v>70.262337185837396</v>
       </c>
       <c r="F3">
-        <v>39.175640549572897</v>
+        <v>38.9730328777244</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -7531,19 +7533,19 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>4308.7667708141798</v>
+        <v>4397.8156238430201</v>
       </c>
       <c r="C4">
-        <v>143.599856579419</v>
+        <v>149.182436156531</v>
       </c>
       <c r="D4">
-        <v>1092.99800977021</v>
+        <v>1045.0254175744301</v>
       </c>
       <c r="E4">
-        <v>32.081524816002997</v>
+        <v>32.826861752016498</v>
       </c>
       <c r="F4">
-        <v>16.581872997927199</v>
+        <v>16.396497111980601</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -7551,7 +7553,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>4320.1544685546096</v>
+        <v>4364.9769585253398</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -7559,11 +7561,11 @@
       <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>4</v>
+      <c r="E5">
+        <v>19.651880965749498</v>
+      </c>
+      <c r="F5">
+        <v>14.6051208077893</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -7571,19 +7573,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1503.3975084937699</v>
+        <v>1519.5467422096301</v>
       </c>
       <c r="C6">
-        <v>34.463276836158101</v>
+        <v>35.950804162724602</v>
       </c>
       <c r="D6">
-        <v>158.613057912209</v>
+        <v>168.71508379888201</v>
       </c>
       <c r="E6">
-        <v>9.2680158880272305</v>
+        <v>9.0566037735849001</v>
       </c>
       <c r="F6">
-        <v>3.60326190024653</v>
+        <v>3.3994334277620299</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -7591,19 +7593,19 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>1926.08854738382</v>
+        <v>1915.7933443647701</v>
       </c>
       <c r="C7">
-        <v>19.651464590285499</v>
+        <v>19.801980198019798</v>
       </c>
       <c r="D7">
-        <v>76.696165191740405</v>
+        <v>78.198198198198199</v>
       </c>
       <c r="E7">
-        <v>2.6163333956269801</v>
+        <v>2.8000746686578299</v>
       </c>
       <c r="F7">
-        <v>7.2436849925705697</v>
+        <v>7.3696145124716503</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -7611,7 +7613,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>1079.67183226982</v>
+        <v>1131.62739322533</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -7619,11 +7621,11 @@
       <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" t="s">
-        <v>4</v>
+      <c r="E8">
+        <v>1.6891891891891799</v>
+      </c>
+      <c r="F8">
+        <v>4.71527022125498</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -7631,7 +7633,7 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>210.21184139054799</v>
+        <v>227.54600109309499</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -7639,8 +7641,8 @@
       <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" t="s">
-        <v>4</v>
+      <c r="E9">
+        <v>0.35612535612535601</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
@@ -7672,19 +7674,19 @@
       </c>
       <c r="B12" s="3">
         <f xml:space="preserve"> IF(B2 = MIN($B2:$F2), 9999.99, B2 / MIN($B2:$F2))</f>
-        <v>332.746842533684</v>
+        <v>343.57413114224778</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:F12" si="0" xml:space="preserve"> C2/MIN($B2:$F2)</f>
-        <v>14.325122893734195</v>
+        <v>12.026843582007581</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>58.556035850635247</v>
+        <v>53.374574410888954</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>6.3728307942069069</v>
+        <v>6.1890675160989321</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
@@ -7697,19 +7699,19 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" ref="B13:B19" si="1" xml:space="preserve"> IF(B3 = MIN($B3:$F3), 9999.99, B3 / MIN($B3:$F3))</f>
-        <v>666.89171571387453</v>
+        <v>657.84713118886725</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" ref="B13:F13" si="2" xml:space="preserve"> C3/MIN($B3:$F3)</f>
-        <v>8.4259909444211445</v>
+        <f t="shared" ref="C13:F13" si="2" xml:space="preserve"> C3/MIN($B3:$F3)</f>
+        <v>8.5389014062621271</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="2"/>
-        <v>37.959376386982719</v>
+        <v>41.670140785915777</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="2"/>
-        <v>1.8198606371180286</v>
+        <v>1.8028449930053263</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="2"/>
@@ -7722,19 +7724,19 @@
       </c>
       <c r="B14" s="3">
         <f t="shared" si="1"/>
-        <v>259.84801423535163</v>
+        <v>268.21677787688088</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" ref="B14:F14" si="3" xml:space="preserve"> C4/MIN($B4:$F4)</f>
-        <v>8.660050441670224</v>
+        <f t="shared" ref="C14:F14" si="3" xml:space="preserve"> C4/MIN($B4:$F4)</f>
+        <v>9.098433350592078</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="3"/>
-        <v>65.91523224830145</v>
+        <v>63.734675183204246</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="3"/>
-        <v>1.9347346840741886</v>
+        <v>2.0020655343530995</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="3"/>
@@ -7747,23 +7749,23 @@
       </c>
       <c r="B15" s="3">
         <f t="shared" si="1"/>
-        <v>9999.99</v>
+        <v>298.8662001479222</v>
       </c>
       <c r="C15" s="3" t="e">
-        <f t="shared" ref="B15:F15" si="4" xml:space="preserve"> C5/MIN($B5:$F5)</f>
+        <f t="shared" ref="C15:F15" si="4" xml:space="preserve"> C5/MIN($B5:$F5)</f>
         <v>#VALUE!</v>
       </c>
       <c r="D15" s="3" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E15" s="3" t="e">
+      <c r="E15" s="3">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F15" s="3" t="e">
+        <v>1.3455473066178698</v>
+      </c>
+      <c r="F15" s="3">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -7772,19 +7774,19 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" si="1"/>
-        <v>417.23237169935095</v>
+        <v>447.0000000000008</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" ref="B16:F16" si="5" xml:space="preserve"> C6/MIN($B6:$F6)</f>
-        <v>9.5644662503716908</v>
+        <f t="shared" ref="C16:F16" si="5" xml:space="preserve"> C6/MIN($B6:$F6)</f>
+        <v>10.57552822453485</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="5"/>
-        <v>44.019297598477905</v>
+        <v>49.630353817504599</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="5"/>
-        <v>2.5721183040825109</v>
+        <v>2.6641509433962325</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="5"/>
@@ -7797,15 +7799,15 @@
       </c>
       <c r="B17" s="3">
         <f t="shared" si="1"/>
-        <v>736.17855836077445</v>
+        <v>684.19366305080507</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" ref="B17:F17" si="6" xml:space="preserve"> C7/MIN($B7:$F7)</f>
-        <v>7.5110705016155661</v>
+        <f t="shared" ref="C17:F17" si="6" xml:space="preserve"> C7/MIN($B7:$F7)</f>
+        <v>7.0719471947194732</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="6"/>
-        <v>29.314369995785984</v>
+        <v>27.927183183183192</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="6"/>
@@ -7813,7 +7815,7 @@
       </c>
       <c r="F17" s="3">
         <f t="shared" si="6"/>
-        <v>2.768639885374657</v>
+        <v>2.6319349962207097</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -7822,23 +7824,23 @@
       </c>
       <c r="B18" s="3">
         <f t="shared" si="1"/>
-        <v>9999.99</v>
+        <v>669.92341678939908</v>
       </c>
       <c r="C18" s="3" t="e">
-        <f t="shared" ref="B18:F18" si="7" xml:space="preserve"> C8/MIN($B8:$F8)</f>
+        <f t="shared" ref="C18:F18" si="7" xml:space="preserve"> C8/MIN($B8:$F8)</f>
         <v>#VALUE!</v>
       </c>
       <c r="D18" s="3" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E18" s="3" t="e">
+      <c r="E18" s="3">
         <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F18" s="3" t="e">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
         <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+        <v>2.7914399709829634</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -7847,19 +7849,19 @@
       </c>
       <c r="B19" s="3">
         <f t="shared" si="1"/>
-        <v>9999.99</v>
+        <v>638.94917106941091</v>
       </c>
       <c r="C19" s="3" t="e">
-        <f t="shared" ref="B19:F19" si="8" xml:space="preserve"> C9/MIN($B9:$F9)</f>
+        <f t="shared" ref="C19:F19" si="8" xml:space="preserve"> C9/MIN($B9:$F9)</f>
         <v>#VALUE!</v>
       </c>
       <c r="D19" s="3" t="e">
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E19" s="3" t="e">
+      <c r="E19" s="3">
         <f t="shared" si="8"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="F19" s="3" t="e">
         <f t="shared" si="8"/>
@@ -7883,7 +7885,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7918,19 +7920,19 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>16749.399371650299</v>
+        <v>16432.237079869799</v>
       </c>
       <c r="C2">
-        <v>779.77248489157398</v>
+        <v>826.40178239881095</v>
       </c>
       <c r="D2">
-        <v>3334.98987667955</v>
+        <v>3290.4903417533401</v>
       </c>
       <c r="E2">
-        <v>401.16937004903798</v>
+        <v>399.92432841468002</v>
       </c>
       <c r="F2">
-        <v>62.442943217089599</v>
+        <v>60.199456029011699</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7938,19 +7940,19 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>14503.514613392501</v>
+        <v>15842.9675994108</v>
       </c>
       <c r="C3">
-        <v>329.31801334321699</v>
+        <v>335.57926258656101</v>
       </c>
       <c r="D3">
-        <v>1591.9689119170901</v>
+        <v>1612.77224067921</v>
       </c>
       <c r="E3">
-        <v>72.338069754567201</v>
+        <v>74.423876086135195</v>
       </c>
       <c r="F3">
-        <v>39.071138960560198</v>
+        <v>40.578098943857697</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -7958,19 +7960,19 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>3444.5876288659701</v>
+        <v>3373.4455010972902</v>
       </c>
       <c r="C4">
-        <v>143.20029563931999</v>
+        <v>156.04274134119299</v>
       </c>
       <c r="D4">
-        <v>1041.3450937155401</v>
+        <v>1143.8862209087499</v>
       </c>
       <c r="E4">
-        <v>31.498980915323301</v>
+        <v>33.358181140514297</v>
       </c>
       <c r="F4">
-        <v>16.174534511942799</v>
+        <v>15.898825654923201</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -7978,7 +7980,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>3097.37221022318</v>
+        <v>3251.85856754306</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -7986,11 +7988,11 @@
       <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>4</v>
+      <c r="E5">
+        <v>16.414371694327901</v>
+      </c>
+      <c r="F5">
+        <v>15.126050420167999</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -7998,19 +8000,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>873.50835322195701</v>
+        <v>892.47506799637301</v>
       </c>
       <c r="C6">
-        <v>34.646243617797197</v>
+        <v>35.0424197713021</v>
       </c>
       <c r="D6">
-        <v>155.71190520274001</v>
+        <v>160.88791047514201</v>
       </c>
       <c r="E6">
-        <v>9.2365692742695504</v>
+        <v>8.5279940674823802</v>
       </c>
       <c r="F6">
-        <v>3.5667354984043498</v>
+        <v>3.5808518658122801</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -8018,19 +8020,19 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>1589.69148346573</v>
+        <v>1583.5557928456999</v>
       </c>
       <c r="C7">
-        <v>21.377222852818701</v>
+        <v>20.612708018154301</v>
       </c>
       <c r="D7">
-        <v>72.4144450746833</v>
+        <v>76.093023255813904</v>
       </c>
       <c r="E7">
-        <v>2.6305900037579799</v>
+        <v>2.8280542986425301</v>
       </c>
       <c r="F7">
-        <v>7.1590052750565096</v>
+        <v>7.3152889539136696</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -8038,7 +8040,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>811.22819767441797</v>
+        <v>784.14809489575805</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -8046,11 +8048,11 @@
       <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" t="s">
-        <v>4</v>
+      <c r="E8">
+        <v>1.8611576400521099</v>
+      </c>
+      <c r="F8">
+        <v>4.89549990585577</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -8058,7 +8060,7 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>112.361526288025</v>
+        <v>134.14634146341399</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -8066,8 +8068,8 @@
       <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" t="s">
-        <v>4</v>
+      <c r="E9">
+        <v>0.354547066123027</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
@@ -8099,19 +8101,19 @@
       </c>
       <c r="B12" s="3">
         <f xml:space="preserve"> IF(B2 = MIN($B2:$F2), 9999.99, B2 / MIN($B2:$F2))</f>
-        <v>268.23526420622443</v>
+        <v>272.96321534783755</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:F12" si="0" xml:space="preserve"> C2/MIN($B2:$F2)</f>
-        <v>12.487759940792849</v>
+        <v>13.727728403401954</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>53.408595188812598</v>
+        <v>54.659801911956919</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>6.4245749700543353</v>
+        <v>6.6433212988161552</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
@@ -8124,19 +8126,19 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" ref="B13:B19" si="1" xml:space="preserve"> IF(B3 = MIN($B3:$F3), 9999.99, B3 / MIN($B3:$F3))</f>
-        <v>371.20787873711248</v>
+        <v>390.4314891964388</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" ref="B13:F13" si="2" xml:space="preserve"> C3/MIN($B3:$F3)</f>
-        <v>8.4286770773598985</v>
+        <f t="shared" ref="C13:F13" si="2" xml:space="preserve"> C3/MIN($B3:$F3)</f>
+        <v>8.2699601834688128</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="2"/>
-        <v>40.745393000293141</v>
+        <v>39.744893986053413</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="2"/>
-        <v>1.8514451249447279</v>
+        <v>1.8340897682048936</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="2"/>
@@ -8149,19 +8151,19 @@
       </c>
       <c r="B14" s="3">
         <f t="shared" si="1"/>
-        <v>212.96363282186502</v>
+        <v>212.18205509742634</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" ref="B14:F14" si="3" xml:space="preserve"> C4/MIN($B4:$F4)</f>
-        <v>8.8534415338868087</v>
+        <f t="shared" ref="C14:F14" si="3" xml:space="preserve"> C4/MIN($B4:$F4)</f>
+        <v>9.814733787767091</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="3"/>
-        <v>64.381765852157386</v>
+        <v>71.94784355374928</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="3"/>
-        <v>1.9474428084508635</v>
+        <v>2.0981537796903047</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="3"/>
@@ -8174,23 +8176,23 @@
       </c>
       <c r="B15" s="3">
         <f t="shared" si="1"/>
-        <v>9999.99</v>
+        <v>214.98398307645883</v>
       </c>
       <c r="C15" s="3" t="e">
-        <f t="shared" ref="B15:F15" si="4" xml:space="preserve"> C5/MIN($B5:$F5)</f>
+        <f t="shared" ref="C15:F15" si="4" xml:space="preserve"> C5/MIN($B5:$F5)</f>
         <v>#VALUE!</v>
       </c>
       <c r="D15" s="3" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E15" s="3" t="e">
+      <c r="E15" s="3">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F15" s="3" t="e">
+        <v>1.085172350902794</v>
+      </c>
+      <c r="F15" s="3">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -8199,19 +8201,19 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" si="1"/>
-        <v>244.90415776912485</v>
+        <v>249.23540583098767</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" ref="B16:F16" si="5" xml:space="preserve"> C6/MIN($B6:$F6)</f>
-        <v>9.7137126185266283</v>
+        <f t="shared" ref="C16:F16" si="5" xml:space="preserve"> C6/MIN($B6:$F6)</f>
+        <v>9.7860568056068082</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="5"/>
-        <v>43.656701000789333</v>
+        <v>44.930065946373965</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="5"/>
-        <v>2.5896423433702087</v>
+        <v>2.3815545537927161</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="5"/>
@@ -8224,15 +8226,15 @@
       </c>
       <c r="B17" s="3">
         <f t="shared" si="1"/>
-        <v>604.30986250033095</v>
+        <v>559.94532835024029</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" ref="B17:F17" si="6" xml:space="preserve"> C7/MIN($B7:$F7)</f>
-        <v>8.1263985730500981</v>
+        <f t="shared" ref="C17:F17" si="6" xml:space="preserve"> C7/MIN($B7:$F7)</f>
+        <v>7.288653555219371</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="6"/>
-        <v>27.527834049104669</v>
+        <v>26.906493023255834</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="6"/>
@@ -8240,7 +8242,7 @@
       </c>
       <c r="F17" s="3">
         <f t="shared" si="6"/>
-        <v>2.7214447195607736</v>
+        <v>2.5866861741038769</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -8249,23 +8251,23 @@
       </c>
       <c r="B18" s="3">
         <f t="shared" si="1"/>
-        <v>9999.99</v>
+        <v>421.32277138749134</v>
       </c>
       <c r="C18" s="3" t="e">
-        <f t="shared" ref="B18:F18" si="7" xml:space="preserve"> C8/MIN($B8:$F8)</f>
+        <f t="shared" ref="C18:F18" si="7" xml:space="preserve"> C8/MIN($B8:$F8)</f>
         <v>#VALUE!</v>
       </c>
       <c r="D18" s="3" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E18" s="3" t="e">
+      <c r="E18" s="3">
         <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F18" s="3" t="e">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
         <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+        <v>2.6303520994163088</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -8274,19 +8276,19 @@
       </c>
       <c r="B19" s="3">
         <f t="shared" si="1"/>
-        <v>9999.99</v>
+        <v>378.35975609756002</v>
       </c>
       <c r="C19" s="3" t="e">
-        <f t="shared" ref="B19:F19" si="8" xml:space="preserve"> C9/MIN($B9:$F9)</f>
+        <f t="shared" ref="C19:F19" si="8" xml:space="preserve"> C9/MIN($B9:$F9)</f>
         <v>#VALUE!</v>
       </c>
       <c r="D19" s="3" t="e">
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E19" s="3" t="e">
+      <c r="E19" s="3">
         <f t="shared" si="8"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="F19" s="3" t="e">
         <f t="shared" si="8"/>
@@ -8305,7 +8307,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8325,10 +8327,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -8336,13 +8338,13 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>84474.4925946242</v>
+        <v>95835.242771412901</v>
       </c>
       <c r="C2">
-        <v>4.3939948736726402</v>
+        <v>183.42981186685901</v>
       </c>
       <c r="D2">
-        <v>177.410666187825</v>
+        <v>4.7050307636626796</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -8350,13 +8352,13 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>65514.801712902598</v>
+        <v>66020.511889635105</v>
       </c>
       <c r="C3">
-        <v>8.2508250825082499</v>
+        <v>758.99612474626304</v>
       </c>
       <c r="D3">
-        <v>760.90942427575999</v>
+        <v>8.5232536594404298</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -8364,13 +8366,13 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>11692.474674384899</v>
+        <v>12671.068850149601</v>
       </c>
       <c r="C4">
-        <v>4.0389205067009302</v>
+        <v>79.673321234119697</v>
       </c>
       <c r="D4">
-        <v>79.009648643728298</v>
+        <v>4.11445670469422</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -8378,13 +8380,13 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>11202.996528412201</v>
+        <v>3498.8162447641598</v>
       </c>
       <c r="C5">
-        <v>5.8426145700200802</v>
+        <v>959.05213270142099</v>
       </c>
       <c r="D5">
-        <v>914.52830188679195</v>
+        <v>6.0998151571164501</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -8392,13 +8394,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5208.7633532500404</v>
+        <v>5398.1735159817299</v>
       </c>
       <c r="C6">
-        <v>8.3348768290424093</v>
+        <v>735.16988062442601</v>
       </c>
       <c r="D6">
-        <v>740.86502609992499</v>
+        <v>8.8695980373655399</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -8406,13 +8408,13 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>3656.17128463476</v>
+        <v>3563.6396790663698</v>
       </c>
       <c r="C7">
-        <v>5.4246165357276404</v>
+        <v>234.01510963699999</v>
       </c>
       <c r="D7">
-        <v>226.08854071779899</v>
+        <v>5.8964437073889799</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -8420,13 +8422,13 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>530.54196121080201</v>
+        <v>532.55813953488303</v>
       </c>
       <c r="C8">
-        <v>0.73139513622234398</v>
+        <v>11.198825041307099</v>
       </c>
       <c r="D8">
-        <v>10.193133047210299</v>
+        <v>0.90334236675699997</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -8437,10 +8439,10 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
         <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -8449,15 +8451,15 @@
       </c>
       <c r="B12" s="1">
         <f xml:space="preserve"> B2 / MIN($B2:$E2)</f>
-        <v>19224.986606326587</v>
+        <v>20368.675059801091</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" ref="C12:D12" si="0" xml:space="preserve"> C2 / MIN($B2:$E2)</f>
-        <v>1</v>
+        <v>38.9858900144717</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>40.375710779912573</v>
+        <v>1</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -8467,15 +8469,15 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" ref="B13:D18" si="1" xml:space="preserve"> B3 / MIN($B3:$E3)</f>
-        <v>7940.3939676037953</v>
+        <v>7745.9283188774061</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>89.050045331643076</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>92.222222222222115</v>
+        <v>1</v>
       </c>
       <c r="E13" s="1"/>
     </row>
@@ -8485,15 +8487,15 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" si="1"/>
-        <v>2894.950434153393</v>
+        <v>3079.6456882613606</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>19.364238574492642</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="1"/>
-        <v>19.562070734654032</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -8503,15 +8505,15 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" si="1"/>
-        <v>1917.4628745660521</v>
+        <v>573.59381467194271</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>157.22642539135418</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>156.52723466981135</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1"/>
     </row>
@@ -8521,15 +8523,15 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" si="1"/>
-        <v>624.93585209326636</v>
+        <v>608.61535023802526</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>82.886493562315607</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="1"/>
-        <v>88.8873394647444</v>
+        <v>1</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -8539,15 +8541,15 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" si="1"/>
-        <v>673.99626509163625</v>
+        <v>604.37101682166224</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>39.687499999999979</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="1"/>
-        <v>41.678253057839825</v>
+        <v>1</v>
       </c>
       <c r="E17" s="1"/>
     </row>
@@ -8557,15 +8559,15 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" si="1"/>
-        <v>725.38349646546919</v>
+        <v>589.54186046511609</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>12.397099320726971</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="1"/>
-        <v>13.936561158798284</v>
+        <v>1</v>
       </c>
       <c r="E18" s="1"/>
     </row>
@@ -8585,9 +8587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EFA07C-E270-4B85-8B26-6FA6BD53AA2B}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Complement #257 - more benchmarks
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB59B0F-A062-4BC3-BD47-ABB26641B1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4B2CF7-1C99-463E-B365-3F82A6310BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
   <sheets>
     <sheet name="is" sheetId="2" r:id="rId1"/>
@@ -341,28 +341,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1783.0047956673916</c:v>
+                  <c:v>1764.5191293299706</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1731.489894307435</c:v>
+                  <c:v>1944.1519364144128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1001.5800577932603</c:v>
+                  <c:v>758.18277222341987</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>947.77617797030143</c:v>
+                  <c:v>883.68582976315463</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1967.8209887888288</c:v>
+                  <c:v>2089.6837638376387</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>927.17780214425011</c:v>
+                  <c:v>857.94955012853325</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>843.15395306858841</c:v>
+                  <c:v>848.18670541227914</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1541.7506384531175</c:v>
+                  <c:v>1704.3474314757707</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -436,22 +436,22 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2754.0771315573656</c:v>
+                  <c:v>2860.3210852941093</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2099.18831168831</c:v>
+                  <c:v>1974.7179487179505</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>759.01963109269548</c:v>
+                  <c:v>798.72524728518533</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1894.3512730447903</c:v>
+                  <c:v>1979.4544955136416</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>677.86179279941291</c:v>
+                  <c:v>611.42307692307509</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -531,22 +531,22 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>662.67459316639543</c:v>
+                  <c:v>800.45346006214595</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>922.90893916913751</c:v>
+                  <c:v>889.92322222222299</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>417.88113110080889</c:v>
+                  <c:v>491.81215704459623</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>636.38403767304044</c:v>
+                  <c:v>573.46513312805575</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>250.18360128617391</c:v>
+                  <c:v>260.70581514022001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -626,22 +626,22 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>129.62210518857898</c:v>
+                  <c:v>130.8583237815331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>104.52103441995976</c:v>
+                  <c:v>108.9934610612809</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>206.40249309584775</c:v>
+                  <c:v>185.96576107182801</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>142.1766887336033</c:v>
+                  <c:v>138.98787535410753</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>126.55968447648989</c:v>
+                  <c:v>128.63532618957703</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -721,19 +721,19 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5.9989255461205744</c:v>
+                  <c:v>6.1104979905224663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7877147124719925</c:v>
+                  <c:v>1.6864145743408927</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.04975118048797</c:v>
+                  <c:v>2.0648768017189139</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2028466545053254</c:v>
+                  <c:v>1.1486275067557974</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6652733253713872</c:v>
+                  <c:v>2.5900776368112091</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -831,10 +831,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.8058311245740275</c:v>
+                  <c:v>2.8652670678954304</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.6844251463092288</c:v>
+                  <c:v>2.5930168113800187</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1995,28 +1995,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>272.96321534783755</c:v>
+                  <c:v>283.13403818299639</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>390.4314891964388</c:v>
+                  <c:v>495.29232917566679</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>212.18205509742634</c:v>
+                  <c:v>252.54024391833602</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>214.98398307645883</c:v>
+                  <c:v>248.39834536173248</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>249.23540583098767</c:v>
+                  <c:v>307.16142875173443</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>559.94532835024029</c:v>
+                  <c:v>631.4905683792515</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>421.32277138749134</c:v>
+                  <c:v>461.83902171929259</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>378.35975609756002</c:v>
+                  <c:v>392.13524379811719</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2090,22 +2090,22 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>13.727728403401954</c:v>
+                  <c:v>16.02803810574073</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.2699601834688128</c:v>
+                  <c:v>9.9918866527901002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.814733787767091</c:v>
+                  <c:v>10.794444681314225</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.7860568056068082</c:v>
+                  <c:v>11.408586589483866</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.288653555219371</c:v>
+                  <c:v>7.9052287581699545</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2185,22 +2185,22 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>54.659801911956919</c:v>
+                  <c:v>64.466407051013007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39.744893986053413</c:v>
+                  <c:v>47.718226239708493</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.94784355374928</c:v>
+                  <c:v>77.129251504638702</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.930065946373965</c:v>
+                  <c:v>50.002449179524881</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.906493023255834</c:v>
+                  <c:v>30.278356371899314</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2280,19 +2280,19 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.6433212988161552</c:v>
+                  <c:v>7.3326517140362739</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8340897682048936</c:v>
+                  <c:v>1.9245696850218221</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0981537796903047</c:v>
+                  <c:v>2.258986283735406</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.085172350902794</c:v>
+                  <c:v>1.2966796032772736</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3815545537927161</c:v>
+                  <c:v>2.6641438032166569</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -2390,10 +2390,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5866861741038769</c:v>
+                  <c:v>2.4437422552664221</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.6303520994163088</c:v>
+                  <c:v>2.2734845667534413</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -6967,7 +6967,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7007,22 +7007,22 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>111761.746821448</v>
+        <v>121233.908665947</v>
       </c>
       <c r="C2" s="2">
-        <v>172630.19810815601</v>
+        <v>196522.61029411701</v>
       </c>
       <c r="D2">
-        <v>41537.560799855797</v>
+        <v>54996.3443611771</v>
       </c>
       <c r="E2">
-        <v>8124.9321021184096</v>
+        <v>8990.8155767817698</v>
       </c>
       <c r="F2">
-        <v>376.02276769832798</v>
+        <v>419.83084398056502</v>
       </c>
       <c r="G2">
-        <v>62.681686046511601</v>
+        <v>68.706485892268205</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -7030,22 +7030,22 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>69259.595772297398</v>
+        <v>84733.014177867793</v>
       </c>
       <c r="C3" s="2">
-        <v>83967.532467532394</v>
+        <v>86065.189048239903</v>
       </c>
       <c r="D3">
-        <v>36916.357566765502</v>
+        <v>38786</v>
       </c>
       <c r="E3">
-        <v>4180.8413767983902</v>
+        <v>4750.32033681127</v>
       </c>
       <c r="F3">
-        <v>71.508588498879703</v>
+        <v>73.499908809046104</v>
       </c>
       <c r="G3">
-        <v>40</v>
+        <v>43.583535108958799</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -7053,22 +7053,22 @@
         <v>15</v>
       </c>
       <c r="B4" s="2">
-        <v>16044.460509669199</v>
+        <v>13463.058572191499</v>
       </c>
       <c r="C4" s="2">
-        <v>12158.8488133059</v>
+        <v>14182.9716807649</v>
       </c>
       <c r="D4">
-        <v>6694.1002404290703</v>
+        <v>8733.1130690161499</v>
       </c>
       <c r="E4">
-        <v>3306.39235855988</v>
+        <v>3302.1957573502</v>
       </c>
       <c r="F4">
-        <v>32.835270245342102</v>
+        <v>36.666036666036597</v>
       </c>
       <c r="G4">
-        <v>16.019149327932201</v>
+        <v>17.757009345794302</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -7076,7 +7076,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="2">
-        <v>14551.1414704296</v>
+        <v>14607.7338129496</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
@@ -7088,10 +7088,10 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>18.467220683287099</v>
+        <v>18.9873417721519</v>
       </c>
       <c r="G5">
-        <v>15.3529301628908</v>
+        <v>16.530460624071299</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -7099,22 +7099,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>6543.6500643264098</v>
+        <v>7791.5129151291503</v>
       </c>
       <c r="C6" s="2">
-        <v>6299.3391677085101</v>
+        <v>7380.51638893975</v>
       </c>
       <c r="D6">
-        <v>2116.1856046766502</v>
+        <v>2138.19960152146</v>
       </c>
       <c r="E6">
-        <v>472.78411180581099</v>
+        <v>518.22474032105697</v>
       </c>
       <c r="F6">
-        <v>8.8629077880445006</v>
+        <v>9.6572618822192702</v>
       </c>
       <c r="G6">
-        <v>3.3253279142804302</v>
+        <v>3.72856077554064</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -7122,22 +7122,22 @@
         <v>17</v>
       </c>
       <c r="B7" s="2">
-        <v>2627.5584795321602</v>
+        <v>2590.5251560778502</v>
       </c>
       <c r="C7" s="2">
-        <v>1921.0139603232899</v>
+        <v>1846.15384615384</v>
       </c>
       <c r="D7">
-        <v>709.00321543408302</v>
+        <v>787.18494852680101</v>
       </c>
       <c r="E7">
-        <v>358.66149010907702</v>
+        <v>388.40634441087599</v>
       </c>
       <c r="F7">
-        <v>2.8339316077838599</v>
+        <v>3.0194376297414598</v>
       </c>
       <c r="G7">
-        <v>7.9515335100340696</v>
+        <v>8.6514952040624404</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -7145,7 +7145,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="2">
-        <v>1541.6967509025201</v>
+        <v>1752.4518706865199</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
@@ -7157,10 +7157,10 @@
         <v>4</v>
       </c>
       <c r="F8">
-        <v>1.82848784055586</v>
+        <v>2.0661157024793302</v>
       </c>
       <c r="G8">
-        <v>4.90843873890881</v>
+        <v>5.3574727507851403</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -7168,7 +7168,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="2">
-        <v>549.25209777453404</v>
+        <v>612.63387184606995</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
@@ -7180,7 +7180,7 @@
         <v>4</v>
       </c>
       <c r="F9">
-        <v>0.35625222657641598</v>
+        <v>0.35945363048166701</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
@@ -7215,23 +7215,23 @@
       </c>
       <c r="B12" s="3">
         <f xml:space="preserve"> IF(B2 = MIN($B2:$G2), 9999.99, B2 / MIN($B2:$G2))</f>
-        <v>1783.0047956673916</v>
+        <v>1764.5191293299706</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:G12" si="0" xml:space="preserve"> C2 / MIN($B2:$G2)</f>
-        <v>2754.0771315573656</v>
+        <v>2860.3210852941093</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>662.67459316639543</v>
+        <v>800.45346006214595</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>129.62210518857898</v>
+        <v>130.8583237815331</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
-        <v>5.9989255461205744</v>
+        <v>6.1104979905224663</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="0"/>
@@ -7244,23 +7244,23 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" ref="B13:B19" si="1" xml:space="preserve"> IF(B3 = MIN($B3:$G3), 9999.99, B3 / MIN($B3:$G3))</f>
-        <v>1731.489894307435</v>
+        <v>1944.1519364144128</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" ref="C13:G13" si="2" xml:space="preserve"> C3 / MIN($B3:$G3)</f>
-        <v>2099.18831168831</v>
+        <v>1974.7179487179505</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="2"/>
-        <v>922.90893916913751</v>
+        <v>889.92322222222299</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="2"/>
-        <v>104.52103441995976</v>
+        <v>108.9934610612809</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="2"/>
-        <v>1.7877147124719925</v>
+        <v>1.6864145743408927</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="2"/>
@@ -7273,23 +7273,23 @@
       </c>
       <c r="B14" s="3">
         <f t="shared" si="1"/>
-        <v>1001.5800577932603</v>
+        <v>758.18277222341987</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" ref="C14:G14" si="3" xml:space="preserve"> C4 / MIN($B4:$G4)</f>
-        <v>759.01963109269548</v>
+        <v>798.72524728518533</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="3"/>
-        <v>417.88113110080889</v>
+        <v>491.81215704459623</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="3"/>
-        <v>206.40249309584775</v>
+        <v>185.96576107182801</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="3"/>
-        <v>2.04975118048797</v>
+        <v>2.0648768017189139</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="3"/>
@@ -7302,7 +7302,7 @@
       </c>
       <c r="B15" s="3">
         <f t="shared" si="1"/>
-        <v>947.77617797030143</v>
+        <v>883.68582976315463</v>
       </c>
       <c r="C15" s="3" t="e">
         <f t="shared" ref="C15:G15" si="4" xml:space="preserve"> C5 / MIN($B5:$G5)</f>
@@ -7318,7 +7318,7 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" si="4"/>
-        <v>1.2028466545053254</v>
+        <v>1.1486275067557974</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="4"/>
@@ -7331,23 +7331,23 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" si="1"/>
-        <v>1967.8209887888288</v>
+        <v>2089.6837638376387</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" ref="C16:G16" si="5" xml:space="preserve"> C6 / MIN($B6:$G6)</f>
-        <v>1894.3512730447903</v>
+        <v>1979.4544955136416</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="5"/>
-        <v>636.38403767304044</v>
+        <v>573.46513312805575</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="5"/>
-        <v>142.1766887336033</v>
+        <v>138.98787535410753</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="5"/>
-        <v>2.6652733253713872</v>
+        <v>2.5900776368112091</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="5"/>
@@ -7360,19 +7360,19 @@
       </c>
       <c r="B17" s="3">
         <f t="shared" si="1"/>
-        <v>927.17780214425011</v>
+        <v>857.94955012853325</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" ref="C17:G17" si="6" xml:space="preserve"> C7 / MIN($B7:$G7)</f>
-        <v>677.86179279941291</v>
+        <v>611.42307692307509</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="6"/>
-        <v>250.18360128617391</v>
+        <v>260.70581514022001</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="6"/>
-        <v>126.55968447648989</v>
+        <v>128.63532618957703</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="6"/>
@@ -7380,7 +7380,7 @@
       </c>
       <c r="G17" s="3">
         <f t="shared" si="6"/>
-        <v>2.8058311245740275</v>
+        <v>2.8652670678954304</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -7389,7 +7389,7 @@
       </c>
       <c r="B18" s="3">
         <f t="shared" si="1"/>
-        <v>843.15395306858841</v>
+        <v>848.18670541227914</v>
       </c>
       <c r="C18" s="3" t="e">
         <f t="shared" ref="C18:G18" si="7" xml:space="preserve"> C8 / MIN($B8:$G8)</f>
@@ -7409,7 +7409,7 @@
       </c>
       <c r="G18" s="3">
         <f t="shared" si="7"/>
-        <v>2.6844251463092288</v>
+        <v>2.5930168113800187</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -7418,7 +7418,7 @@
       </c>
       <c r="B19" s="3">
         <f t="shared" si="1"/>
-        <v>1541.7506384531175</v>
+        <v>1704.3474314757707</v>
       </c>
       <c r="C19" s="3" t="e">
         <f t="shared" ref="C19:G19" si="8" xml:space="preserve"> C9 / MIN($B9:$G9)</f>
@@ -7884,8 +7884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4DC42C-376D-41DF-9AD8-63D3F4858048}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7920,19 +7920,19 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>16432.237079869799</v>
+        <v>16285.3127196064</v>
       </c>
       <c r="C2">
-        <v>826.40178239881095</v>
+        <v>921.90121155638303</v>
       </c>
       <c r="D2">
-        <v>3290.4903417533401</v>
+        <v>3707.9808753218099</v>
       </c>
       <c r="E2">
-        <v>399.92432841468002</v>
+        <v>421.759697256386</v>
       </c>
       <c r="F2">
-        <v>60.199456029011699</v>
+        <v>57.518032180506701</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7940,19 +7940,19 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>15842.9675994108</v>
+        <v>17822.3125230882</v>
       </c>
       <c r="C3">
-        <v>335.57926258656101</v>
+        <v>359.54226651901001</v>
       </c>
       <c r="D3">
-        <v>1612.77224067921</v>
+        <v>1717.06503613118</v>
       </c>
       <c r="E3">
-        <v>74.423876086135195</v>
+        <v>69.252601702932793</v>
       </c>
       <c r="F3">
-        <v>40.578098943857697</v>
+        <v>35.983421250941902</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -7960,19 +7960,19 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>3373.4455010972902</v>
+        <v>3869.4554633970401</v>
       </c>
       <c r="C4">
-        <v>156.04274134119299</v>
+        <v>165.39392810579201</v>
       </c>
       <c r="D4">
-        <v>1143.8862209087499</v>
+        <v>1181.7847286108499</v>
       </c>
       <c r="E4">
-        <v>33.358181140514297</v>
+        <v>34.612490594431897</v>
       </c>
       <c r="F4">
-        <v>15.898825654923201</v>
+        <v>15.322134022521601</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -7980,7 +7980,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>3251.85856754306</v>
+        <v>3434.0785073050502</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -7989,10 +7989,10 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>16.414371694327901</v>
+        <v>17.926446128257201</v>
       </c>
       <c r="F5">
-        <v>15.126050420167999</v>
+        <v>13.824884792626699</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -8000,19 +8000,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>892.47506799637301</v>
+        <v>1047.14123438091</v>
       </c>
       <c r="C6">
-        <v>35.0424197713021</v>
+        <v>38.892908827785803</v>
       </c>
       <c r="D6">
-        <v>160.88791047514201</v>
+        <v>170.46289493019799</v>
       </c>
       <c r="E6">
-        <v>8.5279940674823802</v>
+        <v>9.0823084200567603</v>
       </c>
       <c r="F6">
-        <v>3.5808518658122801</v>
+        <v>3.4090909090908998</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -8020,19 +8020,19 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>1583.5557928456999</v>
+        <v>1777.1779597915099</v>
       </c>
       <c r="C7">
-        <v>20.612708018154301</v>
+        <v>22.247360482654599</v>
       </c>
       <c r="D7">
-        <v>76.093023255813904</v>
+        <v>85.211134254875901</v>
       </c>
       <c r="E7">
-        <v>2.8280542986425301</v>
+        <v>2.8142589118198802</v>
       </c>
       <c r="F7">
-        <v>7.3152889539136696</v>
+        <v>6.8773234200743403</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -8040,7 +8040,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>784.14809489575805</v>
+        <v>868.77167366307697</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -8049,10 +8049,10 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <v>1.8611576400521099</v>
+        <v>1.8811136192625999</v>
       </c>
       <c r="F8">
-        <v>4.89549990585577</v>
+        <v>4.2766827817032302</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -8060,7 +8060,7 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>134.14634146341399</v>
+        <v>141.48845166809201</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -8069,7 +8069,7 @@
         <v>4</v>
       </c>
       <c r="E9">
-        <v>0.354547066123027</v>
+        <v>0.36081544290095602</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
@@ -8101,19 +8101,19 @@
       </c>
       <c r="B12" s="3">
         <f xml:space="preserve"> IF(B2 = MIN($B2:$F2), 9999.99, B2 / MIN($B2:$F2))</f>
-        <v>272.96321534783755</v>
+        <v>283.13403818299639</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ref="C12:F12" si="0" xml:space="preserve"> C2/MIN($B2:$F2)</f>
-        <v>13.727728403401954</v>
+        <v>16.02803810574073</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>54.659801911956919</v>
+        <v>64.466407051013007</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>6.6433212988161552</v>
+        <v>7.3326517140362739</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
@@ -8126,19 +8126,19 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" ref="B13:B19" si="1" xml:space="preserve"> IF(B3 = MIN($B3:$F3), 9999.99, B3 / MIN($B3:$F3))</f>
-        <v>390.4314891964388</v>
+        <v>495.29232917566679</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" ref="C13:F13" si="2" xml:space="preserve"> C3/MIN($B3:$F3)</f>
-        <v>8.2699601834688128</v>
+        <v>9.9918866527901002</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="2"/>
-        <v>39.744893986053413</v>
+        <v>47.718226239708493</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="2"/>
-        <v>1.8340897682048936</v>
+        <v>1.9245696850218221</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="2"/>
@@ -8151,19 +8151,19 @@
       </c>
       <c r="B14" s="3">
         <f t="shared" si="1"/>
-        <v>212.18205509742634</v>
+        <v>252.54024391833602</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" ref="C14:F14" si="3" xml:space="preserve"> C4/MIN($B4:$F4)</f>
-        <v>9.814733787767091</v>
+        <v>10.794444681314225</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="3"/>
-        <v>71.94784355374928</v>
+        <v>77.129251504638702</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="3"/>
-        <v>2.0981537796903047</v>
+        <v>2.258986283735406</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="3"/>
@@ -8176,7 +8176,7 @@
       </c>
       <c r="B15" s="3">
         <f t="shared" si="1"/>
-        <v>214.98398307645883</v>
+        <v>248.39834536173248</v>
       </c>
       <c r="C15" s="3" t="e">
         <f t="shared" ref="C15:F15" si="4" xml:space="preserve"> C5/MIN($B5:$F5)</f>
@@ -8188,7 +8188,7 @@
       </c>
       <c r="E15" s="3">
         <f t="shared" si="4"/>
-        <v>1.085172350902794</v>
+        <v>1.2966796032772736</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="4"/>
@@ -8201,19 +8201,19 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" si="1"/>
-        <v>249.23540583098767</v>
+        <v>307.16142875173443</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" ref="C16:F16" si="5" xml:space="preserve"> C6/MIN($B6:$F6)</f>
-        <v>9.7860568056068082</v>
+        <v>11.408586589483866</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="5"/>
-        <v>44.930065946373965</v>
+        <v>50.002449179524881</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" si="5"/>
-        <v>2.3815545537927161</v>
+        <v>2.6641438032166569</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="5"/>
@@ -8226,15 +8226,15 @@
       </c>
       <c r="B17" s="3">
         <f t="shared" si="1"/>
-        <v>559.94532835024029</v>
+        <v>631.4905683792515</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" ref="C17:F17" si="6" xml:space="preserve"> C7/MIN($B7:$F7)</f>
-        <v>7.288653555219371</v>
+        <v>7.9052287581699545</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="6"/>
-        <v>26.906493023255834</v>
+        <v>30.278356371899314</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="6"/>
@@ -8242,7 +8242,7 @@
       </c>
       <c r="F17" s="3">
         <f t="shared" si="6"/>
-        <v>2.5866861741038769</v>
+        <v>2.4437422552664221</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -8251,7 +8251,7 @@
       </c>
       <c r="B18" s="3">
         <f t="shared" si="1"/>
-        <v>421.32277138749134</v>
+        <v>461.83902171929259</v>
       </c>
       <c r="C18" s="3" t="e">
         <f t="shared" ref="C18:F18" si="7" xml:space="preserve"> C8/MIN($B8:$F8)</f>
@@ -8267,7 +8267,7 @@
       </c>
       <c r="F18" s="3">
         <f t="shared" si="7"/>
-        <v>2.6303520994163088</v>
+        <v>2.2734845667534413</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -8276,7 +8276,7 @@
       </c>
       <c r="B19" s="3">
         <f t="shared" si="1"/>
-        <v>378.35975609756002</v>
+        <v>392.13524379811719</v>
       </c>
       <c r="C19" s="3" t="e">
         <f t="shared" ref="C19:F19" si="8" xml:space="preserve"> C9/MIN($B9:$F9)</f>
@@ -8587,7 +8587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EFA07C-E270-4B85-8B26-6FA6BD53AA2B}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Close #262 - `assertStringify()`
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4B2CF7-1C99-463E-B365-3F82A6310BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAACDB3-E796-4116-8E3E-A5D51F0980AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
   <sheets>
     <sheet name="is" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="26">
   <si>
     <t>Components</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>fast-json-stringify</t>
-  </si>
-  <si>
-    <t>spaces</t>
   </si>
   <si>
     <t>ultimate union</t>
@@ -112,6 +109,12 @@
   </si>
   <si>
     <t>Measured by Intel i5-1135g7</t>
+  </si>
+  <si>
+    <t>TSON.stringify()</t>
+  </si>
+  <si>
+    <t>TSON.assertStringify()</t>
   </si>
 </sst>
 </file>
@@ -3249,11 +3252,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>stringify!$B$12</c:f>
+              <c:f>stringify!$B$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>typescript-json</c:v>
+                  <c:v>TSON.stringify()</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3270,9 +3273,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>stringify!$A$13:$A$20</c:f>
+              <c:f>stringify!$A$11:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>object (simple)</c:v>
                 </c:pt>
@@ -3293,42 +3296,36 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>array (union)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ultimate union</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stringify!$B$13:$B$20</c:f>
+              <c:f>stringify!$B$11:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>36.291171455034032</c:v>
+                  <c:v>15.533323740562109</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1710636518261817</c:v>
+                  <c:v>2.9922910413184978</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0593143220054593</c:v>
+                  <c:v>3.9650337825418949</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.3011099149172027</c:v>
+                  <c:v>2.1899582452596253</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9065065155159098</c:v>
+                  <c:v>2.064059659016046</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.5954893697394583</c:v>
+                  <c:v>2.0268152296605484</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5952772446217303</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.0191555155795022</c:v>
+                  <c:v>1.1520915800428932</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,11 +3341,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>stringify!$C$12</c:f>
+              <c:f>stringify!$C$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>fast-json-stringify</c:v>
+                  <c:v>TSON.assertStringify()</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3365,9 +3362,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>stringify!$A$13:$A$20</c:f>
+              <c:f>stringify!$A$11:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>object (simple)</c:v>
                 </c:pt>
@@ -3388,42 +3385,36 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>array (union)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ultimate union</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stringify!$C$13:$C$20</c:f>
+              <c:f>stringify!$C$11:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>7.3527904002563034</c:v>
+                  <c:v>4.0938381218627367</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.9822429603856428</c:v>
+                  <c:v>2.4547127717321922</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.97958628905199219</c:v>
+                  <c:v>3.3928511662518726</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.1763133330621232</c:v>
+                  <c:v>1.6026023118120991</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.6694116330601876</c:v>
+                  <c:v>1.5371395940805841</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0140896344372718</c:v>
+                  <c:v>1.8383510203468236</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.9228509176205183</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.95512751353581637</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3435,11 +3426,100 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="3"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>stringify!$D$12</c:f>
+              <c:f>stringify!$D$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fast-json-stringify</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>stringify!$A$11:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>object (simple)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stringify!$D$11:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.1832352053140029</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8742503602361618</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.027068524080927</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9446862336287483</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6916183960391256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0390610328638483</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.88713261845729896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-10A9-46CC-8EF6-634D2185069C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stringify!$E$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3460,9 +3540,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>stringify!$A$13:$A$20</c:f>
+              <c:f>stringify!$A$11:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>object (simple)</c:v>
                 </c:pt>
@@ -3483,19 +3563,16 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>array (union)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ultimate union</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stringify!$D$13:$D$20</c:f>
+              <c:f>stringify!$E$11:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3515,9 +3592,6 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -3596,7 +3670,7 @@
         <c:axId val="555336592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="37"/>
+          <c:max val="16"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3649,8 +3723,8 @@
         <c:crossAx val="555339920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10"/>
-        <c:minorUnit val="5"/>
+        <c:majorUnit val="5"/>
+        <c:minorUnit val="2"/>
       </c:valAx>
       <c:dTable>
         <c:showHorzBorder val="1"/>
@@ -6630,16 +6704,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>550544</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>131444</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>344804</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>116204</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6987,19 +7061,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -7050,7 +7124,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2">
         <v>13463.058572191499</v>
@@ -7073,7 +7147,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
         <v>14607.7338129496</v>
@@ -7119,7 +7193,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2">
         <v>2590.5251560778502</v>
@@ -7142,7 +7216,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2">
         <v>1752.4518706865199</v>
@@ -7165,7 +7239,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>612.63387184606995</v>
@@ -7194,19 +7268,19 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
         <v>19</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>20</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -7269,7 +7343,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <f t="shared" si="1"/>
@@ -7298,7 +7372,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <f t="shared" si="1"/>
@@ -7356,7 +7430,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3">
         <f t="shared" si="1"/>
@@ -7385,7 +7459,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3">
         <f t="shared" si="1"/>
@@ -7414,7 +7488,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <f t="shared" si="1"/>
@@ -7443,7 +7517,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -7476,16 +7550,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -7530,7 +7604,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>4397.8156238430201</v>
@@ -7550,7 +7624,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>4364.9769585253398</v>
@@ -7590,7 +7664,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>1915.7933443647701</v>
@@ -7610,7 +7684,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>1131.62739322533</v>
@@ -7630,7 +7704,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>227.54600109309499</v>
@@ -7656,16 +7730,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>20</v>
-      </c>
-      <c r="F11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -7720,7 +7794,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <f t="shared" si="1"/>
@@ -7745,7 +7819,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <f t="shared" si="1"/>
@@ -7795,7 +7869,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3">
         <f t="shared" si="1"/>
@@ -7820,7 +7894,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3">
         <f t="shared" si="1"/>
@@ -7845,7 +7919,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <f t="shared" si="1"/>
@@ -7870,7 +7944,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -7884,9 +7958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4DC42C-376D-41DF-9AD8-63D3F4858048}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7903,16 +7975,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -7957,7 +8029,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>3869.4554633970401</v>
@@ -7977,7 +8049,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>3434.0785073050502</v>
@@ -8017,7 +8089,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>1777.1779597915099</v>
@@ -8037,7 +8109,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>868.77167366307697</v>
@@ -8057,7 +8129,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>141.48845166809201</v>
@@ -8083,16 +8155,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>20</v>
-      </c>
-      <c r="F11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -8147,7 +8219,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <f t="shared" si="1"/>
@@ -8172,7 +8244,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <f t="shared" si="1"/>
@@ -8222,7 +8294,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3">
         <f t="shared" si="1"/>
@@ -8247,7 +8319,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3">
         <f t="shared" si="1"/>
@@ -8272,7 +8344,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <f t="shared" si="1"/>
@@ -8327,10 +8399,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -8363,7 +8435,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>12671.068850149601</v>
@@ -8405,7 +8477,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>3563.6396790663698</v>
@@ -8419,7 +8491,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>532.55813953488303</v>
@@ -8439,10 +8511,10 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -8483,7 +8555,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="1"/>
@@ -8537,7 +8609,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" si="1"/>
@@ -8555,7 +8627,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="1"/>
@@ -8585,17 +8657,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EFA07C-E270-4B85-8B26-6FA6BD53AA2B}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -8603,16 +8677,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -8620,13 +8694,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="2">
-        <v>153388.39848675899</v>
+        <v>94608.078994613999</v>
       </c>
       <c r="C2" s="2">
-        <v>31077.330895795199</v>
-      </c>
-      <c r="D2" s="2">
-        <v>4226.6036707250496</v>
+        <v>24934.145897762399</v>
+      </c>
+      <c r="D2">
+        <v>25478.6324786324</v>
+      </c>
+      <c r="E2" s="2">
+        <v>6090.6526236599502</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -8634,13 +8711,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>5112.9676716309395</v>
+        <v>4423.7664017741599</v>
       </c>
       <c r="C3" s="2">
-        <v>4881.5077439820798</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1225.8186636380799</v>
+        <v>3629.0172766115502</v>
+      </c>
+      <c r="D3">
+        <v>4249.2565055761997</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1478.3877439358</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -8648,27 +8728,33 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>5599.7051234795399</v>
+        <v>4772.4034495688002</v>
       </c>
       <c r="C4" s="2">
-        <v>905.28301886792406</v>
-      </c>
-      <c r="D4" s="2">
-        <v>924.14831545266304</v>
+        <v>4083.7116397312502</v>
+      </c>
+      <c r="D4">
+        <v>1236.2026747033301</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1203.62239297475</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
-        <v>2150.9571558796702</v>
+        <v>1380.2919708029101</v>
       </c>
       <c r="C5" s="2">
-        <v>1588.4536847967299</v>
-      </c>
-      <c r="D5" s="2">
-        <v>500.093510379652</v>
+        <v>1010.09190845197</v>
+      </c>
+      <c r="D5">
+        <v>1225.70135746606</v>
+      </c>
+      <c r="E5" s="2">
+        <v>630.28232332314303</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -8676,13 +8762,16 @@
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>381.49763722282802</v>
+        <v>105.83941605839399</v>
       </c>
       <c r="C6" s="2">
-        <v>553.65763089491202</v>
-      </c>
-      <c r="D6" s="2">
-        <v>97.656982193064593</v>
+        <v>78.820375335120602</v>
+      </c>
+      <c r="D6">
+        <v>138.01893663510501</v>
+      </c>
+      <c r="E6" s="2">
+        <v>51.277304701962201</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -8690,212 +8779,217 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>253.86313465783601</v>
+        <v>254.221899400762</v>
       </c>
       <c r="C7" s="2">
-        <v>71.600816175106601</v>
-      </c>
-      <c r="D7" s="2">
-        <v>70.606003398149895</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>230.582976345688</v>
+      </c>
+      <c r="D7">
+        <v>130.32863849765201</v>
+      </c>
+      <c r="E7" s="2">
+        <v>125.429242725465</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2">
-        <v>392.47510143858301</v>
+        <v>312.06057328285499</v>
       </c>
       <c r="C8" s="2">
-        <v>139.55965909090901</v>
-      </c>
-      <c r="D8" s="2">
-        <v>151.226656902233</v>
+        <v>258.71002322672803</v>
+      </c>
+      <c r="D8">
+        <v>240.29262802476001</v>
+      </c>
+      <c r="E8" s="2">
+        <v>270.86438152011903</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1237.2001432151801</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="2">
-        <v>137.174721189591</v>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" s="1"/>
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1">
+        <f xml:space="preserve"> B2 / $E2</f>
+        <v>15.533323740562109</v>
+      </c>
+      <c r="C11" s="1">
+        <f xml:space="preserve"> C2 / $E2</f>
+        <v>4.0938381218627367</v>
+      </c>
+      <c r="D11" s="1">
+        <f xml:space="preserve"> D2 / $E2</f>
+        <v>4.1832352053140029</v>
+      </c>
+      <c r="E11" s="1">
+        <f xml:space="preserve"> E2 / $E2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <f xml:space="preserve"> B3 / $E3</f>
+        <v>2.9922910413184978</v>
+      </c>
+      <c r="C12" s="1">
+        <f xml:space="preserve"> C3 / $E3</f>
+        <v>2.4547127717321922</v>
+      </c>
+      <c r="D12" s="1">
+        <f xml:space="preserve"> D3 / $E3</f>
+        <v>2.8742503602361618</v>
+      </c>
+      <c r="E12" s="1">
+        <f xml:space="preserve"> E3 / $E3</f>
         <v>1</v>
       </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1">
-        <f xml:space="preserve"> B2 / $D2</f>
-        <v>36.291171455034032</v>
+        <f xml:space="preserve"> B4 / $E4</f>
+        <v>3.9650337825418949</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" ref="C13:D13" si="0" xml:space="preserve"> C2 / $D2</f>
-        <v>7.3527904002563034</v>
+        <f xml:space="preserve"> C4 / $E4</f>
+        <v>3.3928511662518726</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> D4 / $E4</f>
+        <v>1.027068524080927</v>
+      </c>
+      <c r="E13" s="1">
+        <f xml:space="preserve"> E4 / $E4</f>
         <v>1</v>
       </c>
-      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" ref="B14:D14" si="1" xml:space="preserve"> B3 / $D3</f>
-        <v>4.1710636518261817</v>
+        <f xml:space="preserve"> B5 / $E5</f>
+        <v>2.1899582452596253</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="1"/>
-        <v>3.9822429603856428</v>
+        <f xml:space="preserve"> C5 / $E5</f>
+        <v>1.6026023118120991</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="1"/>
+        <f xml:space="preserve"> D5 / $E5</f>
+        <v>1.9446862336287483</v>
+      </c>
+      <c r="E14" s="1">
+        <f xml:space="preserve"> E5 / $E5</f>
         <v>1</v>
       </c>
-      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" ref="B15:D15" si="2" xml:space="preserve"> B4 / $D4</f>
-        <v>6.0593143220054593</v>
+        <f xml:space="preserve"> B6 / $E6</f>
+        <v>2.064059659016046</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="2"/>
-        <v>0.97958628905199219</v>
+        <f xml:space="preserve"> C6 / $E6</f>
+        <v>1.5371395940805841</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="2"/>
+        <f xml:space="preserve"> D6 / $E6</f>
+        <v>2.6916183960391256</v>
+      </c>
+      <c r="E15" s="1">
+        <f xml:space="preserve"> E6 / $E6</f>
         <v>1</v>
       </c>
-      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" ref="B16:D16" si="3" xml:space="preserve"> B5 / $D5</f>
-        <v>4.3011099149172027</v>
+        <f xml:space="preserve"> B7 / $E7</f>
+        <v>2.0268152296605484</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="3"/>
-        <v>3.1763133330621232</v>
+        <f xml:space="preserve"> C7 / $E7</f>
+        <v>1.8383510203468236</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> D7 / $E7</f>
+        <v>1.0390610328638483</v>
+      </c>
+      <c r="E16" s="1">
+        <f xml:space="preserve"> E7 / $E7</f>
         <v>1</v>
       </c>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" ref="B17:D17" si="4" xml:space="preserve"> B6 / $D6</f>
-        <v>3.9065065155159098</v>
+        <f xml:space="preserve"> B8 / $E8</f>
+        <v>1.1520915800428932</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="4"/>
-        <v>5.6694116330601876</v>
+        <f xml:space="preserve"> C8 / $E8</f>
+        <v>0.95512751353581637</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="4"/>
+        <f xml:space="preserve"> D8 / $E8</f>
+        <v>0.88713261845729896</v>
+      </c>
+      <c r="E17" s="1">
+        <f xml:space="preserve"> E8 / $E8</f>
         <v>1</v>
       </c>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1">
-        <f t="shared" ref="B18:D18" si="5" xml:space="preserve"> B7 / $D7</f>
-        <v>3.5954893697394583</v>
-      </c>
-      <c r="C18" s="1">
-        <f t="shared" si="5"/>
-        <v>1.0140896344372718</v>
-      </c>
-      <c r="D18" s="1">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="1">
-        <f t="shared" ref="B19:D19" si="6" xml:space="preserve"> B8 / $D8</f>
-        <v>2.5952772446217303</v>
-      </c>
-      <c r="C19" s="1">
-        <f t="shared" si="6"/>
-        <v>0.9228509176205183</v>
-      </c>
-      <c r="D19" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="1">
-        <f t="shared" ref="B20:D20" si="7" xml:space="preserve"> B9 / $D9</f>
-        <v>9.0191555155795022</v>
-      </c>
-      <c r="C20" s="1" t="e">
-        <f t="shared" si="7"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D20" s="1">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="F21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Close #266 -  function
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAACDB3-E796-4116-8E3E-A5D51F0980AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A3403F-604A-43F1-B524-BDC897A4B72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
+    <workbookView xWindow="-14685" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
   <sheets>
     <sheet name="is" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="27">
   <si>
     <t>Components</t>
   </si>
@@ -116,15 +116,19 @@
   <si>
     <t>TSON.assertStringify()</t>
   </si>
+  <si>
+    <t>TSON.isStringify()</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="##,##0%"/>
+    <numFmt numFmtId="167" formatCode="#,###%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -164,11 +168,13 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="백분율" xfId="1" builtinId="5"/>
@@ -3304,28 +3310,28 @@
             <c:numRef>
               <c:f>stringify!$B$11:$B$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>#,###%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>15.533323740562109</c:v>
+                  <c:v>37.667815498574349</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.9922910413184978</c:v>
+                  <c:v>4.5155919487202283</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9650337825418949</c:v>
+                  <c:v>6.8340172166227529</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1899582452596253</c:v>
+                  <c:v>3.8213903326325305</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.064059659016046</c:v>
+                  <c:v>3.6619337774712575</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0268152296605484</c:v>
+                  <c:v>3.4348613119400033</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1520915800428932</c:v>
+                  <c:v>2.0719330472927138</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3393,28 +3399,28 @@
             <c:numRef>
               <c:f>stringify!$C$11:$C$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>#,###%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.0938381218627367</c:v>
+                  <c:v>9.6511048733443126</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4547127717321922</c:v>
+                  <c:v>3.4645473154567994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.3928511662518726</c:v>
+                  <c:v>6.00613678504231</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6026023118120991</c:v>
+                  <c:v>2.6753023362709167</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5371395940805841</c:v>
+                  <c:v>2.9532024792917211</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8383510203468236</c:v>
+                  <c:v>3.0567452675176559</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.95512751353581637</c:v>
+                  <c:v>1.7792433923091913</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3434,7 +3440,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>fast-json-stringify</c:v>
+                  <c:v>TSON.isStringify()</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3482,28 +3488,28 @@
             <c:numRef>
               <c:f>stringify!$D$11:$D$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>#,###%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.1832352053140029</c:v>
+                  <c:v>9.4545287239162992</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8742503602361618</c:v>
+                  <c:v>4.0774230407945433</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.027068524080927</c:v>
+                  <c:v>6.2605874099228576</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9446862336287483</c:v>
+                  <c:v>3.3584020613449828</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6916183960391256</c:v>
+                  <c:v>3.4284582809393633</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0390610328638483</c:v>
+                  <c:v>3.261774323188773</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.88713261845729896</c:v>
+                  <c:v>1.8704685660215872</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3571,7 +3577,7 @@
             <c:numRef>
               <c:f>stringify!$E$11:$E$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>#,###%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
@@ -3600,6 +3606,95 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-1CE8-45C7-9E81-77C2BCCB8731}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stringify!$F$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fast-json-stringify</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>stringify!$A$11:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>object (simple)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>object (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>object (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>object (union)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>array (hierarchical)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>array (recursive)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>array (union)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stringify!$F$11:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>#,###%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.6441149082489375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1489366027582166</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0422732429547579</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.655269329737822</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.30187097509965</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.020143072289156</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.9812964569673267</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-03ED-4EB9-B72A-F1707F74F7B7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3670,7 +3765,7 @@
         <c:axId val="555336592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="16"/>
+          <c:max val="40"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3689,7 +3784,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="#,###%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6704,16 +6799,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>131444</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1904</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1905</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>116204</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>588644</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1905</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7044,16 +7139,16 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7076,7 +7171,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -7099,7 +7194,7 @@
         <v>68.706485892268205</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -7122,7 +7217,7 @@
         <v>43.583535108958799</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -7145,7 +7240,7 @@
         <v>17.757009345794302</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -7168,7 +7263,7 @@
         <v>16.530460624071299</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -7191,7 +7286,7 @@
         <v>3.72856077554064</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -7214,7 +7309,7 @@
         <v>8.6514952040624404</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -7237,7 +7332,7 @@
         <v>5.3574727507851403</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -7260,7 +7355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -7283,7 +7378,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -7312,7 +7407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -7341,7 +7436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -7370,7 +7465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -7399,7 +7494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -7428,7 +7523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -7457,7 +7552,7 @@
         <v>2.8652670678954304</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -7486,7 +7581,7 @@
         <v>2.5930168113800187</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -7515,7 +7610,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I24" t="s">
         <v>22</v>
       </c>
@@ -7535,14 +7630,14 @@
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7562,7 +7657,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -7582,7 +7677,7 @@
         <v>62.148940025366898</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -7602,7 +7697,7 @@
         <v>38.9730328777244</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -7622,7 +7717,7 @@
         <v>16.396497111980601</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -7642,7 +7737,7 @@
         <v>14.6051208077893</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -7662,7 +7757,7 @@
         <v>3.3994334277620299</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -7682,7 +7777,7 @@
         <v>7.3696145124716503</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -7702,7 +7797,7 @@
         <v>4.71527022125498</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -7722,7 +7817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -7742,7 +7837,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -7767,7 +7862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -7792,7 +7887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -7817,7 +7912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -7842,7 +7937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -7867,7 +7962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -7892,7 +7987,7 @@
         <v>2.6319349962207097</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -7917,7 +8012,7 @@
         <v>2.7914399709829634</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -7942,7 +8037,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H23" t="s">
         <v>23</v>
       </c>
@@ -7960,14 +8055,14 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7987,7 +8082,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -8007,7 +8102,7 @@
         <v>57.518032180506701</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -8027,7 +8122,7 @@
         <v>35.983421250941902</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -8047,7 +8142,7 @@
         <v>15.322134022521601</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -8067,7 +8162,7 @@
         <v>13.824884792626699</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -8087,7 +8182,7 @@
         <v>3.4090909090908998</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -8107,7 +8202,7 @@
         <v>6.8773234200743403</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -8127,7 +8222,7 @@
         <v>4.2766827817032302</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -8147,7 +8242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -8167,7 +8262,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -8192,7 +8287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -8217,7 +8312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -8242,7 +8337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -8267,7 +8362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -8292,7 +8387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -8317,7 +8412,7 @@
         <v>2.4437422552664221</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -8342,7 +8437,7 @@
         <v>2.2734845667534413</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -8382,16 +8477,16 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8405,7 +8500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -8419,7 +8514,7 @@
         <v>4.7050307636626796</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -8433,7 +8528,7 @@
         <v>8.5232536594404298</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -8447,7 +8542,7 @@
         <v>4.11445670469422</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -8461,7 +8556,7 @@
         <v>6.0998151571164501</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -8475,7 +8570,7 @@
         <v>8.8695980373655399</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -8489,7 +8584,7 @@
         <v>5.8964437073889799</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -8503,7 +8598,7 @@
         <v>0.90334236675699997</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -8517,7 +8612,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -8535,7 +8630,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -8553,7 +8648,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -8571,7 +8666,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -8589,7 +8684,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -8607,7 +8702,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -8625,7 +8720,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -8643,7 +8738,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -8660,19 +8755,20 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8683,135 +8779,159 @@
         <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2">
-        <v>94608.078994613999</v>
+        <v>151983.729433272</v>
       </c>
       <c r="C2" s="2">
-        <v>24934.145897762399</v>
-      </c>
-      <c r="D2">
-        <v>25478.6324786324</v>
+        <v>38940.694924504198</v>
+      </c>
+      <c r="D2" s="4">
+        <v>38147.540983606501</v>
       </c>
       <c r="E2" s="2">
-        <v>6090.6526236599502</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4034.8432055749099</v>
+      </c>
+      <c r="F2" s="4">
+        <v>30842.8051001821</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>4423.7664017741599</v>
+        <v>5153.42565597667</v>
       </c>
       <c r="C3" s="2">
-        <v>3629.0172766115502</v>
-      </c>
-      <c r="D3">
-        <v>4249.2565055761997</v>
+        <v>3953.9194915254202</v>
+      </c>
+      <c r="D3" s="4">
+        <v>4653.3647741701398</v>
       </c>
       <c r="E3" s="2">
-        <v>1478.3877439358</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1141.2514050206</v>
+      </c>
+      <c r="F3" s="4">
+        <v>4734.9797272392098</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>4772.4034495688002</v>
+        <v>5616.6264613100702</v>
       </c>
       <c r="C4" s="2">
-        <v>4083.7116397312502</v>
-      </c>
-      <c r="D4">
-        <v>1236.2026747033301</v>
+        <v>4936.2220971675097</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5145.3456722917799</v>
       </c>
       <c r="E4" s="2">
-        <v>1203.62239297475</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>821.86308334846501</v>
+      </c>
+      <c r="F4" s="4">
+        <v>856.60590114640104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2">
-        <v>1380.2919708029101</v>
+        <v>1459.6273291925399</v>
       </c>
       <c r="C5" s="2">
-        <v>1010.09190845197</v>
-      </c>
-      <c r="D5">
-        <v>1225.70135746606</v>
+        <v>1021.86483556198</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1282.7832292595799</v>
       </c>
       <c r="E5" s="2">
-        <v>630.28232332314303</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>381.96237550719201</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1396.17535630524</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>105.83941605839399</v>
+        <v>275.07163323782203</v>
       </c>
       <c r="C6" s="2">
-        <v>78.820375335120602</v>
-      </c>
-      <c r="D6">
-        <v>138.01893663510501</v>
+        <v>221.834221650431</v>
+      </c>
+      <c r="D6" s="4">
+        <v>257.53377208174498</v>
       </c>
       <c r="E6" s="2">
-        <v>51.277304701962201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75.116495806150894</v>
+      </c>
+      <c r="F6" s="4">
+        <v>398.257968865826</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>254.221899400762</v>
+        <v>256.07749954304501</v>
       </c>
       <c r="C7" s="2">
-        <v>230.582976345688</v>
-      </c>
-      <c r="D7">
-        <v>130.32863849765201</v>
+        <v>227.88800296680799</v>
+      </c>
+      <c r="D7" s="4">
+        <v>243.17343173431701</v>
       </c>
       <c r="E7" s="2">
-        <v>125.429242725465</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>74.552500461339704</v>
+      </c>
+      <c r="F7" s="4">
+        <v>76.054216867469805</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2">
-        <v>312.06057328285499</v>
+        <v>338.25116948542598</v>
       </c>
       <c r="C8" s="2">
-        <v>258.71002322672803</v>
-      </c>
-      <c r="D8">
-        <v>240.29262802476001</v>
+        <v>290.46843913908401</v>
+      </c>
+      <c r="D8" s="4">
+        <v>305.36130536130503</v>
       </c>
       <c r="E8" s="2">
-        <v>270.86438152011903</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>163.25390915860001</v>
+      </c>
+      <c r="F8" s="4">
+        <v>160.20048264339999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -8822,171 +8942,202 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1">
-        <f xml:space="preserve"> B2 / $E2</f>
-        <v>15.533323740562109</v>
-      </c>
-      <c r="C11" s="1">
-        <f xml:space="preserve"> C2 / $E2</f>
-        <v>4.0938381218627367</v>
-      </c>
-      <c r="D11" s="1">
-        <f xml:space="preserve"> D2 / $E2</f>
-        <v>4.1832352053140029</v>
-      </c>
-      <c r="E11" s="1">
-        <f xml:space="preserve"> E2 / $E2</f>
+      <c r="B11" s="5">
+        <f t="shared" ref="B11:F11" si="0" xml:space="preserve"> B2 / $E2</f>
+        <v>37.667815498574349</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" si="0"/>
+        <v>9.6511048733443126</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
+        <v>9.4545287239162992</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="5">
+        <f t="shared" si="0"/>
+        <v>7.6441149082489375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1">
-        <f xml:space="preserve"> B3 / $E3</f>
-        <v>2.9922910413184978</v>
-      </c>
-      <c r="C12" s="1">
-        <f xml:space="preserve"> C3 / $E3</f>
-        <v>2.4547127717321922</v>
-      </c>
-      <c r="D12" s="1">
-        <f xml:space="preserve"> D3 / $E3</f>
-        <v>2.8742503602361618</v>
-      </c>
-      <c r="E12" s="1">
-        <f xml:space="preserve"> E3 / $E3</f>
+      <c r="B12" s="5">
+        <f t="shared" ref="B12:F12" si="1" xml:space="preserve"> B3 / $E3</f>
+        <v>4.5155919487202283</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" si="1"/>
+        <v>3.4645473154567994</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="1"/>
+        <v>4.0774230407945433</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="5">
+        <f t="shared" si="1"/>
+        <v>4.1489366027582166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="1">
-        <f xml:space="preserve"> B4 / $E4</f>
-        <v>3.9650337825418949</v>
-      </c>
-      <c r="C13" s="1">
-        <f xml:space="preserve"> C4 / $E4</f>
-        <v>3.3928511662518726</v>
-      </c>
-      <c r="D13" s="1">
-        <f xml:space="preserve"> D4 / $E4</f>
-        <v>1.027068524080927</v>
-      </c>
-      <c r="E13" s="1">
-        <f xml:space="preserve"> E4 / $E4</f>
+      <c r="B13" s="5">
+        <f t="shared" ref="B13:F13" si="2" xml:space="preserve"> B4 / $E4</f>
+        <v>6.8340172166227529</v>
+      </c>
+      <c r="C13" s="5">
+        <f t="shared" si="2"/>
+        <v>6.00613678504231</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="2"/>
+        <v>6.2605874099228576</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="5">
+        <f t="shared" si="2"/>
+        <v>1.0422732429547579</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
-        <f xml:space="preserve"> B5 / $E5</f>
-        <v>2.1899582452596253</v>
-      </c>
-      <c r="C14" s="1">
-        <f xml:space="preserve"> C5 / $E5</f>
-        <v>1.6026023118120991</v>
-      </c>
-      <c r="D14" s="1">
-        <f xml:space="preserve"> D5 / $E5</f>
-        <v>1.9446862336287483</v>
-      </c>
-      <c r="E14" s="1">
-        <f xml:space="preserve"> E5 / $E5</f>
+      <c r="B14" s="5">
+        <f t="shared" ref="B14:F14" si="3" xml:space="preserve"> B5 / $E5</f>
+        <v>3.8213903326325305</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" si="3"/>
+        <v>2.6753023362709167</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" si="3"/>
+        <v>3.3584020613449828</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="5">
+        <f t="shared" si="3"/>
+        <v>3.655269329737822</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="1">
-        <f xml:space="preserve"> B6 / $E6</f>
-        <v>2.064059659016046</v>
-      </c>
-      <c r="C15" s="1">
-        <f xml:space="preserve"> C6 / $E6</f>
-        <v>1.5371395940805841</v>
-      </c>
-      <c r="D15" s="1">
-        <f xml:space="preserve"> D6 / $E6</f>
-        <v>2.6916183960391256</v>
-      </c>
-      <c r="E15" s="1">
-        <f xml:space="preserve"> E6 / $E6</f>
+      <c r="B15" s="5">
+        <f t="shared" ref="B15:F15" si="4" xml:space="preserve"> B6 / $E6</f>
+        <v>3.6619337774712575</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" si="4"/>
+        <v>2.9532024792917211</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="4"/>
+        <v>3.4284582809393633</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="5">
+        <f t="shared" si="4"/>
+        <v>5.30187097509965</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="1">
-        <f xml:space="preserve"> B7 / $E7</f>
-        <v>2.0268152296605484</v>
-      </c>
-      <c r="C16" s="1">
-        <f xml:space="preserve"> C7 / $E7</f>
-        <v>1.8383510203468236</v>
-      </c>
-      <c r="D16" s="1">
-        <f xml:space="preserve"> D7 / $E7</f>
-        <v>1.0390610328638483</v>
-      </c>
-      <c r="E16" s="1">
-        <f xml:space="preserve"> E7 / $E7</f>
+      <c r="B16" s="5">
+        <f t="shared" ref="B16:F16" si="5" xml:space="preserve"> B7 / $E7</f>
+        <v>3.4348613119400033</v>
+      </c>
+      <c r="C16" s="5">
+        <f t="shared" si="5"/>
+        <v>3.0567452675176559</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" si="5"/>
+        <v>3.261774323188773</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="5">
+        <f t="shared" si="5"/>
+        <v>1.020143072289156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="1">
-        <f xml:space="preserve"> B8 / $E8</f>
-        <v>1.1520915800428932</v>
-      </c>
-      <c r="C17" s="1">
-        <f xml:space="preserve"> C8 / $E8</f>
-        <v>0.95512751353581637</v>
-      </c>
-      <c r="D17" s="1">
-        <f xml:space="preserve"> D8 / $E8</f>
-        <v>0.88713261845729896</v>
-      </c>
-      <c r="E17" s="1">
-        <f xml:space="preserve"> E8 / $E8</f>
+      <c r="B17" s="5">
+        <f t="shared" ref="B17:F17" si="6" xml:space="preserve"> B8 / $E8</f>
+        <v>2.0719330472927138</v>
+      </c>
+      <c r="C17" s="5">
+        <f t="shared" si="6"/>
+        <v>1.7792433923091913</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" si="6"/>
+        <v>1.8704685660215872</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="5">
+        <f t="shared" si="6"/>
+        <v>0.9812964569673267</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="F21" s="1"/>

</xml_diff>

<commit_message>
Revise README for #281
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE2875F-4772-4B34-A977-945201710C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E00D5E-F85F-4A43-B94A-353E55714D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="10" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="8" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
   <sheets>
     <sheet name="TSON" sheetId="11" r:id="rId1"/>
@@ -6982,7 +6982,7 @@
                   <a:srgbClr val="7030A0"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>equals()</a:t>
+              <a:t>validateEquals()</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
@@ -14917,7 +14917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EFA07C-E270-4B85-8B26-6FA6BD53AA2B}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -15592,27 +15592,27 @@
         <v>7</v>
       </c>
       <c r="B13" s="3">
-        <f xml:space="preserve"> B2 / MIN($B2:$G2)</f>
+        <f t="shared" ref="B13:G21" si="0" xml:space="preserve"> B2 / MIN($B2:$G2)</f>
         <v>2564.707576357684</v>
       </c>
       <c r="C13" s="3">
-        <f xml:space="preserve"> C2 / MIN($B2:$G2)</f>
+        <f t="shared" si="0"/>
         <v>9320.565749917163</v>
       </c>
       <c r="D13" s="3">
-        <f xml:space="preserve"> D2 / MIN($B2:$G2)</f>
+        <f t="shared" si="0"/>
         <v>2340.1687451825233</v>
       </c>
       <c r="E13" s="3">
-        <f xml:space="preserve"> E2 / MIN($B2:$G2)</f>
+        <f t="shared" si="0"/>
         <v>229.85033657781318</v>
       </c>
       <c r="F13" s="3">
-        <f xml:space="preserve"> F2 / MIN($B2:$G2)</f>
+        <f t="shared" si="0"/>
         <v>22.206056657117706</v>
       </c>
       <c r="G13" s="3">
-        <f xml:space="preserve"> G2 / MIN($B2:$G2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -15621,27 +15621,27 @@
         <v>2</v>
       </c>
       <c r="B14" s="3">
-        <f xml:space="preserve"> B3 / MIN($B3:$G3)</f>
+        <f t="shared" si="0"/>
         <v>2177.7957546860434</v>
       </c>
       <c r="C14" s="3">
-        <f xml:space="preserve"> C3 / MIN($B3:$G3)</f>
+        <f t="shared" si="0"/>
         <v>3671.9312328071892</v>
       </c>
       <c r="D14" s="3">
-        <f xml:space="preserve"> D3 / MIN($B3:$G3)</f>
+        <f t="shared" si="0"/>
         <v>993.22281726787128</v>
       </c>
       <c r="E14" s="3">
-        <f xml:space="preserve"> E3 / MIN($B3:$G3)</f>
+        <f t="shared" si="0"/>
         <v>195.46314484123539</v>
       </c>
       <c r="F14" s="3">
-        <f xml:space="preserve"> F3 / MIN($B3:$G3)</f>
+        <f t="shared" si="0"/>
         <v>9.4811325934996251</v>
       </c>
       <c r="G14" s="3">
-        <f xml:space="preserve"> G3 / MIN($B3:$G3)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -15650,27 +15650,27 @@
         <v>3</v>
       </c>
       <c r="B15" s="3">
-        <f xml:space="preserve"> B4 / MIN($B4:$G4)</f>
+        <f t="shared" si="0"/>
         <v>2189.0764682944045</v>
       </c>
       <c r="C15" s="3">
-        <f xml:space="preserve"> C4 / MIN($B4:$G4)</f>
+        <f t="shared" si="0"/>
         <v>2364.6876346741719</v>
       </c>
       <c r="D15" s="3">
-        <f xml:space="preserve"> D4 / MIN($B4:$G4)</f>
+        <f t="shared" si="0"/>
         <v>1186.6348502576104</v>
       </c>
       <c r="E15" s="3">
-        <f xml:space="preserve"> E4 / MIN($B4:$G4)</f>
+        <f t="shared" si="0"/>
         <v>152.13070523555021</v>
       </c>
       <c r="F15" s="3">
-        <f xml:space="preserve"> F4 / MIN($B4:$G4)</f>
+        <f t="shared" si="0"/>
         <v>1.8920316704159512</v>
       </c>
       <c r="G15" s="3">
-        <f xml:space="preserve"> G4 / MIN($B4:$G4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -15679,27 +15679,27 @@
         <v>14</v>
       </c>
       <c r="B16" s="3">
-        <f xml:space="preserve"> B5 / MIN($B5:$G5)</f>
+        <f t="shared" si="0"/>
         <v>427.96782279603872</v>
       </c>
       <c r="C16" s="3">
-        <f xml:space="preserve"> C5 / MIN($B5:$G5)</f>
+        <f t="shared" si="0"/>
         <v>378.75143141257126</v>
       </c>
       <c r="D16" s="3">
-        <f xml:space="preserve"> D5 / MIN($B5:$G5)</f>
+        <f t="shared" si="0"/>
         <v>215.43462691023518</v>
       </c>
       <c r="E16" s="3">
-        <f xml:space="preserve"> E5 / MIN($B5:$G5)</f>
+        <f t="shared" si="0"/>
         <v>92.690148090985943</v>
       </c>
       <c r="F16" s="3">
-        <f xml:space="preserve"> F5 / MIN($B5:$G5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G16" s="3">
-        <f xml:space="preserve"> G5 / MIN($B5:$G5)</f>
+        <f t="shared" si="0"/>
         <v>2.3251337378010435</v>
       </c>
     </row>
@@ -15708,27 +15708,27 @@
         <v>15</v>
       </c>
       <c r="B17" s="3">
-        <f xml:space="preserve"> B6 / MIN($B6:$G6)</f>
+        <f t="shared" si="0"/>
         <v>852.67113961797122</v>
       </c>
       <c r="C17" s="3" t="e">
-        <f xml:space="preserve"> C6 / MIN($B6:$G6)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="D17" s="3" t="e">
-        <f xml:space="preserve"> D6 / MIN($B6:$G6)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="E17" s="3" t="e">
-        <f xml:space="preserve"> E6 / MIN($B6:$G6)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="F17" s="3">
-        <f xml:space="preserve"> F6 / MIN($B6:$G6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G17" s="3">
-        <f xml:space="preserve"> G6 / MIN($B6:$G6)</f>
+        <f t="shared" si="0"/>
         <v>3.024719101123595</v>
       </c>
     </row>
@@ -15737,27 +15737,27 @@
         <v>5</v>
       </c>
       <c r="B18" s="3">
-        <f xml:space="preserve"> B7 / MIN($B7:$G7)</f>
+        <f t="shared" si="0"/>
         <v>1814.4827670198492</v>
       </c>
       <c r="C18" s="3">
-        <f xml:space="preserve"> C7 / MIN($B7:$G7)</f>
+        <f t="shared" si="0"/>
         <v>1932.4938090881353</v>
       </c>
       <c r="D18" s="3">
-        <f xml:space="preserve"> D7 / MIN($B7:$G7)</f>
+        <f t="shared" si="0"/>
         <v>673.96995443910646</v>
       </c>
       <c r="E18" s="3">
-        <f xml:space="preserve"> E7 / MIN($B7:$G7)</f>
+        <f t="shared" si="0"/>
         <v>147.27808003868915</v>
       </c>
       <c r="F18" s="3">
-        <f xml:space="preserve"> F7 / MIN($B7:$G7)</f>
+        <f t="shared" si="0"/>
         <v>2.7726318389526967</v>
       </c>
       <c r="G18" s="3">
-        <f xml:space="preserve"> G7 / MIN($B7:$G7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -15766,27 +15766,27 @@
         <v>16</v>
       </c>
       <c r="B19" s="3">
-        <f xml:space="preserve"> B8 / MIN($B8:$G8)</f>
+        <f t="shared" si="0"/>
         <v>1455.7520761350572</v>
       </c>
       <c r="C19" s="3">
-        <f xml:space="preserve"> C8 / MIN($B8:$G8)</f>
+        <f t="shared" si="0"/>
         <v>714.79334708935164</v>
       </c>
       <c r="D19" s="3">
-        <f xml:space="preserve"> D8 / MIN($B8:$G8)</f>
+        <f t="shared" si="0"/>
         <v>297.67457627118722</v>
       </c>
       <c r="E19" s="3">
-        <f xml:space="preserve"> E8 / MIN($B8:$G8)</f>
+        <f t="shared" si="0"/>
         <v>132.84216417910457</v>
       </c>
       <c r="F19" s="3">
-        <f xml:space="preserve"> F8 / MIN($B8:$G8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G19" s="3">
-        <f xml:space="preserve"> G8 / MIN($B8:$G8)</f>
+        <f t="shared" si="0"/>
         <v>10.094678899082574</v>
       </c>
     </row>
@@ -15795,27 +15795,27 @@
         <v>17</v>
       </c>
       <c r="B20" s="3">
-        <f xml:space="preserve"> B9 / MIN($B9:$G9)</f>
+        <f t="shared" si="0"/>
         <v>1096.9599353796464</v>
       </c>
       <c r="C20" s="3" t="e">
-        <f xml:space="preserve"> C9 / MIN($B9:$G9)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="D20" s="3" t="e">
-        <f xml:space="preserve"> D9 / MIN($B9:$G9)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="E20" s="3" t="e">
-        <f xml:space="preserve"> E9 / MIN($B9:$G9)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="F20" s="3">
-        <f xml:space="preserve"> F9 / MIN($B9:$G9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G20" s="3">
-        <f xml:space="preserve"> G9 / MIN($B9:$G9)</f>
+        <f t="shared" si="0"/>
         <v>11.130969529085894</v>
       </c>
     </row>
@@ -15824,27 +15824,27 @@
         <v>10</v>
       </c>
       <c r="B21" s="3">
-        <f xml:space="preserve"> B10 / MIN($B10:$G10)</f>
+        <f t="shared" si="0"/>
         <v>1301.0866497829227</v>
       </c>
       <c r="C21" s="3" t="e">
-        <f xml:space="preserve"> C10 / MIN($B10:$G10)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="D21" s="3" t="e">
-        <f xml:space="preserve"> D10 / MIN($B10:$G10)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="E21" s="3" t="e">
-        <f xml:space="preserve"> E10 / MIN($B10:$G10)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="F21" s="3">
-        <f xml:space="preserve"> F10 / MIN($B10:$G10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G21" s="3" t="e">
-        <f xml:space="preserve"> G10 / MIN($B10:$G10)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -18138,8 +18138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8493B1B1-D0E4-4633-B757-06DDEF8B12BC}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Benchmark #290 on i5-1135g7 and AMD-5900HX
</commit_message>
<xml_diff>
--- a/benchmark/results/charts.xlsx
+++ b/benchmark/results/charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\samchon\typescript-json\benchmark\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABDF9C0-3A17-4842-8A25-38F4FC2260D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3A7777-597E-4FCC-B65E-A118A98F8B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="2" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
+    <workbookView xWindow="-10927" yWindow="8002" windowWidth="21795" windowHeight="13875" activeTab="6" xr2:uid="{AF35FF4A-69D2-475D-B4FC-4CBFAD73187A}"/>
   </bookViews>
   <sheets>
     <sheet name="is" sheetId="2" r:id="rId1"/>
@@ -2830,31 +2830,31 @@
                 <c:formatCode>##,##0\x</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>248.70333940497852</c:v>
+                  <c:v>285.96771834339654</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>488.23373909883639</c:v>
+                  <c:v>505.46488355167423</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>153.63712374581948</c:v>
+                  <c:v>147.97208448117522</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>181.42680935969511</c:v>
+                  <c:v>172.92560309913753</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>143.3112570698776</c:v>
+                  <c:v>145.94591671173629</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>113.20934379457957</c:v>
+                  <c:v>151.77725884677616</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42.525631768953268</c:v>
+                  <c:v>42.76078431372563</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.315502183406114</c:v>
+                  <c:v>19.131741982507407</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>118.35904728048367</c:v>
+                  <c:v>103.85025566106658</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2931,25 +2931,25 @@
                 <c:formatCode>##,##0\x</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>12.735618493029801</c:v>
+                  <c:v>15.984503373188184</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.708587821580609</c:v>
+                  <c:v>12.590765220629311</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.5402592660215229</c:v>
+                  <c:v>4.5642380422691797</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.756946887091114</c:v>
+                  <c:v>3.916830973292718</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4847361919887094</c:v>
+                  <c:v>1.4807170016295481</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -3032,25 +3032,25 @@
                 <c:formatCode>##,##0\x</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>57.346535718676769</c:v>
+                  <c:v>62.312937967360917</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.284833024118782</c:v>
+                  <c:v>51.64318813716406</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.103504630470084</c:v>
+                  <c:v>36.376329787234042</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.371644612476398</c:v>
+                  <c:v>13.663477771525102</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.1483375959079565</c:v>
+                  <c:v>6.0916201117318636</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -3133,10 +3133,10 @@
                 <c:formatCode>##,##0\x</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>14.873187108325864</c:v>
+                  <c:v>16.824403861029833</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.4505159474671698</c:v>
+                  <c:v>6.1164499717354355</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -3148,7 +3148,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2376440865308769</c:v>
+                  <c:v>1.1998023389886341</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -3240,22 +3240,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5026695141484274</c:v>
+                  <c:v>2.6263654878726164</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0136338847482076</c:v>
+                  <c:v>3.6163361661945146</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5922018348623852</c:v>
+                  <c:v>2.5411033978808963</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0485507246376975</c:v>
+                  <c:v>4.4110032362459624</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.6230651471338633</c:v>
+                  <c:v>3.3871540099361459</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3336,7 +3336,7 @@
         <c:axId val="381772640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="500"/>
+          <c:max val="510"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -5438,28 +5438,28 @@
                 <c:formatCode>##,##0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>7.8053847905282163</c:v>
+                  <c:v>7.1512627307035981</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.67966214926512</c:v>
+                  <c:v>9.5007977290069121</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.353097276062151</c:v>
+                  <c:v>17.912085279674226</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.680974899963601</c:v>
+                  <c:v>19.798608568290007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.297411516111943</c:v>
+                  <c:v>21.817856487428788</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.018336729023885</c:v>
+                  <c:v>10.830358785648579</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.856039713182602</c:v>
+                  <c:v>11.569968983762152</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.1350476532997265</c:v>
+                  <c:v>7.9181501192879589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5632,7 +5632,7 @@
         <c:axId val="480554528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="25"/>
+          <c:max val="22"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -13112,16 +13112,16 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13144,7 +13144,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -13167,7 +13167,7 @@
         <v>163.17767042404699</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -13190,7 +13190,7 @@
         <v>55.535390199637</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -13213,7 +13213,7 @@
         <v>42.849295000915497</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -13236,7 +13236,7 @@
         <v>112.035496394897</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -13259,7 +13259,7 @@
         <v>78.874282540270301</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -13282,7 +13282,7 @@
         <v>3.77833753148614</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -13305,7 +13305,7 @@
         <v>42.113040265977098</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -13328,7 +13328,7 @@
         <v>29.937864808887198</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -13351,7 +13351,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -13374,7 +13374,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -13403,7 +13403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -13432,7 +13432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -13461,7 +13461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -13490,7 +13490,7 @@
         <v>3.0873861419469457</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -13519,7 +13519,7 @@
         <v>4.187296470152587</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -13548,7 +13548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -13577,7 +13577,7 @@
         <v>12.823420760990031</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -13606,7 +13606,7 @@
         <v>13.758943701751125</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -13635,7 +13635,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
         <v>22</v>
       </c>
@@ -13655,17 +13655,17 @@
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.53125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13685,7 +13685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -13705,7 +13705,7 @@
         <v>23169.116312828799</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -13725,7 +13725,7 @@
         <v>3933.8842975206599</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -13745,7 +13745,7 @@
         <v>1215.7591525738701</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -13765,7 +13765,7 @@
         <v>1216.5202108962999</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -13785,7 +13785,7 @@
         <v>294.30262671106101</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -13805,7 +13805,7 @@
         <v>127.289546716003</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -13825,10 +13825,10 @@
         <v>225.67592422291699</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -13848,7 +13848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -13873,7 +13873,7 @@
         <v>3.7862164651967358</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -13898,7 +13898,7 @@
         <v>2.6036109002111547</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -13923,7 +13923,7 @@
         <v>0.97168698961960165</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -13948,7 +13948,7 @@
         <v>1.9660085247358605</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -13973,7 +13973,7 @@
         <v>2.7733755438044305</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -13998,7 +13998,7 @@
         <v>0.99111933395004725</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -14023,23 +14023,23 @@
         <v>0.88606627474092803</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
         <v>26</v>
       </c>
@@ -14055,18 +14055,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050C2C99-5EE7-403C-9AB2-DBCB91E8248D}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14086,7 +14086,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -14106,7 +14106,7 @@
         <v>201.980198019802</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -14126,7 +14126,7 @@
         <v>68.181818181818102</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -14146,7 +14146,7 @@
         <v>42.475948447994099</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -14166,7 +14166,7 @@
         <v>117.836812144212</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -14186,7 +14186,7 @@
         <v>78.145205985590195</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -14206,7 +14206,7 @@
         <v>3.8917716827279398</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -14226,7 +14226,7 @@
         <v>40.991073055201298</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -14246,7 +14246,7 @@
         <v>29.055690072639202</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -14266,7 +14266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -14286,7 +14286,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -14311,7 +14311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -14336,7 +14336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -14361,7 +14361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -14386,7 +14386,7 @@
         <v>3.1429012433090584</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -14411,7 +14411,7 @@
         <v>4.0054999868042644</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -14436,7 +14436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -14461,7 +14461,7 @@
         <v>12.422572417562419</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -14486,7 +14486,7 @@
         <v>13.41888619854722</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -14511,7 +14511,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
         <v>27</v>
       </c>
@@ -14527,18 +14527,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE14540-4BE6-4050-B316-6848D183C4F0}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14558,52 +14558,52 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>547.90528233151099</v>
+        <v>58166.510757717399</v>
       </c>
       <c r="C2">
-        <v>28.057173107464202</v>
+        <v>3251.28581925055</v>
       </c>
       <c r="D2">
-        <v>126.33714496495701</v>
+        <v>12674.599068804901</v>
       </c>
       <c r="E2">
-        <v>32.766338406445797</v>
+        <v>3422.1235664076899</v>
       </c>
       <c r="F2">
-        <v>2.2030475491096002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+        <v>203.402366863905</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>355.01453488371999</v>
+        <v>37372.634643377001</v>
       </c>
       <c r="C3">
-        <v>8.5137886359429906</v>
+        <v>930.92533978774895</v>
       </c>
       <c r="D3">
-        <v>37.291280148422999</v>
+        <v>3818.3503243744199</v>
       </c>
       <c r="E3">
-        <v>4.6904315196998096</v>
+        <v>452.23289994346999</v>
       </c>
       <c r="F3">
-        <v>0.72714051990547102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+        <v>73.937153419593301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>54.626532887402398</v>
+        <v>5215.7943067033902</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -14612,38 +14612,38 @@
         <v>4</v>
       </c>
       <c r="E4">
-        <v>0.35555555555555501</v>
+        <v>35.248501938667602</v>
       </c>
       <c r="F4">
-        <v>0.88983804947499501</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+        <v>92.575448990927597</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5">
-        <v>65.662978414656195</v>
+        <v>6321.5354815988703</v>
       </c>
       <c r="C5">
-        <v>1.6432353478181401</v>
+        <v>166.85205784204601</v>
       </c>
       <c r="D5">
-        <v>10.895224260032601</v>
+        <v>1329.7872340425499</v>
       </c>
       <c r="E5">
-        <v>0.361925443358668</v>
+        <v>36.556388228842899</v>
       </c>
       <c r="F5">
-        <v>1.0907107798582001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+        <v>132.200188857412</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6">
-        <v>50.720671410326503</v>
+        <v>5246.0789616008597</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -14652,58 +14652,58 @@
         <v>4</v>
       </c>
       <c r="E6">
-        <v>0.35391966023712601</v>
+        <v>35.945363048166698</v>
       </c>
       <c r="F6">
-        <v>0.91743119266054995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+        <v>91.340884179758802</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>14.4436519258202</v>
+        <v>2083.7075624214099</v>
       </c>
       <c r="C7">
-        <v>0.35174111853675599</v>
+        <v>53.773077612475298</v>
       </c>
       <c r="D7">
-        <v>1.3232514177693699</v>
+        <v>187.58206715438001</v>
       </c>
       <c r="E7">
-        <v>0.15790304752881701</v>
+        <v>16.471750947125599</v>
       </c>
       <c r="F7">
-        <v>0.12758356723653899</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+        <v>13.7287204832509</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8">
-        <v>5.0541516245487301</v>
+        <v>522.87581699346401</v>
       </c>
       <c r="C8">
-        <v>0.17646020822304501</v>
+        <v>18.1061017562918</v>
       </c>
       <c r="D8">
-        <v>0.73072707343806997</v>
+        <v>74.487895716945999</v>
       </c>
       <c r="E8">
-        <v>0.118849536486807</v>
+        <v>12.227928588897001</v>
       </c>
       <c r="F8">
-        <v>0.36231884057970998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+        <v>53.937432578209197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9">
-        <v>2.0014556040756899</v>
+        <v>200.43731778425601</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -14712,18 +14712,18 @@
         <v>4</v>
       </c>
       <c r="E9">
-        <v>9.38967136150234E-2</v>
+        <v>10.476689366160199</v>
       </c>
       <c r="F9">
-        <v>0.340193910529001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+        <v>35.486160397444898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>2.8439388553146099</v>
+        <v>310.44558071585101</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -14732,13 +14732,13 @@
         <v>4</v>
       </c>
       <c r="E10">
-        <v>2.40280647796626E-2</v>
+        <v>2.9893578859261001</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -14758,63 +14758,63 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="9">
         <f xml:space="preserve"> B2 / MIN($B2:$G2)</f>
-        <v>248.70333940497852</v>
+        <v>285.96771834339654</v>
       </c>
       <c r="C13" s="9">
         <f t="shared" ref="C13:F13" si="0" xml:space="preserve"> C2 / MIN($B2:$G2)</f>
-        <v>12.735618493029801</v>
+        <v>15.984503373188184</v>
       </c>
       <c r="D13" s="9">
         <f t="shared" si="0"/>
-        <v>57.346535718676769</v>
+        <v>62.312937967360917</v>
       </c>
       <c r="E13" s="9">
         <f t="shared" si="0"/>
-        <v>14.873187108325864</v>
+        <v>16.824403861029833</v>
       </c>
       <c r="F13" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="9">
         <f t="shared" ref="B14:F14" si="1" xml:space="preserve"> B3 / MIN($B3:$G3)</f>
-        <v>488.23373909883639</v>
+        <v>505.46488355167423</v>
       </c>
       <c r="C14" s="9">
         <f t="shared" si="1"/>
-        <v>11.708587821580609</v>
+        <v>12.590765220629311</v>
       </c>
       <c r="D14" s="9">
         <f t="shared" si="1"/>
-        <v>51.284833024118782</v>
+        <v>51.64318813716406</v>
       </c>
       <c r="E14" s="9">
         <f t="shared" si="1"/>
-        <v>6.4505159474671698</v>
+        <v>6.1164499717354355</v>
       </c>
       <c r="F14" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="9">
         <f t="shared" ref="B15:F15" si="2" xml:space="preserve"> B4 / MIN($B4:$G4)</f>
-        <v>153.63712374581948</v>
+        <v>147.97208448117522</v>
       </c>
       <c r="C15" s="9" t="e">
         <f t="shared" si="2"/>
@@ -14830,24 +14830,24 @@
       </c>
       <c r="F15" s="9">
         <f t="shared" si="2"/>
-        <v>2.5026695141484274</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+        <v>2.6263654878726164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="9">
         <f t="shared" ref="B16:F16" si="3" xml:space="preserve"> B5 / MIN($B5:$G5)</f>
-        <v>181.42680935969511</v>
+        <v>172.92560309913753</v>
       </c>
       <c r="C16" s="9">
         <f t="shared" si="3"/>
-        <v>4.5402592660215229</v>
+        <v>4.5642380422691797</v>
       </c>
       <c r="D16" s="9">
         <f t="shared" si="3"/>
-        <v>30.103504630470084</v>
+        <v>36.376329787234042</v>
       </c>
       <c r="E16" s="9">
         <f t="shared" si="3"/>
@@ -14855,16 +14855,16 @@
       </c>
       <c r="F16" s="9">
         <f t="shared" si="3"/>
-        <v>3.0136338847482076</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+        <v>3.6163361661945146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="9">
         <f t="shared" ref="B17:F17" si="4" xml:space="preserve"> B6 / MIN($B6:$G6)</f>
-        <v>143.3112570698776</v>
+        <v>145.94591671173629</v>
       </c>
       <c r="C17" s="9" t="e">
         <f t="shared" si="4"/>
@@ -14880,49 +14880,49 @@
       </c>
       <c r="F17" s="9">
         <f t="shared" si="4"/>
-        <v>2.5922018348623852</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+        <v>2.5411033978808963</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="9">
         <f t="shared" ref="B18:F18" si="5" xml:space="preserve"> B7 / MIN($B7:$G7)</f>
-        <v>113.20934379457957</v>
+        <v>151.77725884677616</v>
       </c>
       <c r="C18" s="9">
         <f t="shared" si="5"/>
-        <v>2.756946887091114</v>
+        <v>3.916830973292718</v>
       </c>
       <c r="D18" s="9">
         <f t="shared" si="5"/>
-        <v>10.371644612476398</v>
+        <v>13.663477771525102</v>
       </c>
       <c r="E18" s="9">
         <f t="shared" si="5"/>
-        <v>1.2376440865308769</v>
+        <v>1.1998023389886341</v>
       </c>
       <c r="F18" s="9">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="9">
         <f t="shared" ref="B19:F19" si="6" xml:space="preserve"> B8 / MIN($B8:$G8)</f>
-        <v>42.525631768953268</v>
+        <v>42.76078431372563</v>
       </c>
       <c r="C19" s="9">
         <f t="shared" si="6"/>
-        <v>1.4847361919887094</v>
+        <v>1.4807170016295481</v>
       </c>
       <c r="D19" s="9">
         <f t="shared" si="6"/>
-        <v>6.1483375959079565</v>
+        <v>6.0916201117318636</v>
       </c>
       <c r="E19" s="9">
         <f t="shared" si="6"/>
@@ -14930,16 +14930,16 @@
       </c>
       <c r="F19" s="9">
         <f t="shared" si="6"/>
-        <v>3.0485507246376975</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+        <v>4.4110032362459624</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="9">
         <f t="shared" ref="B20:F20" si="7" xml:space="preserve"> B9 / MIN($B9:$G9)</f>
-        <v>21.315502183406114</v>
+        <v>19.131741982507407</v>
       </c>
       <c r="C20" s="9" t="e">
         <f t="shared" si="7"/>
@@ -14955,16 +14955,16 @@
       </c>
       <c r="F20" s="9">
         <f t="shared" si="7"/>
-        <v>3.6230651471338633</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+        <v>3.3871540099361459</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="9">
         <f t="shared" ref="B21:F21" si="8" xml:space="preserve"> B10 / MIN($B10:$G10)</f>
-        <v>118.35904728048367</v>
+        <v>103.85025566106658</v>
       </c>
       <c r="C21" s="9" t="e">
         <f t="shared" si="8"/>
@@ -14983,7 +14983,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
         <v>26</v>
       </c>
@@ -15003,14 +15003,14 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15030,7 +15030,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -15050,7 +15050,7 @@
         <v>207.18540580789201</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -15070,7 +15070,7 @@
         <v>68.475210477081305</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -15090,7 +15090,7 @@
         <v>43.357420789327399</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -15110,7 +15110,7 @@
         <v>111.274329783327</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -15130,7 +15130,7 @@
         <v>77.638053581191897</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -15150,7 +15150,7 @@
         <v>3.9004457652303102</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -15170,7 +15170,7 @@
         <v>39.642857142857103</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -15190,7 +15190,7 @@
         <v>29.5209803193464</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -15210,7 +15210,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -15230,7 +15230,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -15255,7 +15255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -15280,7 +15280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -15305,7 +15305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -15330,7 +15330,7 @@
         <v>3.0359623111033152</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -15355,7 +15355,7 @@
         <v>3.989856544039164</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -15380,7 +15380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -15405,7 +15405,7 @@
         <v>12.084464285714276</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -15430,7 +15430,7 @@
         <v>13.306581878945433</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -15455,7 +15455,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>22</v>
       </c>
@@ -15475,16 +15475,16 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15495,7 +15495,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -15506,7 +15506,7 @@
         <v>61068.169323804199</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -15517,7 +15517,7 @@
         <v>16050.635242128499</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -15528,7 +15528,7 @@
         <v>10091.9178842241</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -15539,7 +15539,7 @@
         <v>2990.7875722543299</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -15550,7 +15550,7 @@
         <v>2112.88604898828</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -15561,7 +15561,7 @@
         <v>1011.74311926605</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -15572,7 +15572,7 @@
         <v>594.21901056142201</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -15583,7 +15583,7 @@
         <v>407.85169029443801</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -15594,7 +15594,7 @@
         <v>192.66055045871499</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -15609,7 +15609,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -15626,7 +15626,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -15643,7 +15643,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -15660,7 +15660,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -15677,7 +15677,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -15694,7 +15694,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -15711,7 +15711,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -15728,7 +15728,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -15741,7 +15741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
         <v>26</v>
       </c>
@@ -15757,20 +15757,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A11EBC7-9C72-4EA8-8A85-7349BC2CCE95}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15781,7 +15781,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -15792,7 +15792,7 @@
         <v>1877.1040723981901</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -15803,7 +15803,7 @@
         <v>619.98567335243501</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -15814,7 +15814,7 @@
         <v>276.44096250699499</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -15825,7 +15825,7 @@
         <v>99.999999999999901</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -15836,7 +15836,7 @@
         <v>71.981862837710096</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -15847,7 +15847,7 @@
         <v>28.2539084573365</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -15858,7 +15858,7 @@
         <v>15.358361774744001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -15869,7 +15869,7 @@
         <v>6.1383928571428497</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -15880,7 +15880,7 @@
         <v>3.8167938931297698</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -15895,7 +15895,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -15912,7 +15912,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -15929,7 +15929,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -15946,7 +15946,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -15963,7 +15963,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -15980,7 +15980,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -15997,7 +15997,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -16014,7 +16014,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -16027,7 +16027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
         <v>26</v>
       </c>
@@ -16043,20 +16043,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3B2414-9220-4890-9B5B-088FCD382078}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16067,106 +16067,106 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2">
-        <v>153.68852459016301</v>
+        <v>14973.7631184407</v>
       </c>
       <c r="C2" s="2">
-        <v>19.690063810391901</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+        <v>2093.8628158844699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>59.9112426035502</v>
+        <v>5846.0996654340497</v>
       </c>
       <c r="C3" s="2">
-        <v>5.6098443720593503</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+        <v>615.32724221517799</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>50.081952285558103</v>
+        <v>5030.5425799496898</v>
       </c>
       <c r="C4" s="2">
-        <v>2.5878003696857599</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+        <v>280.84628346751498</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="2">
-        <v>17.460894870862099</v>
+        <v>2196.99743683632</v>
       </c>
       <c r="C5" s="2">
-        <v>0.70746374248319699</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+        <v>110.96726465692601</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="2">
-        <v>14.7913365029054</v>
+        <v>1596.62323362084</v>
       </c>
       <c r="C6" s="2">
-        <v>0.728730187648023</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+        <v>73.179656055616505</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>5.3713650676051099</v>
+        <v>386.38454461821499</v>
       </c>
       <c r="C7" s="2">
-        <v>0.35765379113018603</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+        <v>35.6760613628255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="2">
-        <v>2.2062879205736299</v>
+        <v>200.69330414158</v>
       </c>
       <c r="C8" s="2">
-        <v>0.171614896172987</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>17.346053772766599</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2">
-        <v>1.0789426362165</v>
+        <v>110.111947146265</v>
       </c>
       <c r="C9" s="2">
-        <v>0.15121729925903499</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>13.9062717285495</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>1.96113389195935</v>
+        <v>200.766563241467</v>
       </c>
       <c r="C10">
-        <v>0.13106159895150701</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>13.1044424059756</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -16181,13 +16181,13 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="3">
         <f xml:space="preserve"> B2 / MIN($B2:$C2)</f>
-        <v>7.8053847905282163</v>
+        <v>7.1512627307035981</v>
       </c>
       <c r="C13" s="3">
         <f xml:space="preserve"> C2 / MIN($B2:$C2)</f>
@@ -16198,13 +16198,13 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="3">
         <f t="shared" ref="B14:C20" si="0" xml:space="preserve"> B3 / MIN($B3:$C3)</f>
-        <v>10.67966214926512</v>
+        <v>9.5007977290069121</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="0"/>
@@ -16215,13 +16215,13 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="3">
         <f t="shared" si="0"/>
-        <v>19.353097276062151</v>
+        <v>17.912085279674226</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="0"/>
@@ -16232,13 +16232,13 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="3">
         <f t="shared" si="0"/>
-        <v>24.680974899963601</v>
+        <v>19.798608568290007</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="0"/>
@@ -16249,13 +16249,13 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="3">
         <f t="shared" si="0"/>
-        <v>20.297411516111943</v>
+        <v>21.817856487428788</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="0"/>
@@ -16266,13 +16266,13 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="3">
         <f t="shared" si="0"/>
-        <v>15.018336729023885</v>
+        <v>10.830358785648579</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="0"/>
@@ -16283,13 +16283,13 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="3">
         <f t="shared" si="0"/>
-        <v>12.856039713182602</v>
+        <v>11.569968983762152</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="0"/>
@@ -16300,20 +16300,20 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="3">
         <f t="shared" si="0"/>
-        <v>7.1350476532997265</v>
+        <v>7.9181501192879589</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
         <v>26</v>
       </c>
@@ -16333,16 +16333,16 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16353,7 +16353,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -16364,7 +16364,7 @@
         <v>2293.4621099554201</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -16375,7 +16375,7 @@
         <v>641.58636026686395</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -16386,7 +16386,7 @@
         <v>271.60262417994301</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -16397,7 +16397,7 @@
         <v>95.176966807262005</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -16408,7 +16408,7 @@
         <v>72.254883368101602</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -16419,7 +16419,7 @@
         <v>30.6876302329986</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -16430,7 +16430,7 @@
         <v>14.700339238597801</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -16441,7 +16441,7 @@
         <v>6.8014358586812698</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -16452,7 +16452,7 @@
         <v>3.9215686274509798</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -16467,7 +16467,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -16484,7 +16484,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -16501,7 +16501,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -16518,7 +16518,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -16535,7 +16535,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -16552,7 +16552,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -16569,7 +16569,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -16586,7 +16586,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -16599,7 +16599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
         <v>26</v>
       </c>
@@ -16619,16 +16619,16 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16642,7 +16642,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -16656,7 +16656,7 @@
         <v>4.3533466352258303</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -16670,7 +16670,7 @@
         <v>7.9659133012226704</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -16684,7 +16684,7 @@
         <v>3.9436619718309802</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -16698,7 +16698,7 @@
         <v>5.5228276877761404</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -16712,7 +16712,7 @@
         <v>8.1496573439525797</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -16726,7 +16726,7 @@
         <v>5.3299025914353901</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -16740,7 +16740,7 @@
         <v>0.72293511657328702</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -16754,7 +16754,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -16772,7 +16772,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -16790,7 +16790,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -16808,7 +16808,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -16826,7 +16826,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -16844,7 +16844,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -16862,7 +16862,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -16880,13 +16880,13 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>26</v>
       </c>

</xml_diff>